<commit_message>
udah baca sales channel, merchant data dan data owner
</commit_message>
<xml_diff>
--- a/attachments/Input Merchant Acquisition (1).xlsx
+++ b/attachments/Input Merchant Acquisition (1).xlsx
@@ -8,16 +8,26 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MerchantAcquisition\attachments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55B8D8E8-0951-4922-A91C-7687E7064724}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D36E7906-358F-4F4B-A2FB-F14E4ECB600D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Versi 1" sheetId="1" r:id="rId1"/>
     <sheet name="Versi 2" sheetId="2" r:id="rId2"/>
     <sheet name="ASCCEND" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -1146,22 +1156,43 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1186,55 +1217,34 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1467,8 +1477,8 @@
   </sheetPr>
   <dimension ref="A1:R81"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="F47" sqref="F47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1489,10 +1499,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="119" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="103"/>
+      <c r="A1" s="111" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="101"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -1519,12 +1529,12 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="96" t="s">
+      <c r="A6" s="112" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="97"/>
-      <c r="C6" s="97"/>
-      <c r="D6" s="98"/>
+      <c r="B6" s="95"/>
+      <c r="C6" s="95"/>
+      <c r="D6" s="105"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
@@ -1699,38 +1709,38 @@
       <c r="D20" s="83"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A22" s="120" t="s">
+      <c r="A22" s="113" t="s">
         <v>26</v>
       </c>
-      <c r="B22" s="102"/>
-      <c r="C22" s="102"/>
-      <c r="D22" s="102"/>
-      <c r="E22" s="102"/>
-      <c r="F22" s="102"/>
-      <c r="G22" s="102"/>
-      <c r="H22" s="102"/>
-      <c r="I22" s="103"/>
+      <c r="B22" s="100"/>
+      <c r="C22" s="100"/>
+      <c r="D22" s="100"/>
+      <c r="E22" s="100"/>
+      <c r="F22" s="100"/>
+      <c r="G22" s="100"/>
+      <c r="H22" s="100"/>
+      <c r="I22" s="101"/>
       <c r="J22" s="19"/>
       <c r="K22" s="19"/>
       <c r="L22" s="19"/>
       <c r="M22" s="19"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A23" s="121" t="s">
+      <c r="A23" s="114" t="s">
         <v>27</v>
       </c>
-      <c r="B23" s="102"/>
-      <c r="C23" s="102"/>
-      <c r="D23" s="121" t="s">
+      <c r="B23" s="100"/>
+      <c r="C23" s="100"/>
+      <c r="D23" s="114" t="s">
         <v>28</v>
       </c>
-      <c r="E23" s="102"/>
-      <c r="F23" s="102"/>
-      <c r="G23" s="121" t="s">
+      <c r="E23" s="100"/>
+      <c r="F23" s="100"/>
+      <c r="G23" s="114" t="s">
         <v>29</v>
       </c>
-      <c r="H23" s="102"/>
-      <c r="I23" s="103"/>
+      <c r="H23" s="100"/>
+      <c r="I23" s="101"/>
       <c r="L23" s="19"/>
       <c r="M23" s="19"/>
     </row>
@@ -1738,86 +1748,86 @@
       <c r="A24" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="B24" s="118"/>
-      <c r="C24" s="98"/>
+      <c r="B24" s="110"/>
+      <c r="C24" s="105"/>
       <c r="D24" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="E24" s="118"/>
-      <c r="F24" s="98"/>
+      <c r="E24" s="110"/>
+      <c r="F24" s="105"/>
       <c r="G24" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="H24" s="118"/>
-      <c r="I24" s="98"/>
+      <c r="H24" s="110"/>
+      <c r="I24" s="105"/>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B25" s="116"/>
-      <c r="C25" s="100"/>
+      <c r="B25" s="115"/>
+      <c r="C25" s="98"/>
       <c r="D25" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="E25" s="116"/>
-      <c r="F25" s="100"/>
+      <c r="E25" s="115"/>
+      <c r="F25" s="98"/>
       <c r="G25" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="H25" s="116"/>
-      <c r="I25" s="100"/>
+      <c r="H25" s="115"/>
+      <c r="I25" s="98"/>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="B26" s="116"/>
-      <c r="C26" s="100"/>
+      <c r="B26" s="115"/>
+      <c r="C26" s="98"/>
       <c r="D26" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="E26" s="116"/>
-      <c r="F26" s="100"/>
+      <c r="E26" s="115"/>
+      <c r="F26" s="98"/>
       <c r="G26" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="H26" s="116"/>
-      <c r="I26" s="100"/>
+      <c r="H26" s="115"/>
+      <c r="I26" s="98"/>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B27" s="116"/>
-      <c r="C27" s="100"/>
+      <c r="B27" s="115"/>
+      <c r="C27" s="98"/>
       <c r="D27" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="E27" s="116"/>
-      <c r="F27" s="100"/>
+      <c r="E27" s="115"/>
+      <c r="F27" s="98"/>
       <c r="G27" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="H27" s="116"/>
-      <c r="I27" s="100"/>
+      <c r="H27" s="115"/>
+      <c r="I27" s="98"/>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A28" s="104" t="s">
+      <c r="A28" s="116" t="s">
         <v>32</v>
       </c>
       <c r="B28" s="21" t="s">
         <v>33</v>
       </c>
       <c r="C28" s="11"/>
-      <c r="D28" s="104" t="s">
+      <c r="D28" s="116" t="s">
         <v>32</v>
       </c>
       <c r="E28" s="21" t="s">
         <v>33</v>
       </c>
       <c r="F28" s="11"/>
-      <c r="G28" s="104" t="s">
+      <c r="G28" s="116" t="s">
         <v>32</v>
       </c>
       <c r="H28" s="21" t="s">
@@ -1826,34 +1836,34 @@
       <c r="I28" s="11"/>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A29" s="105"/>
+      <c r="A29" s="107"/>
       <c r="B29" s="1" t="s">
         <v>34</v>
       </c>
       <c r="C29" s="2"/>
-      <c r="D29" s="105"/>
+      <c r="D29" s="107"/>
       <c r="E29" s="1" t="s">
         <v>34</v>
       </c>
       <c r="F29" s="2"/>
-      <c r="G29" s="105"/>
+      <c r="G29" s="107"/>
       <c r="H29" s="1" t="s">
         <v>34</v>
       </c>
       <c r="I29" s="2"/>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A30" s="105"/>
+      <c r="A30" s="107"/>
       <c r="B30" s="1" t="s">
         <v>35</v>
       </c>
       <c r="C30" s="2"/>
-      <c r="D30" s="105"/>
+      <c r="D30" s="107"/>
       <c r="E30" s="1" t="s">
         <v>35</v>
       </c>
       <c r="F30" s="2"/>
-      <c r="G30" s="105"/>
+      <c r="G30" s="107"/>
       <c r="H30" s="1" t="s">
         <v>35</v>
       </c>
@@ -1861,17 +1871,17 @@
       <c r="M30" s="22"/>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A31" s="105"/>
+      <c r="A31" s="107"/>
       <c r="B31" s="1" t="s">
         <v>36</v>
       </c>
       <c r="C31" s="2"/>
-      <c r="D31" s="105"/>
+      <c r="D31" s="107"/>
       <c r="E31" s="1" t="s">
         <v>36</v>
       </c>
       <c r="F31" s="2"/>
-      <c r="G31" s="105"/>
+      <c r="G31" s="107"/>
       <c r="H31" s="1" t="s">
         <v>36</v>
       </c>
@@ -1879,17 +1889,17 @@
       <c r="M31" s="22"/>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A32" s="105"/>
+      <c r="A32" s="107"/>
       <c r="B32" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C32" s="2"/>
-      <c r="D32" s="105"/>
+      <c r="D32" s="107"/>
       <c r="E32" s="1" t="s">
         <v>37</v>
       </c>
       <c r="F32" s="2"/>
-      <c r="G32" s="105"/>
+      <c r="G32" s="107"/>
       <c r="H32" s="1" t="s">
         <v>37</v>
       </c>
@@ -1897,17 +1907,17 @@
       <c r="M32" s="22"/>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A33" s="105"/>
+      <c r="A33" s="107"/>
       <c r="B33" s="1" t="s">
         <v>38</v>
       </c>
       <c r="C33" s="2"/>
-      <c r="D33" s="105"/>
+      <c r="D33" s="107"/>
       <c r="E33" s="1" t="s">
         <v>38</v>
       </c>
       <c r="F33" s="2"/>
-      <c r="G33" s="105"/>
+      <c r="G33" s="107"/>
       <c r="H33" s="1" t="s">
         <v>38</v>
       </c>
@@ -1915,17 +1925,17 @@
       <c r="M33" s="22"/>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A34" s="105"/>
+      <c r="A34" s="107"/>
       <c r="B34" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C34" s="2"/>
-      <c r="D34" s="105"/>
+      <c r="D34" s="107"/>
       <c r="E34" s="1" t="s">
         <v>39</v>
       </c>
       <c r="F34" s="2"/>
-      <c r="G34" s="105"/>
+      <c r="G34" s="107"/>
       <c r="H34" s="1" t="s">
         <v>39</v>
       </c>
@@ -1933,17 +1943,17 @@
       <c r="M34" s="22"/>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A35" s="106"/>
+      <c r="A35" s="117"/>
       <c r="B35" s="3" t="s">
         <v>40</v>
       </c>
       <c r="C35" s="4"/>
-      <c r="D35" s="106"/>
+      <c r="D35" s="117"/>
       <c r="E35" s="3" t="s">
         <v>40</v>
       </c>
       <c r="F35" s="4"/>
-      <c r="G35" s="106"/>
+      <c r="G35" s="117"/>
       <c r="H35" s="3" t="s">
         <v>40</v>
       </c>
@@ -1954,25 +1964,25 @@
       <c r="A36" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="B36" s="94"/>
-      <c r="C36" s="95"/>
+      <c r="B36" s="127"/>
+      <c r="C36" s="109"/>
       <c r="D36" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="E36" s="94"/>
-      <c r="F36" s="95"/>
+      <c r="E36" s="127"/>
+      <c r="F36" s="109"/>
       <c r="G36" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="H36" s="94"/>
-      <c r="I36" s="95"/>
+      <c r="H36" s="127"/>
+      <c r="I36" s="109"/>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A38" s="96" t="s">
+      <c r="A38" s="112" t="s">
         <v>42</v>
       </c>
-      <c r="B38" s="97"/>
-      <c r="C38" s="98"/>
+      <c r="B38" s="95"/>
+      <c r="C38" s="105"/>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" s="10" t="s">
@@ -1987,13 +1997,13 @@
       <c r="A40" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="B40" s="99" t="s">
+      <c r="B40" s="97" t="s">
         <v>219</v>
       </c>
-      <c r="C40" s="100"/>
+      <c r="C40" s="98"/>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A41" s="107" t="s">
+      <c r="A41" s="118" t="s">
         <v>32</v>
       </c>
       <c r="B41" s="10" t="s">
@@ -2004,7 +2014,7 @@
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A42" s="108"/>
+      <c r="A42" s="119"/>
       <c r="B42" s="8" t="s">
         <v>34</v>
       </c>
@@ -2013,7 +2023,7 @@
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A43" s="108"/>
+      <c r="A43" s="119"/>
       <c r="B43" s="8" t="s">
         <v>35</v>
       </c>
@@ -2022,7 +2032,7 @@
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A44" s="108"/>
+      <c r="A44" s="119"/>
       <c r="B44" s="8" t="s">
         <v>36</v>
       </c>
@@ -2031,7 +2041,7 @@
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A45" s="108"/>
+      <c r="A45" s="119"/>
       <c r="B45" s="8" t="s">
         <v>37</v>
       </c>
@@ -2040,7 +2050,7 @@
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A46" s="108"/>
+      <c r="A46" s="119"/>
       <c r="B46" s="8" t="s">
         <v>38</v>
       </c>
@@ -2049,7 +2059,7 @@
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A47" s="108"/>
+      <c r="A47" s="119"/>
       <c r="B47" s="8" t="s">
         <v>39</v>
       </c>
@@ -2058,7 +2068,7 @@
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A48" s="109"/>
+      <c r="A48" s="120"/>
       <c r="B48" s="8" t="s">
         <v>40</v>
       </c>
@@ -2070,34 +2080,34 @@
       <c r="A49" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="B49" s="110">
+      <c r="B49" s="121">
         <v>23586598</v>
       </c>
-      <c r="C49" s="111"/>
+      <c r="C49" s="122"/>
     </row>
     <row r="50" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A50" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="B50" s="112">
+      <c r="B50" s="123">
         <v>8123456789</v>
       </c>
-      <c r="C50" s="113"/>
+      <c r="C50" s="124"/>
     </row>
     <row r="51" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A51" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="B51" s="114" t="s">
+      <c r="B51" s="125" t="s">
         <v>225</v>
       </c>
-      <c r="C51" s="115"/>
+      <c r="C51" s="126"/>
     </row>
     <row r="53" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A53" s="96" t="s">
+      <c r="A53" s="112" t="s">
         <v>48</v>
       </c>
-      <c r="B53" s="98"/>
+      <c r="B53" s="105"/>
     </row>
     <row r="54" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A54" s="10" t="s">
@@ -2154,140 +2164,140 @@
       <c r="B60" s="93"/>
     </row>
     <row r="62" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A62" s="124" t="s">
+      <c r="A62" s="99" t="s">
         <v>55</v>
       </c>
-      <c r="B62" s="102"/>
-      <c r="C62" s="102"/>
-      <c r="D62" s="102"/>
-      <c r="E62" s="102"/>
-      <c r="F62" s="102"/>
-      <c r="G62" s="102"/>
-      <c r="H62" s="102"/>
-      <c r="I62" s="102"/>
-      <c r="J62" s="102"/>
-      <c r="K62" s="102"/>
-      <c r="L62" s="102"/>
-      <c r="M62" s="102"/>
-      <c r="N62" s="102"/>
-      <c r="O62" s="102"/>
-      <c r="P62" s="102"/>
-      <c r="Q62" s="102"/>
-      <c r="R62" s="103"/>
+      <c r="B62" s="100"/>
+      <c r="C62" s="100"/>
+      <c r="D62" s="100"/>
+      <c r="E62" s="100"/>
+      <c r="F62" s="100"/>
+      <c r="G62" s="100"/>
+      <c r="H62" s="100"/>
+      <c r="I62" s="100"/>
+      <c r="J62" s="100"/>
+      <c r="K62" s="100"/>
+      <c r="L62" s="100"/>
+      <c r="M62" s="100"/>
+      <c r="N62" s="100"/>
+      <c r="O62" s="100"/>
+      <c r="P62" s="100"/>
+      <c r="Q62" s="100"/>
+      <c r="R62" s="101"/>
     </row>
     <row r="63" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A63" s="125" t="s">
+      <c r="A63" s="102" t="s">
         <v>56</v>
       </c>
-      <c r="B63" s="102"/>
-      <c r="C63" s="102"/>
-      <c r="D63" s="102"/>
-      <c r="E63" s="102"/>
-      <c r="F63" s="103"/>
-      <c r="G63" s="125" t="s">
+      <c r="B63" s="100"/>
+      <c r="C63" s="100"/>
+      <c r="D63" s="100"/>
+      <c r="E63" s="100"/>
+      <c r="F63" s="101"/>
+      <c r="G63" s="102" t="s">
         <v>57</v>
       </c>
-      <c r="H63" s="102"/>
-      <c r="I63" s="102"/>
-      <c r="J63" s="102"/>
-      <c r="K63" s="102"/>
-      <c r="L63" s="102"/>
-      <c r="M63" s="125" t="s">
+      <c r="H63" s="100"/>
+      <c r="I63" s="100"/>
+      <c r="J63" s="100"/>
+      <c r="K63" s="100"/>
+      <c r="L63" s="100"/>
+      <c r="M63" s="102" t="s">
         <v>58</v>
       </c>
-      <c r="N63" s="102"/>
-      <c r="O63" s="102"/>
-      <c r="P63" s="102"/>
-      <c r="Q63" s="102"/>
-      <c r="R63" s="103"/>
+      <c r="N63" s="100"/>
+      <c r="O63" s="100"/>
+      <c r="P63" s="100"/>
+      <c r="Q63" s="100"/>
+      <c r="R63" s="101"/>
     </row>
     <row r="64" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A64" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B64" s="101"/>
-      <c r="C64" s="102"/>
-      <c r="D64" s="102"/>
-      <c r="E64" s="102"/>
-      <c r="F64" s="103"/>
+      <c r="B64" s="103"/>
+      <c r="C64" s="100"/>
+      <c r="D64" s="100"/>
+      <c r="E64" s="100"/>
+      <c r="F64" s="101"/>
       <c r="G64" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="H64" s="101"/>
-      <c r="I64" s="102"/>
-      <c r="J64" s="102"/>
-      <c r="K64" s="102"/>
-      <c r="L64" s="103"/>
+      <c r="H64" s="103"/>
+      <c r="I64" s="100"/>
+      <c r="J64" s="100"/>
+      <c r="K64" s="100"/>
+      <c r="L64" s="101"/>
       <c r="M64" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="N64" s="101"/>
-      <c r="O64" s="102"/>
-      <c r="P64" s="102"/>
-      <c r="Q64" s="102"/>
-      <c r="R64" s="103"/>
+      <c r="N64" s="103"/>
+      <c r="O64" s="100"/>
+      <c r="P64" s="100"/>
+      <c r="Q64" s="100"/>
+      <c r="R64" s="101"/>
     </row>
     <row r="65" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A65" s="104" t="s">
+      <c r="A65" s="116" t="s">
         <v>59</v>
       </c>
       <c r="B65" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="C65" s="122"/>
-      <c r="D65" s="97"/>
-      <c r="E65" s="97"/>
-      <c r="F65" s="97"/>
-      <c r="G65" s="104" t="s">
+      <c r="C65" s="94"/>
+      <c r="D65" s="95"/>
+      <c r="E65" s="95"/>
+      <c r="F65" s="95"/>
+      <c r="G65" s="116" t="s">
         <v>59</v>
       </c>
       <c r="H65" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="I65" s="126"/>
-      <c r="J65" s="97"/>
-      <c r="K65" s="97"/>
-      <c r="L65" s="98"/>
-      <c r="M65" s="127" t="s">
+      <c r="I65" s="104"/>
+      <c r="J65" s="95"/>
+      <c r="K65" s="95"/>
+      <c r="L65" s="105"/>
+      <c r="M65" s="106" t="s">
         <v>59</v>
       </c>
       <c r="N65" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="O65" s="126"/>
-      <c r="P65" s="97"/>
-      <c r="Q65" s="97"/>
-      <c r="R65" s="98"/>
+      <c r="O65" s="104"/>
+      <c r="P65" s="95"/>
+      <c r="Q65" s="95"/>
+      <c r="R65" s="105"/>
     </row>
     <row r="66" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A66" s="105"/>
+      <c r="A66" s="107"/>
       <c r="B66" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="C66" s="123"/>
-      <c r="D66" s="123"/>
-      <c r="E66" s="123"/>
-      <c r="F66" s="123"/>
-      <c r="G66" s="105"/>
+      <c r="C66" s="96"/>
+      <c r="D66" s="96"/>
+      <c r="E66" s="96"/>
+      <c r="F66" s="96"/>
+      <c r="G66" s="107"/>
       <c r="H66" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="I66" s="99"/>
-      <c r="J66" s="123"/>
-      <c r="K66" s="123"/>
-      <c r="L66" s="100"/>
-      <c r="M66" s="105"/>
+      <c r="I66" s="97"/>
+      <c r="J66" s="96"/>
+      <c r="K66" s="96"/>
+      <c r="L66" s="98"/>
+      <c r="M66" s="107"/>
       <c r="N66" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="O66" s="99"/>
-      <c r="P66" s="123"/>
-      <c r="Q66" s="123"/>
-      <c r="R66" s="100"/>
+      <c r="O66" s="97"/>
+      <c r="P66" s="96"/>
+      <c r="Q66" s="96"/>
+      <c r="R66" s="98"/>
     </row>
     <row r="67" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A67" s="105"/>
-      <c r="B67" s="117" t="s">
+      <c r="A67" s="107"/>
+      <c r="B67" s="108" t="s">
         <v>62</v>
       </c>
       <c r="C67" s="30" t="s">
@@ -2302,8 +2312,8 @@
       <c r="F67" s="30" t="s">
         <v>65</v>
       </c>
-      <c r="G67" s="105"/>
-      <c r="H67" s="117" t="s">
+      <c r="G67" s="107"/>
+      <c r="H67" s="108" t="s">
         <v>62</v>
       </c>
       <c r="I67" s="30" t="s">
@@ -2318,8 +2328,8 @@
       <c r="L67" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="M67" s="105"/>
-      <c r="N67" s="117" t="s">
+      <c r="M67" s="107"/>
+      <c r="N67" s="108" t="s">
         <v>62</v>
       </c>
       <c r="O67" s="30" t="s">
@@ -2336,8 +2346,8 @@
       </c>
     </row>
     <row r="68" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A68" s="105"/>
-      <c r="B68" s="100"/>
+      <c r="A68" s="107"/>
+      <c r="B68" s="98"/>
       <c r="C68" s="29" t="s">
         <v>66</v>
       </c>
@@ -2345,8 +2355,8 @@
         <v>0</v>
       </c>
       <c r="E68" s="2"/>
-      <c r="G68" s="105"/>
-      <c r="H68" s="100"/>
+      <c r="G68" s="107"/>
+      <c r="H68" s="98"/>
       <c r="I68" s="29" t="s">
         <v>67</v>
       </c>
@@ -2355,8 +2365,8 @@
       </c>
       <c r="K68" s="2"/>
       <c r="L68" s="2"/>
-      <c r="M68" s="105"/>
-      <c r="N68" s="100"/>
+      <c r="M68" s="107"/>
+      <c r="N68" s="98"/>
       <c r="O68" s="29" t="s">
         <v>67</v>
       </c>
@@ -2367,8 +2377,8 @@
       <c r="R68" s="2"/>
     </row>
     <row r="69" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A69" s="105"/>
-      <c r="B69" s="100"/>
+      <c r="A69" s="107"/>
+      <c r="B69" s="98"/>
       <c r="C69" s="29" t="s">
         <v>68</v>
       </c>
@@ -2376,8 +2386,8 @@
         <v>0</v>
       </c>
       <c r="E69" s="2"/>
-      <c r="G69" s="105"/>
-      <c r="H69" s="100"/>
+      <c r="G69" s="107"/>
+      <c r="H69" s="98"/>
       <c r="I69" s="29" t="s">
         <v>69</v>
       </c>
@@ -2386,8 +2396,8 @@
       </c>
       <c r="K69" s="2"/>
       <c r="L69" s="2"/>
-      <c r="M69" s="105"/>
-      <c r="N69" s="100"/>
+      <c r="M69" s="107"/>
+      <c r="N69" s="98"/>
       <c r="O69" s="29" t="s">
         <v>69</v>
       </c>
@@ -2398,8 +2408,8 @@
       <c r="R69" s="2"/>
     </row>
     <row r="70" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A70" s="105"/>
-      <c r="B70" s="100"/>
+      <c r="A70" s="107"/>
+      <c r="B70" s="98"/>
       <c r="C70" s="29" t="s">
         <v>70</v>
       </c>
@@ -2407,8 +2417,8 @@
         <v>0</v>
       </c>
       <c r="E70" s="2"/>
-      <c r="G70" s="105"/>
-      <c r="H70" s="100"/>
+      <c r="G70" s="107"/>
+      <c r="H70" s="98"/>
       <c r="I70" s="29" t="s">
         <v>70</v>
       </c>
@@ -2417,8 +2427,8 @@
       </c>
       <c r="K70" s="2"/>
       <c r="L70" s="2"/>
-      <c r="M70" s="105"/>
-      <c r="N70" s="100"/>
+      <c r="M70" s="107"/>
+      <c r="N70" s="98"/>
       <c r="O70" s="29" t="s">
         <v>70</v>
       </c>
@@ -2429,8 +2439,8 @@
       <c r="R70" s="2"/>
     </row>
     <row r="71" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A71" s="105"/>
-      <c r="B71" s="100"/>
+      <c r="A71" s="107"/>
+      <c r="B71" s="98"/>
       <c r="C71" s="29" t="s">
         <v>71</v>
       </c>
@@ -2438,8 +2448,8 @@
         <v>0</v>
       </c>
       <c r="E71" s="2"/>
-      <c r="G71" s="105"/>
-      <c r="H71" s="100"/>
+      <c r="G71" s="107"/>
+      <c r="H71" s="98"/>
       <c r="I71" s="29" t="s">
         <v>71</v>
       </c>
@@ -2448,8 +2458,8 @@
       </c>
       <c r="K71" s="2"/>
       <c r="L71" s="2"/>
-      <c r="M71" s="105"/>
-      <c r="N71" s="100"/>
+      <c r="M71" s="107"/>
+      <c r="N71" s="98"/>
       <c r="O71" s="29" t="s">
         <v>71</v>
       </c>
@@ -2460,8 +2470,8 @@
       <c r="R71" s="2"/>
     </row>
     <row r="72" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A72" s="105"/>
-      <c r="B72" s="100"/>
+      <c r="A72" s="107"/>
+      <c r="B72" s="98"/>
       <c r="C72" s="29" t="s">
         <v>72</v>
       </c>
@@ -2469,8 +2479,8 @@
         <v>0</v>
       </c>
       <c r="E72" s="2"/>
-      <c r="G72" s="105"/>
-      <c r="H72" s="100"/>
+      <c r="G72" s="107"/>
+      <c r="H72" s="98"/>
       <c r="I72" s="29" t="s">
         <v>72</v>
       </c>
@@ -2479,8 +2489,8 @@
       </c>
       <c r="K72" s="2"/>
       <c r="L72" s="2"/>
-      <c r="M72" s="105"/>
-      <c r="N72" s="100"/>
+      <c r="M72" s="107"/>
+      <c r="N72" s="98"/>
       <c r="O72" s="29" t="s">
         <v>72</v>
       </c>
@@ -2491,8 +2501,8 @@
       <c r="R72" s="2"/>
     </row>
     <row r="73" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A73" s="105"/>
-      <c r="B73" s="100"/>
+      <c r="A73" s="107"/>
+      <c r="B73" s="98"/>
       <c r="C73" s="29" t="s">
         <v>73</v>
       </c>
@@ -2500,8 +2510,8 @@
         <v>0</v>
       </c>
       <c r="E73" s="2"/>
-      <c r="G73" s="105"/>
-      <c r="H73" s="100"/>
+      <c r="G73" s="107"/>
+      <c r="H73" s="98"/>
       <c r="I73" s="29" t="s">
         <v>73</v>
       </c>
@@ -2510,8 +2520,8 @@
       </c>
       <c r="K73" s="2"/>
       <c r="L73" s="2"/>
-      <c r="M73" s="105"/>
-      <c r="N73" s="100"/>
+      <c r="M73" s="107"/>
+      <c r="N73" s="98"/>
       <c r="O73" s="29" t="s">
         <v>73</v>
       </c>
@@ -2522,8 +2532,8 @@
       <c r="R73" s="2"/>
     </row>
     <row r="74" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A74" s="105"/>
-      <c r="B74" s="100"/>
+      <c r="A74" s="107"/>
+      <c r="B74" s="98"/>
       <c r="C74" s="29" t="s">
         <v>74</v>
       </c>
@@ -2531,8 +2541,8 @@
         <v>0</v>
       </c>
       <c r="E74" s="2"/>
-      <c r="G74" s="105"/>
-      <c r="H74" s="100"/>
+      <c r="G74" s="107"/>
+      <c r="H74" s="98"/>
       <c r="I74" s="29" t="s">
         <v>74</v>
       </c>
@@ -2541,8 +2551,8 @@
       </c>
       <c r="K74" s="2"/>
       <c r="L74" s="2"/>
-      <c r="M74" s="105"/>
-      <c r="N74" s="100"/>
+      <c r="M74" s="107"/>
+      <c r="N74" s="98"/>
       <c r="O74" s="29" t="s">
         <v>74</v>
       </c>
@@ -2553,8 +2563,8 @@
       <c r="R74" s="2"/>
     </row>
     <row r="75" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A75" s="105"/>
-      <c r="B75" s="100"/>
+      <c r="A75" s="107"/>
+      <c r="B75" s="98"/>
       <c r="C75" s="29" t="s">
         <v>75</v>
       </c>
@@ -2562,8 +2572,8 @@
         <v>0</v>
       </c>
       <c r="E75" s="2"/>
-      <c r="G75" s="105"/>
-      <c r="H75" s="100"/>
+      <c r="G75" s="107"/>
+      <c r="H75" s="98"/>
       <c r="I75" s="29" t="s">
         <v>75</v>
       </c>
@@ -2572,8 +2582,8 @@
       </c>
       <c r="K75" s="2"/>
       <c r="L75" s="2"/>
-      <c r="M75" s="105"/>
-      <c r="N75" s="100"/>
+      <c r="M75" s="107"/>
+      <c r="N75" s="98"/>
       <c r="O75" s="29" t="s">
         <v>75</v>
       </c>
@@ -2584,8 +2594,8 @@
       <c r="R75" s="2"/>
     </row>
     <row r="76" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A76" s="105"/>
-      <c r="B76" s="100"/>
+      <c r="A76" s="107"/>
+      <c r="B76" s="98"/>
       <c r="C76" s="29" t="s">
         <v>76</v>
       </c>
@@ -2593,8 +2603,8 @@
         <v>0</v>
       </c>
       <c r="E76" s="2"/>
-      <c r="G76" s="105"/>
-      <c r="H76" s="100"/>
+      <c r="G76" s="107"/>
+      <c r="H76" s="98"/>
       <c r="I76" s="29" t="s">
         <v>76</v>
       </c>
@@ -2603,8 +2613,8 @@
       </c>
       <c r="K76" s="2"/>
       <c r="L76" s="2"/>
-      <c r="M76" s="105"/>
-      <c r="N76" s="100"/>
+      <c r="M76" s="107"/>
+      <c r="N76" s="98"/>
       <c r="O76" s="29" t="s">
         <v>76</v>
       </c>
@@ -2615,8 +2625,8 @@
       <c r="R76" s="2"/>
     </row>
     <row r="77" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A77" s="105"/>
-      <c r="B77" s="100"/>
+      <c r="A77" s="107"/>
+      <c r="B77" s="98"/>
       <c r="C77" s="29" t="s">
         <v>77</v>
       </c>
@@ -2624,8 +2634,8 @@
         <v>0</v>
       </c>
       <c r="E77" s="2"/>
-      <c r="G77" s="105"/>
-      <c r="H77" s="100"/>
+      <c r="G77" s="107"/>
+      <c r="H77" s="98"/>
       <c r="I77" s="29" t="s">
         <v>77</v>
       </c>
@@ -2634,8 +2644,8 @@
       </c>
       <c r="K77" s="2"/>
       <c r="L77" s="2"/>
-      <c r="M77" s="105"/>
-      <c r="N77" s="100"/>
+      <c r="M77" s="107"/>
+      <c r="N77" s="98"/>
       <c r="O77" s="29" t="s">
         <v>77</v>
       </c>
@@ -2646,8 +2656,8 @@
       <c r="R77" s="2"/>
     </row>
     <row r="78" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A78" s="106"/>
-      <c r="B78" s="95"/>
+      <c r="A78" s="117"/>
+      <c r="B78" s="109"/>
       <c r="C78" s="29" t="s">
         <v>78</v>
       </c>
@@ -2655,8 +2665,8 @@
         <v>0</v>
       </c>
       <c r="E78" s="2"/>
-      <c r="G78" s="106"/>
-      <c r="H78" s="95"/>
+      <c r="G78" s="117"/>
+      <c r="H78" s="109"/>
       <c r="I78" s="29" t="s">
         <v>78</v>
       </c>
@@ -2665,8 +2675,8 @@
       </c>
       <c r="K78" s="2"/>
       <c r="L78" s="2"/>
-      <c r="M78" s="105"/>
-      <c r="N78" s="95"/>
+      <c r="M78" s="107"/>
+      <c r="N78" s="109"/>
       <c r="O78" s="29" t="s">
         <v>78</v>
       </c>
@@ -2742,29 +2752,17 @@
     </row>
   </sheetData>
   <mergeCells count="50">
-    <mergeCell ref="C65:F65"/>
-    <mergeCell ref="C66:F66"/>
-    <mergeCell ref="I66:L66"/>
-    <mergeCell ref="O66:R66"/>
-    <mergeCell ref="A62:R62"/>
-    <mergeCell ref="A63:F63"/>
-    <mergeCell ref="G63:L63"/>
-    <mergeCell ref="M63:R63"/>
-    <mergeCell ref="B64:F64"/>
-    <mergeCell ref="N64:R64"/>
-    <mergeCell ref="O65:R65"/>
-    <mergeCell ref="I65:L65"/>
-    <mergeCell ref="M65:M78"/>
-    <mergeCell ref="N67:N78"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A6:D6"/>
-    <mergeCell ref="A22:I22"/>
-    <mergeCell ref="A23:C23"/>
-    <mergeCell ref="D23:F23"/>
-    <mergeCell ref="G23:I23"/>
-    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="H36:I36"/>
+    <mergeCell ref="A38:C38"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="H64:L64"/>
+    <mergeCell ref="A28:A35"/>
+    <mergeCell ref="A41:A48"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B36:C36"/>
     <mergeCell ref="H26:I26"/>
     <mergeCell ref="H27:I27"/>
     <mergeCell ref="G65:G78"/>
@@ -2781,17 +2779,29 @@
     <mergeCell ref="B67:B78"/>
     <mergeCell ref="D28:D35"/>
     <mergeCell ref="G28:G35"/>
-    <mergeCell ref="A28:A35"/>
-    <mergeCell ref="A41:A48"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="H36:I36"/>
-    <mergeCell ref="A38:C38"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="H64:L64"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A6:D6"/>
+    <mergeCell ref="A22:I22"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="D23:F23"/>
+    <mergeCell ref="G23:I23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="C65:F65"/>
+    <mergeCell ref="C66:F66"/>
+    <mergeCell ref="I66:L66"/>
+    <mergeCell ref="O66:R66"/>
+    <mergeCell ref="A62:R62"/>
+    <mergeCell ref="A63:F63"/>
+    <mergeCell ref="G63:L63"/>
+    <mergeCell ref="M63:R63"/>
+    <mergeCell ref="B64:F64"/>
+    <mergeCell ref="N64:R64"/>
+    <mergeCell ref="O65:R65"/>
+    <mergeCell ref="I65:L65"/>
+    <mergeCell ref="M65:M78"/>
+    <mergeCell ref="N67:N78"/>
   </mergeCells>
   <conditionalFormatting sqref="C19">
     <cfRule type="notContainsBlanks" dxfId="0" priority="1">
@@ -2857,421 +2867,421 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:175" x14ac:dyDescent="0.25">
-      <c r="A1" s="129" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="102"/>
-      <c r="C1" s="103"/>
-      <c r="D1" s="129" t="s">
+      <c r="A1" s="131" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="100"/>
+      <c r="C1" s="101"/>
+      <c r="D1" s="131" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="102"/>
-      <c r="F1" s="102"/>
-      <c r="G1" s="102"/>
-      <c r="H1" s="102"/>
-      <c r="I1" s="102"/>
-      <c r="J1" s="102"/>
-      <c r="K1" s="102"/>
-      <c r="L1" s="102"/>
-      <c r="M1" s="102"/>
-      <c r="N1" s="102"/>
-      <c r="O1" s="103"/>
-      <c r="P1" s="129" t="s">
+      <c r="E1" s="100"/>
+      <c r="F1" s="100"/>
+      <c r="G1" s="100"/>
+      <c r="H1" s="100"/>
+      <c r="I1" s="100"/>
+      <c r="J1" s="100"/>
+      <c r="K1" s="100"/>
+      <c r="L1" s="100"/>
+      <c r="M1" s="100"/>
+      <c r="N1" s="100"/>
+      <c r="O1" s="101"/>
+      <c r="P1" s="131" t="s">
         <v>82</v>
       </c>
-      <c r="Q1" s="102"/>
-      <c r="R1" s="102"/>
-      <c r="S1" s="103"/>
-      <c r="T1" s="130" t="s">
+      <c r="Q1" s="100"/>
+      <c r="R1" s="100"/>
+      <c r="S1" s="101"/>
+      <c r="T1" s="128" t="s">
         <v>83</v>
       </c>
-      <c r="U1" s="102"/>
-      <c r="V1" s="102"/>
-      <c r="W1" s="102"/>
-      <c r="X1" s="102"/>
-      <c r="Y1" s="102"/>
-      <c r="Z1" s="102"/>
-      <c r="AA1" s="102"/>
-      <c r="AB1" s="102"/>
-      <c r="AC1" s="102"/>
-      <c r="AD1" s="102"/>
-      <c r="AE1" s="102"/>
-      <c r="AF1" s="103"/>
-      <c r="AG1" s="130" t="s">
+      <c r="U1" s="100"/>
+      <c r="V1" s="100"/>
+      <c r="W1" s="100"/>
+      <c r="X1" s="100"/>
+      <c r="Y1" s="100"/>
+      <c r="Z1" s="100"/>
+      <c r="AA1" s="100"/>
+      <c r="AB1" s="100"/>
+      <c r="AC1" s="100"/>
+      <c r="AD1" s="100"/>
+      <c r="AE1" s="100"/>
+      <c r="AF1" s="101"/>
+      <c r="AG1" s="128" t="s">
         <v>84</v>
       </c>
-      <c r="AH1" s="102"/>
-      <c r="AI1" s="102"/>
-      <c r="AJ1" s="102"/>
-      <c r="AK1" s="102"/>
-      <c r="AL1" s="102"/>
-      <c r="AM1" s="102"/>
-      <c r="AN1" s="102"/>
-      <c r="AO1" s="102"/>
-      <c r="AP1" s="102"/>
-      <c r="AQ1" s="102"/>
-      <c r="AR1" s="102"/>
-      <c r="AS1" s="103"/>
-      <c r="AT1" s="130" t="s">
+      <c r="AH1" s="100"/>
+      <c r="AI1" s="100"/>
+      <c r="AJ1" s="100"/>
+      <c r="AK1" s="100"/>
+      <c r="AL1" s="100"/>
+      <c r="AM1" s="100"/>
+      <c r="AN1" s="100"/>
+      <c r="AO1" s="100"/>
+      <c r="AP1" s="100"/>
+      <c r="AQ1" s="100"/>
+      <c r="AR1" s="100"/>
+      <c r="AS1" s="101"/>
+      <c r="AT1" s="128" t="s">
         <v>48</v>
       </c>
-      <c r="AU1" s="102"/>
-      <c r="AV1" s="102"/>
-      <c r="AW1" s="102"/>
-      <c r="AX1" s="102"/>
-      <c r="AY1" s="102"/>
-      <c r="AZ1" s="103"/>
-      <c r="BA1" s="130" t="s">
+      <c r="AU1" s="100"/>
+      <c r="AV1" s="100"/>
+      <c r="AW1" s="100"/>
+      <c r="AX1" s="100"/>
+      <c r="AY1" s="100"/>
+      <c r="AZ1" s="101"/>
+      <c r="BA1" s="128" t="s">
         <v>85</v>
       </c>
-      <c r="BB1" s="102"/>
-      <c r="BC1" s="102"/>
-      <c r="BD1" s="102"/>
-      <c r="BE1" s="102"/>
-      <c r="BF1" s="102"/>
-      <c r="BG1" s="102"/>
-      <c r="BH1" s="102"/>
-      <c r="BI1" s="102"/>
-      <c r="BJ1" s="102"/>
-      <c r="BK1" s="102"/>
-      <c r="BL1" s="102"/>
-      <c r="BM1" s="102"/>
-      <c r="BN1" s="102"/>
-      <c r="BO1" s="102"/>
-      <c r="BP1" s="102"/>
-      <c r="BQ1" s="102"/>
-      <c r="BR1" s="102"/>
-      <c r="BS1" s="102"/>
-      <c r="BT1" s="102"/>
-      <c r="BU1" s="102"/>
-      <c r="BV1" s="102"/>
-      <c r="BW1" s="102"/>
-      <c r="BX1" s="102"/>
-      <c r="BY1" s="102"/>
-      <c r="BZ1" s="102"/>
-      <c r="CA1" s="102"/>
-      <c r="CB1" s="102"/>
-      <c r="CC1" s="102"/>
-      <c r="CD1" s="102"/>
-      <c r="CE1" s="102"/>
-      <c r="CF1" s="102"/>
-      <c r="CG1" s="102"/>
-      <c r="CH1" s="102"/>
-      <c r="CI1" s="102"/>
-      <c r="CJ1" s="102"/>
-      <c r="CK1" s="102"/>
-      <c r="CL1" s="102"/>
-      <c r="CM1" s="103"/>
+      <c r="BB1" s="100"/>
+      <c r="BC1" s="100"/>
+      <c r="BD1" s="100"/>
+      <c r="BE1" s="100"/>
+      <c r="BF1" s="100"/>
+      <c r="BG1" s="100"/>
+      <c r="BH1" s="100"/>
+      <c r="BI1" s="100"/>
+      <c r="BJ1" s="100"/>
+      <c r="BK1" s="100"/>
+      <c r="BL1" s="100"/>
+      <c r="BM1" s="100"/>
+      <c r="BN1" s="100"/>
+      <c r="BO1" s="100"/>
+      <c r="BP1" s="100"/>
+      <c r="BQ1" s="100"/>
+      <c r="BR1" s="100"/>
+      <c r="BS1" s="100"/>
+      <c r="BT1" s="100"/>
+      <c r="BU1" s="100"/>
+      <c r="BV1" s="100"/>
+      <c r="BW1" s="100"/>
+      <c r="BX1" s="100"/>
+      <c r="BY1" s="100"/>
+      <c r="BZ1" s="100"/>
+      <c r="CA1" s="100"/>
+      <c r="CB1" s="100"/>
+      <c r="CC1" s="100"/>
+      <c r="CD1" s="100"/>
+      <c r="CE1" s="100"/>
+      <c r="CF1" s="100"/>
+      <c r="CG1" s="100"/>
+      <c r="CH1" s="100"/>
+      <c r="CI1" s="100"/>
+      <c r="CJ1" s="100"/>
+      <c r="CK1" s="100"/>
+      <c r="CL1" s="100"/>
+      <c r="CM1" s="101"/>
     </row>
     <row r="2" spans="1:175" x14ac:dyDescent="0.25">
-      <c r="A2" s="131" t="s">
+      <c r="A2" s="132" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="128" t="s">
+      <c r="B2" s="129" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="128" t="s">
+      <c r="C2" s="129" t="s">
         <v>86</v>
       </c>
-      <c r="D2" s="128" t="s">
+      <c r="D2" s="129" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="128" t="s">
+      <c r="E2" s="129" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="128" t="s">
+      <c r="F2" s="129" t="s">
         <v>87</v>
       </c>
-      <c r="G2" s="128" t="s">
+      <c r="G2" s="129" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="128" t="s">
+      <c r="H2" s="129" t="s">
         <v>10</v>
       </c>
-      <c r="I2" s="128" t="s">
+      <c r="I2" s="129" t="s">
         <v>11</v>
       </c>
-      <c r="J2" s="128" t="s">
+      <c r="J2" s="129" t="s">
         <v>12</v>
       </c>
-      <c r="K2" s="128" t="s">
+      <c r="K2" s="129" t="s">
         <v>13</v>
       </c>
-      <c r="L2" s="128" t="s">
+      <c r="L2" s="129" t="s">
         <v>88</v>
       </c>
-      <c r="M2" s="128" t="s">
+      <c r="M2" s="129" t="s">
         <v>15</v>
       </c>
-      <c r="N2" s="128" t="s">
+      <c r="N2" s="129" t="s">
         <v>16</v>
       </c>
-      <c r="O2" s="128" t="s">
+      <c r="O2" s="129" t="s">
         <v>89</v>
       </c>
-      <c r="P2" s="128" t="s">
+      <c r="P2" s="129" t="s">
         <v>90</v>
       </c>
-      <c r="Q2" s="128" t="s">
+      <c r="Q2" s="129" t="s">
         <v>91</v>
       </c>
-      <c r="R2" s="128" t="s">
+      <c r="R2" s="129" t="s">
         <v>23</v>
       </c>
-      <c r="S2" s="128" t="s">
+      <c r="S2" s="129" t="s">
         <v>25</v>
       </c>
-      <c r="T2" s="128" t="s">
+      <c r="T2" s="129" t="s">
         <v>30</v>
       </c>
-      <c r="U2" s="128" t="s">
+      <c r="U2" s="129" t="s">
         <v>6</v>
       </c>
-      <c r="V2" s="128" t="s">
+      <c r="V2" s="129" t="s">
         <v>92</v>
       </c>
-      <c r="W2" s="128" t="s">
+      <c r="W2" s="129" t="s">
         <v>93</v>
       </c>
-      <c r="X2" s="130" t="s">
+      <c r="X2" s="128" t="s">
         <v>32</v>
       </c>
-      <c r="Y2" s="102"/>
-      <c r="Z2" s="102"/>
-      <c r="AA2" s="102"/>
-      <c r="AB2" s="102"/>
-      <c r="AC2" s="102"/>
-      <c r="AD2" s="102"/>
-      <c r="AE2" s="103"/>
-      <c r="AF2" s="128" t="s">
+      <c r="Y2" s="100"/>
+      <c r="Z2" s="100"/>
+      <c r="AA2" s="100"/>
+      <c r="AB2" s="100"/>
+      <c r="AC2" s="100"/>
+      <c r="AD2" s="100"/>
+      <c r="AE2" s="101"/>
+      <c r="AF2" s="129" t="s">
         <v>41</v>
       </c>
-      <c r="AG2" s="128" t="s">
+      <c r="AG2" s="129" t="s">
         <v>94</v>
       </c>
-      <c r="AH2" s="128" t="s">
+      <c r="AH2" s="129" t="s">
         <v>44</v>
       </c>
-      <c r="AI2" s="129" t="s">
+      <c r="AI2" s="131" t="s">
         <v>32</v>
       </c>
-      <c r="AJ2" s="102"/>
-      <c r="AK2" s="102"/>
-      <c r="AL2" s="102"/>
-      <c r="AM2" s="102"/>
-      <c r="AN2" s="102"/>
-      <c r="AO2" s="102"/>
-      <c r="AP2" s="103"/>
-      <c r="AQ2" s="128" t="s">
+      <c r="AJ2" s="100"/>
+      <c r="AK2" s="100"/>
+      <c r="AL2" s="100"/>
+      <c r="AM2" s="100"/>
+      <c r="AN2" s="100"/>
+      <c r="AO2" s="100"/>
+      <c r="AP2" s="101"/>
+      <c r="AQ2" s="129" t="s">
         <v>41</v>
       </c>
-      <c r="AR2" s="128" t="s">
+      <c r="AR2" s="129" t="s">
         <v>46</v>
       </c>
-      <c r="AS2" s="128" t="s">
+      <c r="AS2" s="129" t="s">
         <v>47</v>
       </c>
-      <c r="AT2" s="128" t="s">
+      <c r="AT2" s="129" t="s">
         <v>95</v>
       </c>
-      <c r="AU2" s="128" t="s">
+      <c r="AU2" s="129" t="s">
         <v>50</v>
       </c>
-      <c r="AV2" s="128" t="s">
+      <c r="AV2" s="129" t="s">
         <v>51</v>
       </c>
-      <c r="AW2" s="128" t="s">
+      <c r="AW2" s="129" t="s">
         <v>52</v>
       </c>
-      <c r="AX2" s="128" t="s">
+      <c r="AX2" s="129" t="s">
         <v>22</v>
       </c>
-      <c r="AY2" s="128" t="s">
+      <c r="AY2" s="129" t="s">
         <v>53</v>
       </c>
-      <c r="AZ2" s="128" t="s">
+      <c r="AZ2" s="129" t="s">
         <v>54</v>
       </c>
-      <c r="BA2" s="128" t="s">
+      <c r="BA2" s="129" t="s">
         <v>30</v>
       </c>
-      <c r="BB2" s="130" t="s">
+      <c r="BB2" s="128" t="s">
         <v>59</v>
       </c>
-      <c r="BC2" s="102"/>
-      <c r="BD2" s="102"/>
-      <c r="BE2" s="102"/>
-      <c r="BF2" s="102"/>
-      <c r="BG2" s="102"/>
-      <c r="BH2" s="102"/>
-      <c r="BI2" s="102"/>
-      <c r="BJ2" s="102"/>
-      <c r="BK2" s="102"/>
-      <c r="BL2" s="102"/>
-      <c r="BM2" s="102"/>
-      <c r="BN2" s="102"/>
-      <c r="BO2" s="102"/>
-      <c r="BP2" s="102"/>
-      <c r="BQ2" s="102"/>
-      <c r="BR2" s="102"/>
-      <c r="BS2" s="102"/>
-      <c r="BT2" s="102"/>
-      <c r="BU2" s="102"/>
-      <c r="BV2" s="102"/>
-      <c r="BW2" s="102"/>
-      <c r="BX2" s="102"/>
-      <c r="BY2" s="102"/>
-      <c r="BZ2" s="102"/>
-      <c r="CA2" s="102"/>
-      <c r="CB2" s="102"/>
-      <c r="CC2" s="102"/>
-      <c r="CD2" s="102"/>
-      <c r="CE2" s="102"/>
-      <c r="CF2" s="102"/>
-      <c r="CG2" s="102"/>
-      <c r="CH2" s="102"/>
-      <c r="CI2" s="102"/>
-      <c r="CJ2" s="103"/>
-      <c r="CK2" s="128" t="s">
+      <c r="BC2" s="100"/>
+      <c r="BD2" s="100"/>
+      <c r="BE2" s="100"/>
+      <c r="BF2" s="100"/>
+      <c r="BG2" s="100"/>
+      <c r="BH2" s="100"/>
+      <c r="BI2" s="100"/>
+      <c r="BJ2" s="100"/>
+      <c r="BK2" s="100"/>
+      <c r="BL2" s="100"/>
+      <c r="BM2" s="100"/>
+      <c r="BN2" s="100"/>
+      <c r="BO2" s="100"/>
+      <c r="BP2" s="100"/>
+      <c r="BQ2" s="100"/>
+      <c r="BR2" s="100"/>
+      <c r="BS2" s="100"/>
+      <c r="BT2" s="100"/>
+      <c r="BU2" s="100"/>
+      <c r="BV2" s="100"/>
+      <c r="BW2" s="100"/>
+      <c r="BX2" s="100"/>
+      <c r="BY2" s="100"/>
+      <c r="BZ2" s="100"/>
+      <c r="CA2" s="100"/>
+      <c r="CB2" s="100"/>
+      <c r="CC2" s="100"/>
+      <c r="CD2" s="100"/>
+      <c r="CE2" s="100"/>
+      <c r="CF2" s="100"/>
+      <c r="CG2" s="100"/>
+      <c r="CH2" s="100"/>
+      <c r="CI2" s="100"/>
+      <c r="CJ2" s="101"/>
+      <c r="CK2" s="129" t="s">
         <v>79</v>
       </c>
-      <c r="CL2" s="128" t="s">
+      <c r="CL2" s="129" t="s">
         <v>80</v>
       </c>
-      <c r="CM2" s="128" t="s">
+      <c r="CM2" s="129" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:175" x14ac:dyDescent="0.25">
-      <c r="A3" s="105"/>
-      <c r="B3" s="105"/>
-      <c r="C3" s="105"/>
-      <c r="D3" s="105"/>
-      <c r="E3" s="105"/>
-      <c r="F3" s="105"/>
-      <c r="G3" s="105"/>
-      <c r="H3" s="105"/>
-      <c r="I3" s="105"/>
-      <c r="J3" s="105"/>
-      <c r="K3" s="105"/>
-      <c r="L3" s="105"/>
-      <c r="M3" s="105"/>
-      <c r="N3" s="105"/>
-      <c r="O3" s="105"/>
-      <c r="P3" s="105"/>
-      <c r="Q3" s="105"/>
-      <c r="R3" s="105"/>
-      <c r="S3" s="105"/>
-      <c r="T3" s="105"/>
-      <c r="U3" s="105"/>
-      <c r="V3" s="105"/>
-      <c r="W3" s="105"/>
-      <c r="X3" s="128" t="s">
+      <c r="A3" s="107"/>
+      <c r="B3" s="107"/>
+      <c r="C3" s="107"/>
+      <c r="D3" s="107"/>
+      <c r="E3" s="107"/>
+      <c r="F3" s="107"/>
+      <c r="G3" s="107"/>
+      <c r="H3" s="107"/>
+      <c r="I3" s="107"/>
+      <c r="J3" s="107"/>
+      <c r="K3" s="107"/>
+      <c r="L3" s="107"/>
+      <c r="M3" s="107"/>
+      <c r="N3" s="107"/>
+      <c r="O3" s="107"/>
+      <c r="P3" s="107"/>
+      <c r="Q3" s="107"/>
+      <c r="R3" s="107"/>
+      <c r="S3" s="107"/>
+      <c r="T3" s="107"/>
+      <c r="U3" s="107"/>
+      <c r="V3" s="107"/>
+      <c r="W3" s="107"/>
+      <c r="X3" s="129" t="s">
         <v>96</v>
       </c>
-      <c r="Y3" s="128" t="s">
+      <c r="Y3" s="129" t="s">
         <v>34</v>
       </c>
-      <c r="Z3" s="128" t="s">
+      <c r="Z3" s="129" t="s">
         <v>35</v>
       </c>
-      <c r="AA3" s="128" t="s">
+      <c r="AA3" s="129" t="s">
         <v>36</v>
       </c>
-      <c r="AB3" s="128" t="s">
+      <c r="AB3" s="129" t="s">
         <v>37</v>
       </c>
-      <c r="AC3" s="128" t="s">
+      <c r="AC3" s="129" t="s">
         <v>38</v>
       </c>
-      <c r="AD3" s="128" t="s">
+      <c r="AD3" s="129" t="s">
         <v>39</v>
       </c>
-      <c r="AE3" s="128" t="s">
+      <c r="AE3" s="129" t="s">
         <v>40</v>
       </c>
-      <c r="AF3" s="105"/>
-      <c r="AG3" s="105"/>
-      <c r="AH3" s="105"/>
-      <c r="AI3" s="128" t="s">
+      <c r="AF3" s="107"/>
+      <c r="AG3" s="107"/>
+      <c r="AH3" s="107"/>
+      <c r="AI3" s="129" t="s">
         <v>97</v>
       </c>
-      <c r="AJ3" s="128" t="s">
+      <c r="AJ3" s="129" t="s">
         <v>34</v>
       </c>
-      <c r="AK3" s="128" t="s">
+      <c r="AK3" s="129" t="s">
         <v>35</v>
       </c>
-      <c r="AL3" s="128" t="s">
+      <c r="AL3" s="129" t="s">
         <v>36</v>
       </c>
-      <c r="AM3" s="128" t="s">
+      <c r="AM3" s="129" t="s">
         <v>37</v>
       </c>
-      <c r="AN3" s="128" t="s">
+      <c r="AN3" s="129" t="s">
         <v>98</v>
       </c>
-      <c r="AO3" s="128" t="s">
+      <c r="AO3" s="129" t="s">
         <v>39</v>
       </c>
-      <c r="AP3" s="128" t="s">
+      <c r="AP3" s="129" t="s">
         <v>40</v>
       </c>
-      <c r="AQ3" s="105"/>
-      <c r="AR3" s="105"/>
-      <c r="AS3" s="105"/>
-      <c r="AT3" s="105"/>
-      <c r="AU3" s="105"/>
-      <c r="AV3" s="105"/>
-      <c r="AW3" s="105"/>
-      <c r="AX3" s="105"/>
-      <c r="AY3" s="105"/>
-      <c r="AZ3" s="105"/>
-      <c r="BA3" s="105"/>
-      <c r="BB3" s="132" t="s">
+      <c r="AQ3" s="107"/>
+      <c r="AR3" s="107"/>
+      <c r="AS3" s="107"/>
+      <c r="AT3" s="107"/>
+      <c r="AU3" s="107"/>
+      <c r="AV3" s="107"/>
+      <c r="AW3" s="107"/>
+      <c r="AX3" s="107"/>
+      <c r="AY3" s="107"/>
+      <c r="AZ3" s="107"/>
+      <c r="BA3" s="107"/>
+      <c r="BB3" s="130" t="s">
         <v>60</v>
       </c>
-      <c r="BC3" s="132" t="s">
+      <c r="BC3" s="130" t="s">
         <v>61</v>
       </c>
       <c r="BD3" s="35"/>
-      <c r="BE3" s="112" t="s">
+      <c r="BE3" s="123" t="s">
         <v>62</v>
       </c>
-      <c r="BF3" s="123"/>
-      <c r="BG3" s="123"/>
-      <c r="BH3" s="123"/>
-      <c r="BI3" s="123"/>
-      <c r="BJ3" s="123"/>
-      <c r="BK3" s="123"/>
-      <c r="BL3" s="123"/>
-      <c r="BM3" s="123"/>
-      <c r="BN3" s="123"/>
-      <c r="BO3" s="123"/>
-      <c r="BP3" s="123"/>
-      <c r="BQ3" s="123"/>
-      <c r="BR3" s="123"/>
-      <c r="BS3" s="123"/>
-      <c r="BT3" s="123"/>
-      <c r="BU3" s="123"/>
-      <c r="BV3" s="123"/>
-      <c r="BW3" s="123"/>
-      <c r="BX3" s="123"/>
-      <c r="BY3" s="123"/>
-      <c r="BZ3" s="123"/>
-      <c r="CA3" s="123"/>
-      <c r="CB3" s="123"/>
-      <c r="CC3" s="123"/>
-      <c r="CD3" s="123"/>
-      <c r="CE3" s="123"/>
-      <c r="CF3" s="123"/>
-      <c r="CG3" s="123"/>
-      <c r="CH3" s="123"/>
-      <c r="CI3" s="123"/>
-      <c r="CJ3" s="123"/>
-      <c r="CK3" s="105"/>
-      <c r="CL3" s="105"/>
-      <c r="CM3" s="105"/>
+      <c r="BF3" s="96"/>
+      <c r="BG3" s="96"/>
+      <c r="BH3" s="96"/>
+      <c r="BI3" s="96"/>
+      <c r="BJ3" s="96"/>
+      <c r="BK3" s="96"/>
+      <c r="BL3" s="96"/>
+      <c r="BM3" s="96"/>
+      <c r="BN3" s="96"/>
+      <c r="BO3" s="96"/>
+      <c r="BP3" s="96"/>
+      <c r="BQ3" s="96"/>
+      <c r="BR3" s="96"/>
+      <c r="BS3" s="96"/>
+      <c r="BT3" s="96"/>
+      <c r="BU3" s="96"/>
+      <c r="BV3" s="96"/>
+      <c r="BW3" s="96"/>
+      <c r="BX3" s="96"/>
+      <c r="BY3" s="96"/>
+      <c r="BZ3" s="96"/>
+      <c r="CA3" s="96"/>
+      <c r="CB3" s="96"/>
+      <c r="CC3" s="96"/>
+      <c r="CD3" s="96"/>
+      <c r="CE3" s="96"/>
+      <c r="CF3" s="96"/>
+      <c r="CG3" s="96"/>
+      <c r="CH3" s="96"/>
+      <c r="CI3" s="96"/>
+      <c r="CJ3" s="96"/>
+      <c r="CK3" s="107"/>
+      <c r="CL3" s="107"/>
+      <c r="CM3" s="107"/>
       <c r="CN3" s="22"/>
       <c r="CO3" s="22"/>
       <c r="CP3" s="22"/>
@@ -3357,176 +3367,176 @@
       <c r="FS3" s="22"/>
     </row>
     <row r="4" spans="1:175" x14ac:dyDescent="0.25">
-      <c r="A4" s="105"/>
-      <c r="B4" s="105"/>
-      <c r="C4" s="105"/>
-      <c r="D4" s="105"/>
-      <c r="E4" s="105"/>
-      <c r="F4" s="105"/>
-      <c r="G4" s="105"/>
-      <c r="H4" s="105"/>
-      <c r="I4" s="105"/>
-      <c r="J4" s="105"/>
-      <c r="K4" s="105"/>
-      <c r="L4" s="105"/>
-      <c r="M4" s="105"/>
-      <c r="N4" s="105"/>
-      <c r="O4" s="105"/>
-      <c r="P4" s="105"/>
-      <c r="Q4" s="105"/>
-      <c r="R4" s="105"/>
-      <c r="S4" s="105"/>
-      <c r="T4" s="105"/>
-      <c r="U4" s="105"/>
-      <c r="V4" s="105"/>
-      <c r="W4" s="105"/>
-      <c r="X4" s="105"/>
-      <c r="Y4" s="105"/>
-      <c r="Z4" s="105"/>
-      <c r="AA4" s="105"/>
-      <c r="AB4" s="105"/>
-      <c r="AC4" s="105"/>
-      <c r="AD4" s="105"/>
-      <c r="AE4" s="105"/>
-      <c r="AF4" s="105"/>
-      <c r="AG4" s="105"/>
-      <c r="AH4" s="105"/>
-      <c r="AI4" s="105"/>
-      <c r="AJ4" s="105"/>
-      <c r="AK4" s="105"/>
-      <c r="AL4" s="105"/>
-      <c r="AM4" s="105"/>
-      <c r="AN4" s="105"/>
-      <c r="AO4" s="105"/>
-      <c r="AP4" s="105"/>
-      <c r="AQ4" s="105"/>
-      <c r="AR4" s="105"/>
-      <c r="AS4" s="105"/>
-      <c r="AT4" s="105"/>
-      <c r="AU4" s="105"/>
-      <c r="AV4" s="105"/>
-      <c r="AW4" s="105"/>
-      <c r="AX4" s="105"/>
-      <c r="AY4" s="105"/>
-      <c r="AZ4" s="105"/>
-      <c r="BA4" s="105"/>
-      <c r="BB4" s="105"/>
-      <c r="BC4" s="105"/>
-      <c r="BD4" s="130" t="s">
+      <c r="A4" s="107"/>
+      <c r="B4" s="107"/>
+      <c r="C4" s="107"/>
+      <c r="D4" s="107"/>
+      <c r="E4" s="107"/>
+      <c r="F4" s="107"/>
+      <c r="G4" s="107"/>
+      <c r="H4" s="107"/>
+      <c r="I4" s="107"/>
+      <c r="J4" s="107"/>
+      <c r="K4" s="107"/>
+      <c r="L4" s="107"/>
+      <c r="M4" s="107"/>
+      <c r="N4" s="107"/>
+      <c r="O4" s="107"/>
+      <c r="P4" s="107"/>
+      <c r="Q4" s="107"/>
+      <c r="R4" s="107"/>
+      <c r="S4" s="107"/>
+      <c r="T4" s="107"/>
+      <c r="U4" s="107"/>
+      <c r="V4" s="107"/>
+      <c r="W4" s="107"/>
+      <c r="X4" s="107"/>
+      <c r="Y4" s="107"/>
+      <c r="Z4" s="107"/>
+      <c r="AA4" s="107"/>
+      <c r="AB4" s="107"/>
+      <c r="AC4" s="107"/>
+      <c r="AD4" s="107"/>
+      <c r="AE4" s="107"/>
+      <c r="AF4" s="107"/>
+      <c r="AG4" s="107"/>
+      <c r="AH4" s="107"/>
+      <c r="AI4" s="107"/>
+      <c r="AJ4" s="107"/>
+      <c r="AK4" s="107"/>
+      <c r="AL4" s="107"/>
+      <c r="AM4" s="107"/>
+      <c r="AN4" s="107"/>
+      <c r="AO4" s="107"/>
+      <c r="AP4" s="107"/>
+      <c r="AQ4" s="107"/>
+      <c r="AR4" s="107"/>
+      <c r="AS4" s="107"/>
+      <c r="AT4" s="107"/>
+      <c r="AU4" s="107"/>
+      <c r="AV4" s="107"/>
+      <c r="AW4" s="107"/>
+      <c r="AX4" s="107"/>
+      <c r="AY4" s="107"/>
+      <c r="AZ4" s="107"/>
+      <c r="BA4" s="107"/>
+      <c r="BB4" s="107"/>
+      <c r="BC4" s="107"/>
+      <c r="BD4" s="128" t="s">
         <v>67</v>
       </c>
-      <c r="BE4" s="102"/>
-      <c r="BF4" s="103"/>
-      <c r="BG4" s="130" t="s">
+      <c r="BE4" s="100"/>
+      <c r="BF4" s="101"/>
+      <c r="BG4" s="128" t="s">
         <v>67</v>
       </c>
-      <c r="BH4" s="102"/>
-      <c r="BI4" s="103"/>
-      <c r="BJ4" s="130" t="s">
+      <c r="BH4" s="100"/>
+      <c r="BI4" s="101"/>
+      <c r="BJ4" s="128" t="s">
         <v>70</v>
       </c>
-      <c r="BK4" s="102"/>
-      <c r="BL4" s="103"/>
-      <c r="BM4" s="130" t="s">
+      <c r="BK4" s="100"/>
+      <c r="BL4" s="101"/>
+      <c r="BM4" s="128" t="s">
         <v>71</v>
       </c>
-      <c r="BN4" s="102"/>
-      <c r="BO4" s="103"/>
-      <c r="BP4" s="130" t="s">
+      <c r="BN4" s="100"/>
+      <c r="BO4" s="101"/>
+      <c r="BP4" s="128" t="s">
         <v>72</v>
       </c>
-      <c r="BQ4" s="102"/>
-      <c r="BR4" s="103"/>
-      <c r="BS4" s="130" t="s">
+      <c r="BQ4" s="100"/>
+      <c r="BR4" s="101"/>
+      <c r="BS4" s="128" t="s">
         <v>73</v>
       </c>
-      <c r="BT4" s="102"/>
-      <c r="BU4" s="103"/>
-      <c r="BV4" s="130" t="s">
+      <c r="BT4" s="100"/>
+      <c r="BU4" s="101"/>
+      <c r="BV4" s="128" t="s">
         <v>74</v>
       </c>
-      <c r="BW4" s="102"/>
-      <c r="BX4" s="103"/>
-      <c r="BY4" s="130" t="s">
+      <c r="BW4" s="100"/>
+      <c r="BX4" s="101"/>
+      <c r="BY4" s="128" t="s">
         <v>75</v>
       </c>
-      <c r="BZ4" s="102"/>
-      <c r="CA4" s="103"/>
-      <c r="CB4" s="130" t="s">
+      <c r="BZ4" s="100"/>
+      <c r="CA4" s="101"/>
+      <c r="CB4" s="128" t="s">
         <v>76</v>
       </c>
-      <c r="CC4" s="102"/>
-      <c r="CD4" s="103"/>
-      <c r="CE4" s="130" t="s">
+      <c r="CC4" s="100"/>
+      <c r="CD4" s="101"/>
+      <c r="CE4" s="128" t="s">
         <v>77</v>
       </c>
-      <c r="CF4" s="102"/>
-      <c r="CG4" s="103"/>
-      <c r="CH4" s="130" t="s">
+      <c r="CF4" s="100"/>
+      <c r="CG4" s="101"/>
+      <c r="CH4" s="128" t="s">
         <v>78</v>
       </c>
-      <c r="CI4" s="102"/>
-      <c r="CJ4" s="103"/>
-      <c r="CK4" s="105"/>
-      <c r="CL4" s="105"/>
-      <c r="CM4" s="105"/>
+      <c r="CI4" s="100"/>
+      <c r="CJ4" s="101"/>
+      <c r="CK4" s="107"/>
+      <c r="CL4" s="107"/>
+      <c r="CM4" s="107"/>
     </row>
     <row r="5" spans="1:175" x14ac:dyDescent="0.25">
-      <c r="A5" s="106"/>
-      <c r="B5" s="106"/>
-      <c r="C5" s="106"/>
-      <c r="D5" s="106"/>
-      <c r="E5" s="106"/>
-      <c r="F5" s="106"/>
-      <c r="G5" s="106"/>
-      <c r="H5" s="106"/>
-      <c r="I5" s="106"/>
-      <c r="J5" s="106"/>
-      <c r="K5" s="106"/>
-      <c r="L5" s="106"/>
-      <c r="M5" s="106"/>
-      <c r="N5" s="106"/>
-      <c r="O5" s="106"/>
-      <c r="P5" s="106"/>
-      <c r="Q5" s="106"/>
-      <c r="R5" s="106"/>
-      <c r="S5" s="106"/>
-      <c r="T5" s="106"/>
-      <c r="U5" s="106"/>
-      <c r="V5" s="106"/>
-      <c r="W5" s="106"/>
-      <c r="X5" s="106"/>
-      <c r="Y5" s="106"/>
-      <c r="Z5" s="106"/>
-      <c r="AA5" s="106"/>
-      <c r="AB5" s="106"/>
-      <c r="AC5" s="106"/>
-      <c r="AD5" s="106"/>
-      <c r="AE5" s="106"/>
-      <c r="AF5" s="106"/>
-      <c r="AG5" s="106"/>
-      <c r="AH5" s="106"/>
-      <c r="AI5" s="106"/>
-      <c r="AJ5" s="106"/>
-      <c r="AK5" s="106"/>
-      <c r="AL5" s="106"/>
-      <c r="AM5" s="106"/>
-      <c r="AN5" s="106"/>
-      <c r="AO5" s="106"/>
-      <c r="AP5" s="106"/>
-      <c r="AQ5" s="106"/>
-      <c r="AR5" s="106"/>
-      <c r="AS5" s="106"/>
-      <c r="AT5" s="106"/>
-      <c r="AU5" s="106"/>
-      <c r="AV5" s="106"/>
-      <c r="AW5" s="106"/>
-      <c r="AX5" s="106"/>
-      <c r="AY5" s="106"/>
-      <c r="AZ5" s="106"/>
-      <c r="BA5" s="106"/>
-      <c r="BB5" s="106"/>
-      <c r="BC5" s="106"/>
+      <c r="A5" s="117"/>
+      <c r="B5" s="117"/>
+      <c r="C5" s="117"/>
+      <c r="D5" s="117"/>
+      <c r="E5" s="117"/>
+      <c r="F5" s="117"/>
+      <c r="G5" s="117"/>
+      <c r="H5" s="117"/>
+      <c r="I5" s="117"/>
+      <c r="J5" s="117"/>
+      <c r="K5" s="117"/>
+      <c r="L5" s="117"/>
+      <c r="M5" s="117"/>
+      <c r="N5" s="117"/>
+      <c r="O5" s="117"/>
+      <c r="P5" s="117"/>
+      <c r="Q5" s="117"/>
+      <c r="R5" s="117"/>
+      <c r="S5" s="117"/>
+      <c r="T5" s="117"/>
+      <c r="U5" s="117"/>
+      <c r="V5" s="117"/>
+      <c r="W5" s="117"/>
+      <c r="X5" s="117"/>
+      <c r="Y5" s="117"/>
+      <c r="Z5" s="117"/>
+      <c r="AA5" s="117"/>
+      <c r="AB5" s="117"/>
+      <c r="AC5" s="117"/>
+      <c r="AD5" s="117"/>
+      <c r="AE5" s="117"/>
+      <c r="AF5" s="117"/>
+      <c r="AG5" s="117"/>
+      <c r="AH5" s="117"/>
+      <c r="AI5" s="117"/>
+      <c r="AJ5" s="117"/>
+      <c r="AK5" s="117"/>
+      <c r="AL5" s="117"/>
+      <c r="AM5" s="117"/>
+      <c r="AN5" s="117"/>
+      <c r="AO5" s="117"/>
+      <c r="AP5" s="117"/>
+      <c r="AQ5" s="117"/>
+      <c r="AR5" s="117"/>
+      <c r="AS5" s="117"/>
+      <c r="AT5" s="117"/>
+      <c r="AU5" s="117"/>
+      <c r="AV5" s="117"/>
+      <c r="AW5" s="117"/>
+      <c r="AX5" s="117"/>
+      <c r="AY5" s="117"/>
+      <c r="AZ5" s="117"/>
+      <c r="BA5" s="117"/>
+      <c r="BB5" s="117"/>
+      <c r="BC5" s="117"/>
       <c r="BD5" s="36" t="s">
         <v>99</v>
       </c>
@@ -3626,9 +3636,9 @@
       <c r="CJ5" s="36" t="s">
         <v>65</v>
       </c>
-      <c r="CK5" s="106"/>
-      <c r="CL5" s="106"/>
-      <c r="CM5" s="106"/>
+      <c r="CK5" s="117"/>
+      <c r="CL5" s="117"/>
+      <c r="CM5" s="117"/>
     </row>
     <row r="6" spans="1:175" x14ac:dyDescent="0.25">
       <c r="A6" s="37"/>
@@ -4207,11 +4217,61 @@
     </row>
   </sheetData>
   <mergeCells count="80">
-    <mergeCell ref="BM4:BO4"/>
-    <mergeCell ref="AM3:AM5"/>
-    <mergeCell ref="AN3:AN5"/>
-    <mergeCell ref="AO3:AO5"/>
-    <mergeCell ref="AP3:AP5"/>
+    <mergeCell ref="X3:X5"/>
+    <mergeCell ref="Y3:Y5"/>
+    <mergeCell ref="AL3:AL5"/>
+    <mergeCell ref="Z3:Z5"/>
+    <mergeCell ref="AA3:AA5"/>
+    <mergeCell ref="AB3:AB5"/>
+    <mergeCell ref="AC3:AC5"/>
+    <mergeCell ref="AD3:AD5"/>
+    <mergeCell ref="T2:T5"/>
+    <mergeCell ref="U2:U5"/>
+    <mergeCell ref="AQ2:AQ5"/>
+    <mergeCell ref="AR2:AR5"/>
+    <mergeCell ref="AS2:AS5"/>
+    <mergeCell ref="V2:V5"/>
+    <mergeCell ref="W2:W5"/>
+    <mergeCell ref="X2:AE2"/>
+    <mergeCell ref="AF2:AF5"/>
+    <mergeCell ref="AG2:AG5"/>
+    <mergeCell ref="AH2:AH5"/>
+    <mergeCell ref="AI2:AP2"/>
+    <mergeCell ref="AE3:AE5"/>
+    <mergeCell ref="AI3:AI5"/>
+    <mergeCell ref="AJ3:AJ5"/>
+    <mergeCell ref="AK3:AK5"/>
+    <mergeCell ref="O2:O5"/>
+    <mergeCell ref="P2:P5"/>
+    <mergeCell ref="Q2:Q5"/>
+    <mergeCell ref="R2:R5"/>
+    <mergeCell ref="S2:S5"/>
+    <mergeCell ref="J2:J5"/>
+    <mergeCell ref="K2:K5"/>
+    <mergeCell ref="L2:L5"/>
+    <mergeCell ref="M2:M5"/>
+    <mergeCell ref="N2:N5"/>
+    <mergeCell ref="E2:E5"/>
+    <mergeCell ref="F2:F5"/>
+    <mergeCell ref="G2:G5"/>
+    <mergeCell ref="H2:H5"/>
+    <mergeCell ref="I2:I5"/>
+    <mergeCell ref="CK2:CK5"/>
+    <mergeCell ref="CL2:CL5"/>
+    <mergeCell ref="CM2:CM5"/>
+    <mergeCell ref="BE3:CJ3"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D1:O1"/>
+    <mergeCell ref="P1:S1"/>
+    <mergeCell ref="T1:AF1"/>
+    <mergeCell ref="AG1:AS1"/>
+    <mergeCell ref="AT1:AZ1"/>
+    <mergeCell ref="BA1:CM1"/>
+    <mergeCell ref="BB2:CJ2"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="C2:C5"/>
+    <mergeCell ref="D2:D5"/>
     <mergeCell ref="CE4:CG4"/>
     <mergeCell ref="CH4:CJ4"/>
     <mergeCell ref="AX2:AX5"/>
@@ -4228,65 +4288,15 @@
     <mergeCell ref="BD4:BF4"/>
     <mergeCell ref="BG4:BI4"/>
     <mergeCell ref="BJ4:BL4"/>
-    <mergeCell ref="CK2:CK5"/>
-    <mergeCell ref="CL2:CL5"/>
-    <mergeCell ref="CM2:CM5"/>
-    <mergeCell ref="BE3:CJ3"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="D1:O1"/>
-    <mergeCell ref="P1:S1"/>
-    <mergeCell ref="T1:AF1"/>
-    <mergeCell ref="AG1:AS1"/>
-    <mergeCell ref="AT1:AZ1"/>
-    <mergeCell ref="BA1:CM1"/>
-    <mergeCell ref="BB2:CJ2"/>
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="B2:B5"/>
-    <mergeCell ref="C2:C5"/>
-    <mergeCell ref="D2:D5"/>
-    <mergeCell ref="E2:E5"/>
-    <mergeCell ref="F2:F5"/>
-    <mergeCell ref="G2:G5"/>
-    <mergeCell ref="H2:H5"/>
-    <mergeCell ref="I2:I5"/>
-    <mergeCell ref="J2:J5"/>
-    <mergeCell ref="K2:K5"/>
-    <mergeCell ref="L2:L5"/>
-    <mergeCell ref="M2:M5"/>
-    <mergeCell ref="N2:N5"/>
-    <mergeCell ref="O2:O5"/>
-    <mergeCell ref="P2:P5"/>
-    <mergeCell ref="Q2:Q5"/>
-    <mergeCell ref="R2:R5"/>
-    <mergeCell ref="S2:S5"/>
-    <mergeCell ref="T2:T5"/>
-    <mergeCell ref="U2:U5"/>
-    <mergeCell ref="AQ2:AQ5"/>
-    <mergeCell ref="AR2:AR5"/>
-    <mergeCell ref="AS2:AS5"/>
-    <mergeCell ref="V2:V5"/>
-    <mergeCell ref="W2:W5"/>
-    <mergeCell ref="X2:AE2"/>
-    <mergeCell ref="AF2:AF5"/>
-    <mergeCell ref="AG2:AG5"/>
-    <mergeCell ref="AH2:AH5"/>
-    <mergeCell ref="AI2:AP2"/>
-    <mergeCell ref="AE3:AE5"/>
-    <mergeCell ref="AI3:AI5"/>
-    <mergeCell ref="AJ3:AJ5"/>
-    <mergeCell ref="AK3:AK5"/>
+    <mergeCell ref="BM4:BO4"/>
+    <mergeCell ref="AM3:AM5"/>
+    <mergeCell ref="AN3:AN5"/>
+    <mergeCell ref="AO3:AO5"/>
+    <mergeCell ref="AP3:AP5"/>
     <mergeCell ref="AT2:AT5"/>
     <mergeCell ref="AU2:AU5"/>
     <mergeCell ref="AV2:AV5"/>
     <mergeCell ref="AW2:AW5"/>
-    <mergeCell ref="X3:X5"/>
-    <mergeCell ref="Y3:Y5"/>
-    <mergeCell ref="AL3:AL5"/>
-    <mergeCell ref="Z3:Z5"/>
-    <mergeCell ref="AA3:AA5"/>
-    <mergeCell ref="AB3:AB5"/>
-    <mergeCell ref="AC3:AC5"/>
-    <mergeCell ref="AD3:AD5"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="BB6:BB10" xr:uid="{00000000-0002-0000-0100-000000000000}">
@@ -4320,36 +4330,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="137" t="s">
+      <c r="A1" s="133" t="s">
         <v>100</v>
       </c>
-      <c r="B1" s="123"/>
-      <c r="C1" s="123"/>
-      <c r="D1" s="123"/>
-      <c r="E1" s="123"/>
-      <c r="F1" s="123"/>
-      <c r="G1" s="123"/>
-      <c r="H1" s="123"/>
-      <c r="I1" s="123"/>
-      <c r="J1" s="123"/>
-      <c r="K1" s="123"/>
-      <c r="L1" s="123"/>
+      <c r="B1" s="96"/>
+      <c r="C1" s="96"/>
+      <c r="D1" s="96"/>
+      <c r="E1" s="96"/>
+      <c r="F1" s="96"/>
+      <c r="G1" s="96"/>
+      <c r="H1" s="96"/>
+      <c r="I1" s="96"/>
+      <c r="J1" s="96"/>
+      <c r="K1" s="96"/>
+      <c r="L1" s="96"/>
     </row>
     <row r="3" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A3" s="134" t="s">
         <v>101</v>
       </c>
-      <c r="B3" s="123"/>
-      <c r="C3" s="123"/>
-      <c r="D3" s="123"/>
-      <c r="E3" s="123"/>
-      <c r="F3" s="123"/>
-      <c r="G3" s="123"/>
-      <c r="H3" s="123"/>
-      <c r="I3" s="123"/>
-      <c r="J3" s="123"/>
-      <c r="K3" s="123"/>
-      <c r="L3" s="123"/>
+      <c r="B3" s="96"/>
+      <c r="C3" s="96"/>
+      <c r="D3" s="96"/>
+      <c r="E3" s="96"/>
+      <c r="F3" s="96"/>
+      <c r="G3" s="96"/>
+      <c r="H3" s="96"/>
+      <c r="I3" s="96"/>
+      <c r="J3" s="96"/>
+      <c r="K3" s="96"/>
+      <c r="L3" s="96"/>
     </row>
     <row r="4" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A4" s="39" t="s">
@@ -4386,24 +4396,24 @@
       <c r="L5" s="33"/>
     </row>
     <row r="6" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A6" s="138" t="s">
+      <c r="A6" s="135" t="s">
         <v>105</v>
       </c>
-      <c r="B6" s="97"/>
-      <c r="C6" s="97"/>
-      <c r="D6" s="98"/>
-      <c r="E6" s="138" t="s">
+      <c r="B6" s="95"/>
+      <c r="C6" s="95"/>
+      <c r="D6" s="105"/>
+      <c r="E6" s="135" t="s">
         <v>106</v>
       </c>
-      <c r="F6" s="97"/>
-      <c r="G6" s="97"/>
-      <c r="H6" s="98"/>
-      <c r="I6" s="138" t="s">
+      <c r="F6" s="95"/>
+      <c r="G6" s="95"/>
+      <c r="H6" s="105"/>
+      <c r="I6" s="135" t="s">
         <v>107</v>
       </c>
-      <c r="J6" s="97"/>
-      <c r="K6" s="97"/>
-      <c r="L6" s="98"/>
+      <c r="J6" s="95"/>
+      <c r="K6" s="95"/>
+      <c r="L6" s="105"/>
     </row>
     <row r="7" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A7" s="39" t="s">
@@ -4601,16 +4611,16 @@
       <c r="A17" s="134" t="s">
         <v>125</v>
       </c>
-      <c r="B17" s="123"/>
-      <c r="C17" s="123"/>
-      <c r="D17" s="123"/>
+      <c r="B17" s="96"/>
+      <c r="C17" s="96"/>
+      <c r="D17" s="96"/>
       <c r="E17" s="47"/>
-      <c r="F17" s="135" t="s">
+      <c r="F17" s="136" t="s">
         <v>126</v>
       </c>
-      <c r="G17" s="136"/>
-      <c r="H17" s="136"/>
-      <c r="I17" s="136"/>
+      <c r="G17" s="137"/>
+      <c r="H17" s="137"/>
+      <c r="I17" s="137"/>
     </row>
     <row r="18" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A18" s="48" t="s">
@@ -4698,16 +4708,16 @@
       <c r="A25" s="134" t="s">
         <v>135</v>
       </c>
-      <c r="B25" s="123"/>
-      <c r="C25" s="123"/>
-      <c r="D25" s="123"/>
+      <c r="B25" s="96"/>
+      <c r="C25" s="96"/>
+      <c r="D25" s="96"/>
       <c r="E25" s="67"/>
       <c r="F25" s="134" t="s">
         <v>136</v>
       </c>
-      <c r="G25" s="123"/>
-      <c r="H25" s="123"/>
-      <c r="I25" s="123"/>
+      <c r="G25" s="96"/>
+      <c r="H25" s="96"/>
+      <c r="I25" s="96"/>
     </row>
     <row r="26" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A26" s="39" t="s">
@@ -5043,13 +5053,13 @@
       <c r="A55" s="134" t="s">
         <v>172</v>
       </c>
-      <c r="B55" s="123"/>
-      <c r="C55" s="123"/>
-      <c r="D55" s="123"/>
-      <c r="E55" s="123"/>
-      <c r="F55" s="123"/>
-      <c r="G55" s="123"/>
-      <c r="H55" s="123"/>
+      <c r="B55" s="96"/>
+      <c r="C55" s="96"/>
+      <c r="D55" s="96"/>
+      <c r="E55" s="96"/>
+      <c r="F55" s="96"/>
+      <c r="G55" s="96"/>
+      <c r="H55" s="96"/>
     </row>
     <row r="56" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A56" s="39" t="s">
@@ -5088,18 +5098,18 @@
       <c r="H59" s="33"/>
     </row>
     <row r="60" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A60" s="133" t="s">
+      <c r="A60" s="138" t="s">
         <v>174</v>
       </c>
-      <c r="B60" s="102"/>
-      <c r="C60" s="102"/>
-      <c r="D60" s="103"/>
-      <c r="E60" s="133" t="s">
+      <c r="B60" s="100"/>
+      <c r="C60" s="100"/>
+      <c r="D60" s="101"/>
+      <c r="E60" s="138" t="s">
         <v>175</v>
       </c>
-      <c r="F60" s="102"/>
-      <c r="G60" s="102"/>
-      <c r="H60" s="103"/>
+      <c r="F60" s="100"/>
+      <c r="G60" s="100"/>
+      <c r="H60" s="101"/>
     </row>
     <row r="61" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A61" s="45" t="s">
@@ -5145,16 +5155,16 @@
       <c r="H62" s="33"/>
     </row>
     <row r="63" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A63" s="133" t="s">
+      <c r="A63" s="138" t="s">
         <v>186</v>
       </c>
-      <c r="B63" s="102"/>
-      <c r="C63" s="102"/>
-      <c r="D63" s="102"/>
-      <c r="E63" s="102"/>
-      <c r="F63" s="102"/>
-      <c r="G63" s="102"/>
-      <c r="H63" s="103"/>
+      <c r="B63" s="100"/>
+      <c r="C63" s="100"/>
+      <c r="D63" s="100"/>
+      <c r="E63" s="100"/>
+      <c r="F63" s="100"/>
+      <c r="G63" s="100"/>
+      <c r="H63" s="101"/>
     </row>
     <row r="64" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A64" s="39" t="s">
@@ -5217,18 +5227,18 @@
       <c r="H67" s="7"/>
     </row>
     <row r="68" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A68" s="133" t="s">
+      <c r="A68" s="138" t="s">
         <v>197</v>
       </c>
-      <c r="B68" s="102"/>
-      <c r="C68" s="102"/>
-      <c r="D68" s="103"/>
-      <c r="E68" s="133" t="s">
+      <c r="B68" s="100"/>
+      <c r="C68" s="100"/>
+      <c r="D68" s="101"/>
+      <c r="E68" s="138" t="s">
         <v>198</v>
       </c>
-      <c r="F68" s="102"/>
-      <c r="G68" s="102"/>
-      <c r="H68" s="103"/>
+      <c r="F68" s="100"/>
+      <c r="G68" s="100"/>
+      <c r="H68" s="101"/>
     </row>
     <row r="69" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A69" s="48" t="s">
@@ -5321,18 +5331,18 @@
       <c r="H74" s="33"/>
     </row>
     <row r="75" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A75" s="133" t="s">
+      <c r="A75" s="138" t="s">
         <v>202</v>
       </c>
-      <c r="B75" s="102"/>
-      <c r="C75" s="102"/>
-      <c r="D75" s="103"/>
-      <c r="E75" s="133" t="s">
+      <c r="B75" s="100"/>
+      <c r="C75" s="100"/>
+      <c r="D75" s="101"/>
+      <c r="E75" s="138" t="s">
         <v>203</v>
       </c>
-      <c r="F75" s="102"/>
-      <c r="G75" s="102"/>
-      <c r="H75" s="103"/>
+      <c r="F75" s="100"/>
+      <c r="G75" s="100"/>
+      <c r="H75" s="101"/>
     </row>
     <row r="76" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A76" s="48" t="s">
@@ -5425,18 +5435,18 @@
       <c r="H81" s="33"/>
     </row>
     <row r="82" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A82" s="133" t="s">
+      <c r="A82" s="138" t="s">
         <v>204</v>
       </c>
-      <c r="B82" s="102"/>
-      <c r="C82" s="102"/>
-      <c r="D82" s="103"/>
-      <c r="E82" s="133" t="s">
+      <c r="B82" s="100"/>
+      <c r="C82" s="100"/>
+      <c r="D82" s="101"/>
+      <c r="E82" s="138" t="s">
         <v>205</v>
       </c>
-      <c r="F82" s="102"/>
-      <c r="G82" s="102"/>
-      <c r="H82" s="103"/>
+      <c r="F82" s="100"/>
+      <c r="G82" s="100"/>
+      <c r="H82" s="101"/>
     </row>
     <row r="83" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A83" s="48" t="s">
@@ -5614,16 +5624,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="A1:L1"/>
-    <mergeCell ref="A3:L3"/>
-    <mergeCell ref="A6:D6"/>
-    <mergeCell ref="E6:H6"/>
-    <mergeCell ref="I6:L6"/>
-    <mergeCell ref="A17:D17"/>
-    <mergeCell ref="F17:I17"/>
-    <mergeCell ref="A68:D68"/>
-    <mergeCell ref="A75:D75"/>
-    <mergeCell ref="E75:H75"/>
     <mergeCell ref="A82:D82"/>
     <mergeCell ref="E82:H82"/>
     <mergeCell ref="A25:D25"/>
@@ -5633,6 +5633,16 @@
     <mergeCell ref="E60:H60"/>
     <mergeCell ref="A63:H63"/>
     <mergeCell ref="E68:H68"/>
+    <mergeCell ref="A17:D17"/>
+    <mergeCell ref="F17:I17"/>
+    <mergeCell ref="A68:D68"/>
+    <mergeCell ref="A75:D75"/>
+    <mergeCell ref="E75:H75"/>
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A3:L3"/>
+    <mergeCell ref="A6:D6"/>
+    <mergeCell ref="E6:H6"/>
+    <mergeCell ref="I6:L6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
read recommendation data Clear
</commit_message>
<xml_diff>
--- a/attachments/Input Merchant Acquisition (1).xlsx
+++ b/attachments/Input Merchant Acquisition (1).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MerchantAcquisition\attachments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E985830-AF09-401B-A44F-3EE1B8A7F129}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6014E4E-3A7A-4AD9-8A4F-0FB97E6CAC1D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="579" uniqueCount="280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="580" uniqueCount="281">
   <si>
     <t>Sales Chanel</t>
   </si>
@@ -872,6 +872,9 @@
   </si>
   <si>
     <t>Pembayaran Prepaid</t>
+  </si>
+  <si>
+    <t>this is prepaid</t>
   </si>
 </sst>
 </file>
@@ -1001,7 +1004,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="38">
+  <borders count="35">
     <border>
       <left/>
       <right/>
@@ -1282,9 +1285,7 @@
       <top style="medium">
         <color rgb="FF000000"/>
       </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -1293,9 +1294,7 @@
       <top style="medium">
         <color rgb="FF000000"/>
       </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -1306,153 +1305,86 @@
       <top style="medium">
         <color rgb="FF000000"/>
       </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
+      <left style="thin">
+        <color indexed="64"/>
       </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FFCCCCCC"/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFCCCCCC"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FFCCCCCC"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
       <left/>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FFCCCCCC"/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
       </right>
-      <top/>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
+      <left style="thin">
+        <color indexed="64"/>
       </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
       </right>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FFCCCCCC"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FFCCCCCC"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
+      <left style="thin">
+        <color indexed="64"/>
       </left>
       <right/>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FFCCCCCC"/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FFCCCCCC"/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color rgb="FFCCCCCC"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FFCCCCCC"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color rgb="FFCCCCCC"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1461,7 +1393,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="196">
+  <cellXfs count="194">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1620,172 +1552,22 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1811,44 +1593,188 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2071,8 +1997,8 @@
   </sheetPr>
   <dimension ref="A1:W99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="F74" sqref="F74"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="G93" sqref="G93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2093,10 +2019,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1" s="162" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="152"/>
+      <c r="A1" s="132" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="113"/>
     </row>
     <row r="2" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -2123,12 +2049,12 @@
       </c>
     </row>
     <row r="6" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A6" s="163" t="s">
+      <c r="A6" s="106" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="145"/>
-      <c r="C6" s="145"/>
-      <c r="D6" s="156"/>
+      <c r="B6" s="107"/>
+      <c r="C6" s="107"/>
+      <c r="D6" s="108"/>
     </row>
     <row r="7" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
@@ -2305,38 +2231,38 @@
       <c r="D20" s="82"/>
     </row>
     <row r="22" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A22" s="164" t="s">
+      <c r="A22" s="133" t="s">
         <v>26</v>
       </c>
-      <c r="B22" s="151"/>
-      <c r="C22" s="151"/>
-      <c r="D22" s="151"/>
-      <c r="E22" s="151"/>
-      <c r="F22" s="151"/>
-      <c r="G22" s="151"/>
-      <c r="H22" s="151"/>
-      <c r="I22" s="152"/>
+      <c r="B22" s="112"/>
+      <c r="C22" s="112"/>
+      <c r="D22" s="112"/>
+      <c r="E22" s="112"/>
+      <c r="F22" s="112"/>
+      <c r="G22" s="112"/>
+      <c r="H22" s="112"/>
+      <c r="I22" s="113"/>
       <c r="J22" s="18"/>
       <c r="K22" s="18"/>
       <c r="L22" s="18"/>
       <c r="M22" s="18"/>
     </row>
     <row r="23" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A23" s="165" t="s">
+      <c r="A23" s="134" t="s">
         <v>27</v>
       </c>
-      <c r="B23" s="151"/>
-      <c r="C23" s="151"/>
-      <c r="D23" s="165" t="s">
+      <c r="B23" s="112"/>
+      <c r="C23" s="112"/>
+      <c r="D23" s="134" t="s">
         <v>28</v>
       </c>
-      <c r="E23" s="151"/>
-      <c r="F23" s="151"/>
-      <c r="G23" s="165" t="s">
+      <c r="E23" s="112"/>
+      <c r="F23" s="112"/>
+      <c r="G23" s="134" t="s">
         <v>29</v>
       </c>
-      <c r="H23" s="151"/>
-      <c r="I23" s="152"/>
+      <c r="H23" s="112"/>
+      <c r="I23" s="113"/>
       <c r="L23" s="18"/>
       <c r="M23" s="18"/>
     </row>
@@ -2344,80 +2270,80 @@
       <c r="A24" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="B24" s="161" t="s">
+      <c r="B24" s="131" t="s">
         <v>239</v>
       </c>
-      <c r="C24" s="156"/>
+      <c r="C24" s="108"/>
       <c r="D24" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="E24" s="161"/>
-      <c r="F24" s="156"/>
+      <c r="E24" s="131"/>
+      <c r="F24" s="108"/>
       <c r="G24" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="H24" s="161"/>
-      <c r="I24" s="156"/>
+      <c r="H24" s="131"/>
+      <c r="I24" s="108"/>
     </row>
     <row r="25" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B25" s="166" t="s">
+      <c r="B25" s="127" t="s">
         <v>240</v>
       </c>
-      <c r="C25" s="149"/>
+      <c r="C25" s="110"/>
       <c r="D25" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="E25" s="166"/>
-      <c r="F25" s="149"/>
+      <c r="E25" s="127"/>
+      <c r="F25" s="110"/>
       <c r="G25" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="H25" s="166"/>
-      <c r="I25" s="149"/>
+      <c r="H25" s="127"/>
+      <c r="I25" s="110"/>
     </row>
     <row r="26" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="B26" s="168" t="s">
+      <c r="B26" s="129" t="s">
         <v>247</v>
       </c>
-      <c r="C26" s="169"/>
+      <c r="C26" s="130"/>
       <c r="D26" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="E26" s="166"/>
-      <c r="F26" s="149"/>
+      <c r="E26" s="127"/>
+      <c r="F26" s="110"/>
       <c r="G26" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="H26" s="166"/>
-      <c r="I26" s="149"/>
+      <c r="H26" s="127"/>
+      <c r="I26" s="110"/>
     </row>
     <row r="27" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B27" s="168" t="s">
+      <c r="B27" s="129" t="s">
         <v>246</v>
       </c>
-      <c r="C27" s="169"/>
+      <c r="C27" s="130"/>
       <c r="D27" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="E27" s="166"/>
-      <c r="F27" s="149"/>
+      <c r="E27" s="127"/>
+      <c r="F27" s="110"/>
       <c r="G27" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="H27" s="166"/>
-      <c r="I27" s="149"/>
+      <c r="H27" s="127"/>
+      <c r="I27" s="110"/>
     </row>
     <row r="28" spans="1:13" ht="35.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="167" t="s">
+      <c r="A28" s="114" t="s">
         <v>32</v>
       </c>
       <c r="B28" s="20" t="s">
@@ -2426,14 +2352,14 @@
       <c r="C28" s="103" t="s">
         <v>241</v>
       </c>
-      <c r="D28" s="167" t="s">
+      <c r="D28" s="114" t="s">
         <v>32</v>
       </c>
       <c r="E28" s="20" t="s">
         <v>33</v>
       </c>
       <c r="F28" s="11"/>
-      <c r="G28" s="167" t="s">
+      <c r="G28" s="114" t="s">
         <v>32</v>
       </c>
       <c r="H28" s="20" t="s">
@@ -2442,38 +2368,38 @@
       <c r="I28" s="11"/>
     </row>
     <row r="29" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A29" s="158"/>
+      <c r="A29" s="115"/>
       <c r="B29" s="1" t="s">
         <v>34</v>
       </c>
       <c r="C29" s="90" t="s">
         <v>242</v>
       </c>
-      <c r="D29" s="158"/>
+      <c r="D29" s="115"/>
       <c r="E29" s="1" t="s">
         <v>34</v>
       </c>
       <c r="F29" s="2"/>
-      <c r="G29" s="158"/>
+      <c r="G29" s="115"/>
       <c r="H29" s="1" t="s">
         <v>34</v>
       </c>
       <c r="I29" s="2"/>
     </row>
     <row r="30" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A30" s="158"/>
+      <c r="A30" s="115"/>
       <c r="B30" s="1" t="s">
         <v>35</v>
       </c>
       <c r="C30" s="90">
         <v>123</v>
       </c>
-      <c r="D30" s="158"/>
+      <c r="D30" s="115"/>
       <c r="E30" s="1" t="s">
         <v>35</v>
       </c>
       <c r="F30" s="2"/>
-      <c r="G30" s="158"/>
+      <c r="G30" s="115"/>
       <c r="H30" s="1" t="s">
         <v>35</v>
       </c>
@@ -2481,19 +2407,19 @@
       <c r="M30" s="21"/>
     </row>
     <row r="31" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A31" s="158"/>
+      <c r="A31" s="115"/>
       <c r="B31" s="1" t="s">
         <v>36</v>
       </c>
       <c r="C31" s="90" t="s">
         <v>243</v>
       </c>
-      <c r="D31" s="158"/>
+      <c r="D31" s="115"/>
       <c r="E31" s="1" t="s">
         <v>36</v>
       </c>
       <c r="F31" s="2"/>
-      <c r="G31" s="158"/>
+      <c r="G31" s="115"/>
       <c r="H31" s="1" t="s">
         <v>36</v>
       </c>
@@ -2501,19 +2427,19 @@
       <c r="M31" s="21"/>
     </row>
     <row r="32" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A32" s="158"/>
+      <c r="A32" s="115"/>
       <c r="B32" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C32" s="90">
         <v>123123</v>
       </c>
-      <c r="D32" s="158"/>
+      <c r="D32" s="115"/>
       <c r="E32" s="1" t="s">
         <v>37</v>
       </c>
       <c r="F32" s="2"/>
-      <c r="G32" s="158"/>
+      <c r="G32" s="115"/>
       <c r="H32" s="1" t="s">
         <v>37</v>
       </c>
@@ -2521,19 +2447,19 @@
       <c r="M32" s="21"/>
     </row>
     <row r="33" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A33" s="158"/>
+      <c r="A33" s="115"/>
       <c r="B33" s="1" t="s">
         <v>38</v>
       </c>
       <c r="C33" s="90" t="s">
         <v>244</v>
       </c>
-      <c r="D33" s="158"/>
+      <c r="D33" s="115"/>
       <c r="E33" s="1" t="s">
         <v>38</v>
       </c>
       <c r="F33" s="2"/>
-      <c r="G33" s="158"/>
+      <c r="G33" s="115"/>
       <c r="H33" s="1" t="s">
         <v>38</v>
       </c>
@@ -2541,19 +2467,19 @@
       <c r="M33" s="21"/>
     </row>
     <row r="34" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A34" s="158"/>
+      <c r="A34" s="115"/>
       <c r="B34" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C34" s="90">
         <v>111</v>
       </c>
-      <c r="D34" s="158"/>
+      <c r="D34" s="115"/>
       <c r="E34" s="1" t="s">
         <v>39</v>
       </c>
       <c r="F34" s="2"/>
-      <c r="G34" s="158"/>
+      <c r="G34" s="115"/>
       <c r="H34" s="1" t="s">
         <v>39</v>
       </c>
@@ -2561,19 +2487,19 @@
       <c r="M34" s="21"/>
     </row>
     <row r="35" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A35" s="170"/>
+      <c r="A35" s="116"/>
       <c r="B35" s="3" t="s">
         <v>40</v>
       </c>
       <c r="C35" s="92">
         <v>32231</v>
       </c>
-      <c r="D35" s="170"/>
+      <c r="D35" s="116"/>
       <c r="E35" s="3" t="s">
         <v>40</v>
       </c>
       <c r="F35" s="4"/>
-      <c r="G35" s="170"/>
+      <c r="G35" s="116"/>
       <c r="H35" s="3" t="s">
         <v>40</v>
       </c>
@@ -2584,27 +2510,27 @@
       <c r="A36" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="B36" s="180" t="s">
+      <c r="B36" s="126" t="s">
         <v>245</v>
       </c>
-      <c r="C36" s="160"/>
+      <c r="C36" s="105"/>
       <c r="D36" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="E36" s="181"/>
-      <c r="F36" s="160"/>
+      <c r="E36" s="104"/>
+      <c r="F36" s="105"/>
       <c r="G36" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="H36" s="181"/>
-      <c r="I36" s="160"/>
+      <c r="H36" s="104"/>
+      <c r="I36" s="105"/>
     </row>
     <row r="38" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A38" s="163" t="s">
+      <c r="A38" s="106" t="s">
         <v>42</v>
       </c>
-      <c r="B38" s="145"/>
-      <c r="C38" s="156"/>
+      <c r="B38" s="107"/>
+      <c r="C38" s="108"/>
     </row>
     <row r="39" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A39" s="10" t="s">
@@ -2619,13 +2545,13 @@
       <c r="A40" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="B40" s="147" t="s">
+      <c r="B40" s="109" t="s">
         <v>219</v>
       </c>
-      <c r="C40" s="149"/>
+      <c r="C40" s="110"/>
     </row>
     <row r="41" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A41" s="171" t="s">
+      <c r="A41" s="117" t="s">
         <v>32</v>
       </c>
       <c r="B41" s="10" t="s">
@@ -2636,7 +2562,7 @@
       </c>
     </row>
     <row r="42" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A42" s="172"/>
+      <c r="A42" s="118"/>
       <c r="B42" s="8" t="s">
         <v>34</v>
       </c>
@@ -2645,7 +2571,7 @@
       </c>
     </row>
     <row r="43" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A43" s="172"/>
+      <c r="A43" s="118"/>
       <c r="B43" s="8" t="s">
         <v>35</v>
       </c>
@@ -2654,7 +2580,7 @@
       </c>
     </row>
     <row r="44" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A44" s="172"/>
+      <c r="A44" s="118"/>
       <c r="B44" s="8" t="s">
         <v>36</v>
       </c>
@@ -2663,7 +2589,7 @@
       </c>
     </row>
     <row r="45" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A45" s="172"/>
+      <c r="A45" s="118"/>
       <c r="B45" s="8" t="s">
         <v>37</v>
       </c>
@@ -2672,7 +2598,7 @@
       </c>
     </row>
     <row r="46" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A46" s="172"/>
+      <c r="A46" s="118"/>
       <c r="B46" s="8" t="s">
         <v>38</v>
       </c>
@@ -2681,7 +2607,7 @@
       </c>
     </row>
     <row r="47" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A47" s="172"/>
+      <c r="A47" s="118"/>
       <c r="B47" s="8" t="s">
         <v>39</v>
       </c>
@@ -2690,7 +2616,7 @@
       </c>
     </row>
     <row r="48" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A48" s="173"/>
+      <c r="A48" s="119"/>
       <c r="B48" s="8" t="s">
         <v>40</v>
       </c>
@@ -2702,34 +2628,34 @@
       <c r="A49" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="B49" s="174">
+      <c r="B49" s="120">
         <v>23586598</v>
       </c>
-      <c r="C49" s="175"/>
+      <c r="C49" s="121"/>
     </row>
     <row r="50" spans="1:18" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A50" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="B50" s="176">
+      <c r="B50" s="122">
         <v>8123456789</v>
       </c>
-      <c r="C50" s="177"/>
+      <c r="C50" s="123"/>
     </row>
     <row r="51" spans="1:18" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A51" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="B51" s="178" t="s">
+      <c r="B51" s="124" t="s">
         <v>225</v>
       </c>
-      <c r="C51" s="179"/>
+      <c r="C51" s="125"/>
     </row>
     <row r="53" spans="1:18" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A53" s="163" t="s">
+      <c r="A53" s="106" t="s">
         <v>48</v>
       </c>
-      <c r="B53" s="156"/>
+      <c r="B53" s="108"/>
     </row>
     <row r="54" spans="1:18" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A54" s="10" t="s">
@@ -2786,146 +2712,146 @@
       <c r="B60" s="92"/>
     </row>
     <row r="62" spans="1:18" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A62" s="150" t="s">
+      <c r="A62" s="138" t="s">
         <v>55</v>
       </c>
-      <c r="B62" s="151"/>
-      <c r="C62" s="151"/>
-      <c r="D62" s="151"/>
-      <c r="E62" s="151"/>
-      <c r="F62" s="151"/>
-      <c r="G62" s="151"/>
-      <c r="H62" s="151"/>
-      <c r="I62" s="151"/>
-      <c r="J62" s="151"/>
-      <c r="K62" s="151"/>
-      <c r="L62" s="151"/>
-      <c r="M62" s="151"/>
-      <c r="N62" s="151"/>
-      <c r="O62" s="151"/>
-      <c r="P62" s="151"/>
-      <c r="Q62" s="151"/>
-      <c r="R62" s="152"/>
+      <c r="B62" s="112"/>
+      <c r="C62" s="112"/>
+      <c r="D62" s="112"/>
+      <c r="E62" s="112"/>
+      <c r="F62" s="112"/>
+      <c r="G62" s="112"/>
+      <c r="H62" s="112"/>
+      <c r="I62" s="112"/>
+      <c r="J62" s="112"/>
+      <c r="K62" s="112"/>
+      <c r="L62" s="112"/>
+      <c r="M62" s="112"/>
+      <c r="N62" s="112"/>
+      <c r="O62" s="112"/>
+      <c r="P62" s="112"/>
+      <c r="Q62" s="112"/>
+      <c r="R62" s="113"/>
     </row>
     <row r="63" spans="1:18" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A63" s="153" t="s">
+      <c r="A63" s="139" t="s">
         <v>56</v>
       </c>
-      <c r="B63" s="151"/>
-      <c r="C63" s="151"/>
-      <c r="D63" s="151"/>
-      <c r="E63" s="151"/>
-      <c r="F63" s="152"/>
-      <c r="G63" s="153" t="s">
+      <c r="B63" s="112"/>
+      <c r="C63" s="112"/>
+      <c r="D63" s="112"/>
+      <c r="E63" s="112"/>
+      <c r="F63" s="113"/>
+      <c r="G63" s="139" t="s">
         <v>57</v>
       </c>
-      <c r="H63" s="151"/>
-      <c r="I63" s="151"/>
-      <c r="J63" s="151"/>
-      <c r="K63" s="151"/>
-      <c r="L63" s="151"/>
-      <c r="M63" s="153" t="s">
+      <c r="H63" s="112"/>
+      <c r="I63" s="112"/>
+      <c r="J63" s="112"/>
+      <c r="K63" s="112"/>
+      <c r="L63" s="112"/>
+      <c r="M63" s="139" t="s">
         <v>58</v>
       </c>
-      <c r="N63" s="151"/>
-      <c r="O63" s="151"/>
-      <c r="P63" s="151"/>
-      <c r="Q63" s="151"/>
-      <c r="R63" s="152"/>
+      <c r="N63" s="112"/>
+      <c r="O63" s="112"/>
+      <c r="P63" s="112"/>
+      <c r="Q63" s="112"/>
+      <c r="R63" s="113"/>
     </row>
     <row r="64" spans="1:18" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A64" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B64" s="154" t="s">
+      <c r="B64" s="111" t="s">
         <v>234</v>
       </c>
-      <c r="C64" s="151"/>
-      <c r="D64" s="151"/>
-      <c r="E64" s="151"/>
-      <c r="F64" s="152"/>
+      <c r="C64" s="112"/>
+      <c r="D64" s="112"/>
+      <c r="E64" s="112"/>
+      <c r="F64" s="113"/>
       <c r="G64" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="H64" s="154"/>
-      <c r="I64" s="151"/>
-      <c r="J64" s="151"/>
-      <c r="K64" s="151"/>
-      <c r="L64" s="152"/>
+      <c r="H64" s="111"/>
+      <c r="I64" s="112"/>
+      <c r="J64" s="112"/>
+      <c r="K64" s="112"/>
+      <c r="L64" s="113"/>
       <c r="M64" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="N64" s="154"/>
-      <c r="O64" s="151"/>
-      <c r="P64" s="151"/>
-      <c r="Q64" s="151"/>
-      <c r="R64" s="152"/>
+      <c r="N64" s="111"/>
+      <c r="O64" s="112"/>
+      <c r="P64" s="112"/>
+      <c r="Q64" s="112"/>
+      <c r="R64" s="113"/>
     </row>
     <row r="65" spans="1:18" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A65" s="167" t="s">
+      <c r="A65" s="114" t="s">
         <v>59</v>
       </c>
       <c r="B65" s="26" t="s">
         <v>60</v>
       </c>
-      <c r="C65" s="144" t="s">
+      <c r="C65" s="135" t="s">
         <v>265</v>
       </c>
-      <c r="D65" s="145"/>
-      <c r="E65" s="145"/>
-      <c r="F65" s="145"/>
-      <c r="G65" s="167" t="s">
+      <c r="D65" s="107"/>
+      <c r="E65" s="107"/>
+      <c r="F65" s="107"/>
+      <c r="G65" s="114" t="s">
         <v>59</v>
       </c>
       <c r="H65" s="26" t="s">
         <v>60</v>
       </c>
-      <c r="I65" s="155"/>
-      <c r="J65" s="145"/>
-      <c r="K65" s="145"/>
-      <c r="L65" s="156"/>
-      <c r="M65" s="157" t="s">
+      <c r="I65" s="140"/>
+      <c r="J65" s="107"/>
+      <c r="K65" s="107"/>
+      <c r="L65" s="108"/>
+      <c r="M65" s="141" t="s">
         <v>59</v>
       </c>
       <c r="N65" s="26" t="s">
         <v>60</v>
       </c>
-      <c r="O65" s="155"/>
-      <c r="P65" s="145"/>
-      <c r="Q65" s="145"/>
-      <c r="R65" s="156"/>
+      <c r="O65" s="140"/>
+      <c r="P65" s="107"/>
+      <c r="Q65" s="107"/>
+      <c r="R65" s="108"/>
     </row>
     <row r="66" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="158"/>
+      <c r="A66" s="115"/>
       <c r="B66" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="C66" s="146">
+      <c r="C66" s="136">
         <v>12</v>
       </c>
-      <c r="D66" s="146"/>
-      <c r="E66" s="146"/>
-      <c r="F66" s="146"/>
-      <c r="G66" s="158"/>
+      <c r="D66" s="136"/>
+      <c r="E66" s="136"/>
+      <c r="F66" s="136"/>
+      <c r="G66" s="115"/>
       <c r="H66" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="I66" s="147"/>
-      <c r="J66" s="148"/>
-      <c r="K66" s="148"/>
-      <c r="L66" s="149"/>
-      <c r="M66" s="158"/>
+      <c r="I66" s="109"/>
+      <c r="J66" s="137"/>
+      <c r="K66" s="137"/>
+      <c r="L66" s="110"/>
+      <c r="M66" s="115"/>
       <c r="N66" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="O66" s="147"/>
-      <c r="P66" s="148"/>
-      <c r="Q66" s="148"/>
-      <c r="R66" s="149"/>
+      <c r="O66" s="109"/>
+      <c r="P66" s="137"/>
+      <c r="Q66" s="137"/>
+      <c r="R66" s="110"/>
     </row>
     <row r="67" spans="1:18" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A67" s="158"/>
-      <c r="B67" s="159" t="s">
+      <c r="A67" s="115"/>
+      <c r="B67" s="128" t="s">
         <v>62</v>
       </c>
       <c r="C67" s="29" t="s">
@@ -2940,8 +2866,8 @@
       <c r="F67" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="G67" s="158"/>
-      <c r="H67" s="159" t="s">
+      <c r="G67" s="115"/>
+      <c r="H67" s="128" t="s">
         <v>62</v>
       </c>
       <c r="I67" s="29" t="s">
@@ -2956,8 +2882,8 @@
       <c r="L67" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="M67" s="158"/>
-      <c r="N67" s="159" t="s">
+      <c r="M67" s="115"/>
+      <c r="N67" s="128" t="s">
         <v>62</v>
       </c>
       <c r="O67" s="29" t="s">
@@ -2974,8 +2900,8 @@
       </c>
     </row>
     <row r="68" spans="1:18" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A68" s="158"/>
-      <c r="B68" s="149"/>
+      <c r="A68" s="115"/>
+      <c r="B68" s="110"/>
       <c r="C68" s="28" t="s">
         <v>66</v>
       </c>
@@ -2988,8 +2914,8 @@
       <c r="F68" t="s">
         <v>233</v>
       </c>
-      <c r="G68" s="158"/>
-      <c r="H68" s="149"/>
+      <c r="G68" s="115"/>
+      <c r="H68" s="110"/>
       <c r="I68" s="28" t="s">
         <v>67</v>
       </c>
@@ -2998,8 +2924,8 @@
       </c>
       <c r="K68" s="2"/>
       <c r="L68" s="2"/>
-      <c r="M68" s="158"/>
-      <c r="N68" s="149"/>
+      <c r="M68" s="115"/>
+      <c r="N68" s="110"/>
       <c r="O68" s="28" t="s">
         <v>67</v>
       </c>
@@ -3010,8 +2936,8 @@
       <c r="R68" s="2"/>
     </row>
     <row r="69" spans="1:18" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A69" s="158"/>
-      <c r="B69" s="149"/>
+      <c r="A69" s="115"/>
+      <c r="B69" s="110"/>
       <c r="C69" s="28" t="s">
         <v>68</v>
       </c>
@@ -3021,8 +2947,8 @@
       <c r="E69" s="2">
         <v>2231</v>
       </c>
-      <c r="G69" s="158"/>
-      <c r="H69" s="149"/>
+      <c r="G69" s="115"/>
+      <c r="H69" s="110"/>
       <c r="I69" s="28" t="s">
         <v>69</v>
       </c>
@@ -3031,8 +2957,8 @@
       </c>
       <c r="K69" s="2"/>
       <c r="L69" s="2"/>
-      <c r="M69" s="158"/>
-      <c r="N69" s="149"/>
+      <c r="M69" s="115"/>
+      <c r="N69" s="110"/>
       <c r="O69" s="28" t="s">
         <v>69</v>
       </c>
@@ -3043,8 +2969,8 @@
       <c r="R69" s="2"/>
     </row>
     <row r="70" spans="1:18" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A70" s="158"/>
-      <c r="B70" s="149"/>
+      <c r="A70" s="115"/>
+      <c r="B70" s="110"/>
       <c r="C70" s="28" t="s">
         <v>70</v>
       </c>
@@ -3052,8 +2978,8 @@
         <v>0</v>
       </c>
       <c r="E70" s="2"/>
-      <c r="G70" s="158"/>
-      <c r="H70" s="149"/>
+      <c r="G70" s="115"/>
+      <c r="H70" s="110"/>
       <c r="I70" s="28" t="s">
         <v>70</v>
       </c>
@@ -3062,8 +2988,8 @@
       </c>
       <c r="K70" s="2"/>
       <c r="L70" s="2"/>
-      <c r="M70" s="158"/>
-      <c r="N70" s="149"/>
+      <c r="M70" s="115"/>
+      <c r="N70" s="110"/>
       <c r="O70" s="28" t="s">
         <v>70</v>
       </c>
@@ -3074,8 +3000,8 @@
       <c r="R70" s="2"/>
     </row>
     <row r="71" spans="1:18" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A71" s="158"/>
-      <c r="B71" s="149"/>
+      <c r="A71" s="115"/>
+      <c r="B71" s="110"/>
       <c r="C71" s="28" t="s">
         <v>71</v>
       </c>
@@ -3083,8 +3009,8 @@
         <v>0</v>
       </c>
       <c r="E71" s="2"/>
-      <c r="G71" s="158"/>
-      <c r="H71" s="149"/>
+      <c r="G71" s="115"/>
+      <c r="H71" s="110"/>
       <c r="I71" s="28" t="s">
         <v>71</v>
       </c>
@@ -3093,8 +3019,8 @@
       </c>
       <c r="K71" s="2"/>
       <c r="L71" s="2"/>
-      <c r="M71" s="158"/>
-      <c r="N71" s="149"/>
+      <c r="M71" s="115"/>
+      <c r="N71" s="110"/>
       <c r="O71" s="28" t="s">
         <v>71</v>
       </c>
@@ -3105,8 +3031,8 @@
       <c r="R71" s="2"/>
     </row>
     <row r="72" spans="1:18" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A72" s="158"/>
-      <c r="B72" s="149"/>
+      <c r="A72" s="115"/>
+      <c r="B72" s="110"/>
       <c r="C72" s="28" t="s">
         <v>72</v>
       </c>
@@ -3116,8 +3042,8 @@
       <c r="E72" s="2">
         <v>232</v>
       </c>
-      <c r="G72" s="158"/>
-      <c r="H72" s="149"/>
+      <c r="G72" s="115"/>
+      <c r="H72" s="110"/>
       <c r="I72" s="28" t="s">
         <v>72</v>
       </c>
@@ -3126,8 +3052,8 @@
       </c>
       <c r="K72" s="2"/>
       <c r="L72" s="2"/>
-      <c r="M72" s="158"/>
-      <c r="N72" s="149"/>
+      <c r="M72" s="115"/>
+      <c r="N72" s="110"/>
       <c r="O72" s="28" t="s">
         <v>72</v>
       </c>
@@ -3138,8 +3064,8 @@
       <c r="R72" s="2"/>
     </row>
     <row r="73" spans="1:18" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A73" s="158"/>
-      <c r="B73" s="149"/>
+      <c r="A73" s="115"/>
+      <c r="B73" s="110"/>
       <c r="C73" s="28" t="s">
         <v>73</v>
       </c>
@@ -3149,8 +3075,11 @@
       <c r="E73" s="2">
         <v>53</v>
       </c>
-      <c r="G73" s="158"/>
-      <c r="H73" s="149"/>
+      <c r="F73" t="s">
+        <v>280</v>
+      </c>
+      <c r="G73" s="115"/>
+      <c r="H73" s="110"/>
       <c r="I73" s="28" t="s">
         <v>73</v>
       </c>
@@ -3159,8 +3088,8 @@
       </c>
       <c r="K73" s="2"/>
       <c r="L73" s="2"/>
-      <c r="M73" s="158"/>
-      <c r="N73" s="149"/>
+      <c r="M73" s="115"/>
+      <c r="N73" s="110"/>
       <c r="O73" s="28" t="s">
         <v>73</v>
       </c>
@@ -3171,8 +3100,8 @@
       <c r="R73" s="2"/>
     </row>
     <row r="74" spans="1:18" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A74" s="158"/>
-      <c r="B74" s="149"/>
+      <c r="A74" s="115"/>
+      <c r="B74" s="110"/>
       <c r="C74" s="28" t="s">
         <v>74</v>
       </c>
@@ -3180,8 +3109,8 @@
         <v>0</v>
       </c>
       <c r="E74" s="2"/>
-      <c r="G74" s="158"/>
-      <c r="H74" s="149"/>
+      <c r="G74" s="115"/>
+      <c r="H74" s="110"/>
       <c r="I74" s="28" t="s">
         <v>74</v>
       </c>
@@ -3190,8 +3119,8 @@
       </c>
       <c r="K74" s="2"/>
       <c r="L74" s="2"/>
-      <c r="M74" s="158"/>
-      <c r="N74" s="149"/>
+      <c r="M74" s="115"/>
+      <c r="N74" s="110"/>
       <c r="O74" s="28" t="s">
         <v>74</v>
       </c>
@@ -3202,8 +3131,8 @@
       <c r="R74" s="2"/>
     </row>
     <row r="75" spans="1:18" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A75" s="158"/>
-      <c r="B75" s="149"/>
+      <c r="A75" s="115"/>
+      <c r="B75" s="110"/>
       <c r="C75" s="28" t="s">
         <v>75</v>
       </c>
@@ -3211,8 +3140,8 @@
         <v>0</v>
       </c>
       <c r="E75" s="2"/>
-      <c r="G75" s="158"/>
-      <c r="H75" s="149"/>
+      <c r="G75" s="115"/>
+      <c r="H75" s="110"/>
       <c r="I75" s="28" t="s">
         <v>75</v>
       </c>
@@ -3221,8 +3150,8 @@
       </c>
       <c r="K75" s="2"/>
       <c r="L75" s="2"/>
-      <c r="M75" s="158"/>
-      <c r="N75" s="149"/>
+      <c r="M75" s="115"/>
+      <c r="N75" s="110"/>
       <c r="O75" s="28" t="s">
         <v>75</v>
       </c>
@@ -3233,8 +3162,8 @@
       <c r="R75" s="2"/>
     </row>
     <row r="76" spans="1:18" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A76" s="158"/>
-      <c r="B76" s="149"/>
+      <c r="A76" s="115"/>
+      <c r="B76" s="110"/>
       <c r="C76" s="28" t="s">
         <v>76</v>
       </c>
@@ -3242,8 +3171,8 @@
         <v>0</v>
       </c>
       <c r="E76" s="2"/>
-      <c r="G76" s="158"/>
-      <c r="H76" s="149"/>
+      <c r="G76" s="115"/>
+      <c r="H76" s="110"/>
       <c r="I76" s="28" t="s">
         <v>76</v>
       </c>
@@ -3252,8 +3181,8 @@
       </c>
       <c r="K76" s="2"/>
       <c r="L76" s="2"/>
-      <c r="M76" s="158"/>
-      <c r="N76" s="149"/>
+      <c r="M76" s="115"/>
+      <c r="N76" s="110"/>
       <c r="O76" s="28" t="s">
         <v>76</v>
       </c>
@@ -3264,8 +3193,8 @@
       <c r="R76" s="2"/>
     </row>
     <row r="77" spans="1:18" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A77" s="158"/>
-      <c r="B77" s="149"/>
+      <c r="A77" s="115"/>
+      <c r="B77" s="110"/>
       <c r="C77" s="28" t="s">
         <v>77</v>
       </c>
@@ -3273,8 +3202,8 @@
         <v>0</v>
       </c>
       <c r="E77" s="2"/>
-      <c r="G77" s="158"/>
-      <c r="H77" s="149"/>
+      <c r="G77" s="115"/>
+      <c r="H77" s="110"/>
       <c r="I77" s="28" t="s">
         <v>77</v>
       </c>
@@ -3283,8 +3212,8 @@
       </c>
       <c r="K77" s="2"/>
       <c r="L77" s="2"/>
-      <c r="M77" s="158"/>
-      <c r="N77" s="149"/>
+      <c r="M77" s="115"/>
+      <c r="N77" s="110"/>
       <c r="O77" s="28" t="s">
         <v>77</v>
       </c>
@@ -3295,8 +3224,8 @@
       <c r="R77" s="2"/>
     </row>
     <row r="78" spans="1:18" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A78" s="158"/>
-      <c r="B78" s="149"/>
+      <c r="A78" s="115"/>
+      <c r="B78" s="110"/>
       <c r="C78" s="28" t="s">
         <v>78</v>
       </c>
@@ -3304,8 +3233,8 @@
         <v>0</v>
       </c>
       <c r="E78" s="2"/>
-      <c r="G78" s="158"/>
-      <c r="H78" s="160"/>
+      <c r="G78" s="115"/>
+      <c r="H78" s="105"/>
       <c r="I78" s="28" t="s">
         <v>78</v>
       </c>
@@ -3314,8 +3243,8 @@
       </c>
       <c r="K78" s="2"/>
       <c r="L78" s="2"/>
-      <c r="M78" s="158"/>
-      <c r="N78" s="160"/>
+      <c r="M78" s="115"/>
+      <c r="N78" s="105"/>
       <c r="O78" s="28" t="s">
         <v>78</v>
       </c>
@@ -3329,29 +3258,29 @@
       <c r="A79" s="95" t="s">
         <v>80</v>
       </c>
-      <c r="B79" s="193" t="s">
+      <c r="B79" s="150" t="s">
         <v>279</v>
       </c>
-      <c r="C79" s="194"/>
-      <c r="D79" s="194"/>
-      <c r="E79" s="194"/>
-      <c r="F79" s="195"/>
+      <c r="C79" s="151"/>
+      <c r="D79" s="151"/>
+      <c r="E79" s="151"/>
+      <c r="F79" s="152"/>
       <c r="G79" s="95" t="s">
         <v>80</v>
       </c>
-      <c r="H79" s="134"/>
-      <c r="I79" s="135"/>
-      <c r="J79" s="135"/>
-      <c r="K79" s="135"/>
-      <c r="L79" s="136"/>
+      <c r="H79" s="153"/>
+      <c r="I79" s="154"/>
+      <c r="J79" s="154"/>
+      <c r="K79" s="154"/>
+      <c r="L79" s="155"/>
       <c r="M79" s="95" t="s">
         <v>80</v>
       </c>
-      <c r="N79" s="134"/>
-      <c r="O79" s="135"/>
-      <c r="P79" s="135"/>
-      <c r="Q79" s="135"/>
-      <c r="R79" s="136"/>
+      <c r="N79" s="153"/>
+      <c r="O79" s="154"/>
+      <c r="P79" s="154"/>
+      <c r="Q79" s="154"/>
+      <c r="R79" s="155"/>
     </row>
     <row r="80" spans="1:18" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A80" s="95" t="s">
@@ -3363,11 +3292,11 @@
       <c r="C80" s="97" t="s">
         <v>238</v>
       </c>
-      <c r="D80" s="132" t="s">
+      <c r="D80" s="148" t="s">
         <v>266</v>
       </c>
-      <c r="E80" s="133"/>
-      <c r="F80" s="133"/>
+      <c r="E80" s="149"/>
+      <c r="F80" s="149"/>
       <c r="G80" s="95" t="s">
         <v>79</v>
       </c>
@@ -3377,9 +3306,9 @@
       <c r="I80" s="97" t="s">
         <v>238</v>
       </c>
-      <c r="J80" s="130"/>
-      <c r="K80" s="130"/>
-      <c r="L80" s="130"/>
+      <c r="J80" s="146"/>
+      <c r="K80" s="146"/>
+      <c r="L80" s="146"/>
       <c r="M80" s="95" t="s">
         <v>79</v>
       </c>
@@ -3389,49 +3318,49 @@
       <c r="O80" s="97" t="s">
         <v>238</v>
       </c>
-      <c r="P80" s="130"/>
-      <c r="Q80" s="130"/>
-      <c r="R80" s="130"/>
+      <c r="P80" s="146"/>
+      <c r="Q80" s="146"/>
+      <c r="R80" s="146"/>
     </row>
     <row r="81" spans="1:23" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A81" s="143" t="s">
+      <c r="A81" s="142" t="s">
         <v>81</v>
       </c>
-      <c r="B81" s="137" t="b">
+      <c r="B81" s="143" t="b">
         <v>1</v>
       </c>
       <c r="C81" s="98" t="s">
         <v>235</v>
       </c>
-      <c r="D81" s="140" t="s">
+      <c r="D81" s="156" t="s">
         <v>267</v>
       </c>
-      <c r="E81" s="133"/>
-      <c r="F81" s="133"/>
-      <c r="G81" s="143" t="s">
+      <c r="E81" s="149"/>
+      <c r="F81" s="149"/>
+      <c r="G81" s="142" t="s">
         <v>81</v>
       </c>
-      <c r="H81" s="137" t="b">
+      <c r="H81" s="143" t="b">
         <v>0</v>
       </c>
       <c r="I81" s="98" t="s">
         <v>235</v>
       </c>
-      <c r="J81" s="130"/>
-      <c r="K81" s="130"/>
-      <c r="L81" s="130"/>
-      <c r="M81" s="143" t="s">
+      <c r="J81" s="146"/>
+      <c r="K81" s="146"/>
+      <c r="L81" s="146"/>
+      <c r="M81" s="142" t="s">
         <v>81</v>
       </c>
-      <c r="N81" s="137" t="b">
+      <c r="N81" s="143" t="b">
         <v>0</v>
       </c>
       <c r="O81" s="98" t="s">
         <v>235</v>
       </c>
-      <c r="P81" s="130"/>
-      <c r="Q81" s="130"/>
-      <c r="R81" s="130"/>
+      <c r="P81" s="146"/>
+      <c r="Q81" s="146"/>
+      <c r="R81" s="146"/>
       <c r="S81" s="93"/>
       <c r="T81" s="93"/>
       <c r="U81" s="93"/>
@@ -3439,32 +3368,32 @@
       <c r="W81" s="93"/>
     </row>
     <row r="82" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="143"/>
-      <c r="B82" s="138"/>
+      <c r="A82" s="142"/>
+      <c r="B82" s="144"/>
       <c r="C82" s="99" t="s">
         <v>236</v>
       </c>
-      <c r="D82" s="141" t="s">
+      <c r="D82" s="157" t="s">
         <v>268</v>
       </c>
-      <c r="E82" s="142"/>
-      <c r="F82" s="142"/>
-      <c r="G82" s="143"/>
-      <c r="H82" s="138"/>
+      <c r="E82" s="158"/>
+      <c r="F82" s="158"/>
+      <c r="G82" s="142"/>
+      <c r="H82" s="144"/>
       <c r="I82" s="99" t="s">
         <v>236</v>
       </c>
-      <c r="J82" s="131"/>
-      <c r="K82" s="131"/>
-      <c r="L82" s="131"/>
-      <c r="M82" s="143"/>
-      <c r="N82" s="138"/>
+      <c r="J82" s="147"/>
+      <c r="K82" s="147"/>
+      <c r="L82" s="147"/>
+      <c r="M82" s="142"/>
+      <c r="N82" s="144"/>
       <c r="O82" s="99" t="s">
         <v>236</v>
       </c>
-      <c r="P82" s="131"/>
-      <c r="Q82" s="131"/>
-      <c r="R82" s="131"/>
+      <c r="P82" s="147"/>
+      <c r="Q82" s="147"/>
+      <c r="R82" s="147"/>
       <c r="S82" s="93"/>
       <c r="T82" s="93"/>
       <c r="U82" s="93"/>
@@ -3472,32 +3401,32 @@
       <c r="W82" s="93"/>
     </row>
     <row r="83" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="143"/>
-      <c r="B83" s="139"/>
+      <c r="A83" s="142"/>
+      <c r="B83" s="145"/>
       <c r="C83" s="100" t="s">
         <v>237</v>
       </c>
-      <c r="D83" s="141" t="s">
+      <c r="D83" s="157" t="s">
         <v>269</v>
       </c>
-      <c r="E83" s="142"/>
-      <c r="F83" s="142"/>
-      <c r="G83" s="143"/>
-      <c r="H83" s="139"/>
+      <c r="E83" s="158"/>
+      <c r="F83" s="158"/>
+      <c r="G83" s="142"/>
+      <c r="H83" s="145"/>
       <c r="I83" s="100" t="s">
         <v>237</v>
       </c>
-      <c r="J83" s="131"/>
-      <c r="K83" s="131"/>
-      <c r="L83" s="131"/>
-      <c r="M83" s="143"/>
-      <c r="N83" s="139"/>
+      <c r="J83" s="147"/>
+      <c r="K83" s="147"/>
+      <c r="L83" s="147"/>
+      <c r="M83" s="142"/>
+      <c r="N83" s="145"/>
       <c r="O83" s="100" t="s">
         <v>237</v>
       </c>
-      <c r="P83" s="131"/>
-      <c r="Q83" s="131"/>
-      <c r="R83" s="131"/>
+      <c r="P83" s="147"/>
+      <c r="Q83" s="147"/>
+      <c r="R83" s="147"/>
       <c r="S83" s="93"/>
       <c r="T83" s="93"/>
       <c r="U83" s="93"/>
@@ -3520,14 +3449,14 @@
       <c r="M84" s="93"/>
       <c r="N84" s="94"/>
     </row>
-    <row r="85" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A85" s="127" t="s">
+    <row r="85" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="171" t="s">
         <v>248</v>
       </c>
-      <c r="B85" s="128"/>
-      <c r="C85" s="128"/>
-      <c r="D85" s="128"/>
-      <c r="E85" s="129"/>
+      <c r="B85" s="172"/>
+      <c r="C85" s="172"/>
+      <c r="D85" s="172"/>
+      <c r="E85" s="173"/>
       <c r="F85" s="93"/>
       <c r="G85" s="93"/>
       <c r="H85" s="93"/>
@@ -3538,16 +3467,16 @@
       <c r="M85" s="93"/>
       <c r="N85" s="93"/>
     </row>
-    <row r="86" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A86" s="104" t="s">
+    <row r="86" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="187" t="s">
         <v>146</v>
       </c>
-      <c r="B86" s="107">
+      <c r="B86" s="178">
         <v>1231</v>
       </c>
-      <c r="C86" s="108"/>
-      <c r="D86" s="108"/>
-      <c r="E86" s="109"/>
+      <c r="C86" s="178"/>
+      <c r="D86" s="178"/>
+      <c r="E86" s="179"/>
       <c r="F86" s="93"/>
       <c r="G86" s="93"/>
       <c r="H86" s="93"/>
@@ -3558,18 +3487,18 @@
       <c r="M86" s="93"/>
       <c r="N86" s="93"/>
     </row>
-    <row r="87" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A87" s="110" t="s">
+    <row r="87" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A87" s="170" t="s">
         <v>249</v>
       </c>
-      <c r="B87" s="105" t="s">
+      <c r="B87" s="185" t="s">
         <v>250</v>
       </c>
-      <c r="C87" s="107" t="s">
+      <c r="C87" s="174" t="s">
         <v>273</v>
       </c>
-      <c r="D87" s="108"/>
-      <c r="E87" s="109"/>
+      <c r="D87" s="174"/>
+      <c r="E87" s="180"/>
       <c r="F87" s="93"/>
       <c r="G87" s="93"/>
       <c r="H87" s="93"/>
@@ -3580,159 +3509,219 @@
       <c r="M87" s="93"/>
       <c r="N87" s="93"/>
     </row>
-    <row r="88" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A88" s="112"/>
-      <c r="B88" s="105" t="s">
+    <row r="88" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="170"/>
+      <c r="B88" s="186" t="s">
         <v>251</v>
       </c>
-      <c r="C88" s="107" t="s">
+      <c r="C88" s="174" t="s">
         <v>272</v>
       </c>
-      <c r="D88" s="108"/>
-      <c r="E88" s="109"/>
-    </row>
-    <row r="89" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A89" s="104" t="s">
+      <c r="D88" s="174"/>
+      <c r="E88" s="180"/>
+    </row>
+    <row r="89" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A89" s="187" t="s">
         <v>252</v>
       </c>
-      <c r="B89" s="106" t="s">
+      <c r="B89" s="175" t="s">
         <v>270</v>
       </c>
-      <c r="C89" s="106" t="s">
+      <c r="C89" s="175" t="s">
         <v>253</v>
       </c>
-      <c r="D89" s="119" t="s">
+      <c r="D89" s="176" t="s">
         <v>271</v>
       </c>
-      <c r="E89" s="120"/>
-    </row>
-    <row r="90" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A90" s="110" t="s">
+      <c r="E89" s="181"/>
+    </row>
+    <row r="90" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A90" s="170" t="s">
         <v>254</v>
       </c>
-      <c r="B90" s="113" t="s">
+      <c r="B90" s="188" t="s">
         <v>255</v>
       </c>
-      <c r="C90" s="114"/>
-      <c r="D90" s="121" t="b">
-        <v>0</v>
-      </c>
-      <c r="E90" s="122"/>
-    </row>
-    <row r="91" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A91" s="111"/>
-      <c r="B91" s="115" t="s">
+      <c r="C90" s="189"/>
+      <c r="D90" s="177" t="b">
+        <v>0</v>
+      </c>
+      <c r="E90" s="182"/>
+    </row>
+    <row r="91" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A91" s="170"/>
+      <c r="B91" s="190" t="s">
         <v>256</v>
       </c>
-      <c r="C91" s="116"/>
-      <c r="D91" s="123" t="b">
+      <c r="C91" s="191"/>
+      <c r="D91" s="177" t="b">
         <v>1</v>
       </c>
-      <c r="E91" s="124"/>
-    </row>
-    <row r="92" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A92" s="111"/>
-      <c r="B92" s="115" t="s">
+      <c r="E91" s="182"/>
+    </row>
+    <row r="92" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A92" s="170"/>
+      <c r="B92" s="190" t="s">
         <v>257</v>
       </c>
-      <c r="C92" s="116"/>
-      <c r="D92" s="123" t="b">
-        <v>0</v>
-      </c>
-      <c r="E92" s="124"/>
-    </row>
-    <row r="93" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A93" s="111"/>
-      <c r="B93" s="115" t="s">
+      <c r="C92" s="191"/>
+      <c r="D92" s="177" t="b">
+        <v>0</v>
+      </c>
+      <c r="E92" s="182"/>
+    </row>
+    <row r="93" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A93" s="170"/>
+      <c r="B93" s="190" t="s">
         <v>73</v>
       </c>
-      <c r="C93" s="116"/>
-      <c r="D93" s="123" t="b">
-        <v>0</v>
-      </c>
-      <c r="E93" s="124"/>
-    </row>
-    <row r="94" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A94" s="112"/>
-      <c r="B94" s="117" t="s">
+      <c r="C93" s="191"/>
+      <c r="D93" s="177" t="b">
+        <v>0</v>
+      </c>
+      <c r="E93" s="182"/>
+    </row>
+    <row r="94" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A94" s="170"/>
+      <c r="B94" s="192" t="s">
         <v>258</v>
       </c>
-      <c r="C94" s="118"/>
-      <c r="D94" s="125" t="b">
-        <v>0</v>
-      </c>
-      <c r="E94" s="126"/>
-    </row>
-    <row r="95" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A95" s="110" t="s">
+      <c r="C94" s="193"/>
+      <c r="D94" s="177" t="b">
+        <v>0</v>
+      </c>
+      <c r="E94" s="182"/>
+    </row>
+    <row r="95" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A95" s="170" t="s">
         <v>259</v>
       </c>
-      <c r="B95" s="113" t="s">
+      <c r="B95" s="188" t="s">
         <v>260</v>
       </c>
-      <c r="C95" s="114"/>
-      <c r="D95" s="107" t="s">
+      <c r="C95" s="189"/>
+      <c r="D95" s="174" t="s">
         <v>274</v>
       </c>
-      <c r="E95" s="109"/>
-    </row>
-    <row r="96" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A96" s="111"/>
-      <c r="B96" s="115" t="s">
+      <c r="E95" s="180"/>
+    </row>
+    <row r="96" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A96" s="170"/>
+      <c r="B96" s="190" t="s">
         <v>261</v>
       </c>
-      <c r="C96" s="116"/>
-      <c r="D96" s="107" t="s">
+      <c r="C96" s="191"/>
+      <c r="D96" s="174" t="s">
         <v>275</v>
       </c>
-      <c r="E96" s="109"/>
-    </row>
-    <row r="97" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A97" s="111"/>
-      <c r="B97" s="115" t="s">
+      <c r="E96" s="180"/>
+    </row>
+    <row r="97" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A97" s="170"/>
+      <c r="B97" s="190" t="s">
         <v>262</v>
       </c>
-      <c r="C97" s="116"/>
-      <c r="D97" s="107" t="s">
+      <c r="C97" s="191"/>
+      <c r="D97" s="174" t="s">
         <v>276</v>
       </c>
-      <c r="E97" s="109"/>
-    </row>
-    <row r="98" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A98" s="112"/>
-      <c r="B98" s="117" t="s">
+      <c r="E97" s="180"/>
+    </row>
+    <row r="98" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A98" s="170"/>
+      <c r="B98" s="192" t="s">
         <v>263</v>
       </c>
-      <c r="C98" s="118"/>
-      <c r="D98" s="107" t="s">
+      <c r="C98" s="193"/>
+      <c r="D98" s="174" t="s">
         <v>277</v>
       </c>
-      <c r="E98" s="109"/>
-    </row>
-    <row r="99" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A99" s="104" t="s">
+      <c r="E98" s="180"/>
+    </row>
+    <row r="99" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A99" s="187" t="s">
         <v>264</v>
       </c>
-      <c r="B99" s="107" t="s">
+      <c r="B99" s="183" t="s">
         <v>278</v>
       </c>
-      <c r="C99" s="108"/>
-      <c r="D99" s="108"/>
-      <c r="E99" s="109"/>
+      <c r="C99" s="183"/>
+      <c r="D99" s="183"/>
+      <c r="E99" s="184"/>
     </row>
   </sheetData>
   <mergeCells count="98">
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="H36:I36"/>
-    <mergeCell ref="A38:C38"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="H64:L64"/>
-    <mergeCell ref="A28:A35"/>
-    <mergeCell ref="A41:A48"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B99:E99"/>
+    <mergeCell ref="A95:A98"/>
+    <mergeCell ref="B95:C95"/>
+    <mergeCell ref="D95:E95"/>
+    <mergeCell ref="B96:C96"/>
+    <mergeCell ref="D96:E96"/>
+    <mergeCell ref="B97:C97"/>
+    <mergeCell ref="D97:E97"/>
+    <mergeCell ref="B98:C98"/>
+    <mergeCell ref="D98:E98"/>
+    <mergeCell ref="D89:E89"/>
+    <mergeCell ref="A90:A94"/>
+    <mergeCell ref="B90:C90"/>
+    <mergeCell ref="D90:E90"/>
+    <mergeCell ref="B91:C91"/>
+    <mergeCell ref="D91:E91"/>
+    <mergeCell ref="B92:C92"/>
+    <mergeCell ref="D92:E92"/>
+    <mergeCell ref="B93:C93"/>
+    <mergeCell ref="D93:E93"/>
+    <mergeCell ref="B94:C94"/>
+    <mergeCell ref="D94:E94"/>
+    <mergeCell ref="A85:E85"/>
+    <mergeCell ref="B86:E86"/>
+    <mergeCell ref="A87:A88"/>
+    <mergeCell ref="C87:E87"/>
+    <mergeCell ref="C88:E88"/>
+    <mergeCell ref="P81:R81"/>
+    <mergeCell ref="P82:R82"/>
+    <mergeCell ref="P83:R83"/>
+    <mergeCell ref="D80:F80"/>
+    <mergeCell ref="B79:F79"/>
+    <mergeCell ref="J80:L80"/>
+    <mergeCell ref="H79:L79"/>
+    <mergeCell ref="P80:R80"/>
+    <mergeCell ref="N79:R79"/>
+    <mergeCell ref="N81:N83"/>
+    <mergeCell ref="D81:F81"/>
+    <mergeCell ref="D82:F82"/>
+    <mergeCell ref="D83:F83"/>
+    <mergeCell ref="J81:L81"/>
+    <mergeCell ref="J82:L82"/>
+    <mergeCell ref="J83:L83"/>
+    <mergeCell ref="A81:A83"/>
+    <mergeCell ref="B81:B83"/>
+    <mergeCell ref="G81:G83"/>
+    <mergeCell ref="H81:H83"/>
+    <mergeCell ref="M81:M83"/>
+    <mergeCell ref="C65:F65"/>
+    <mergeCell ref="C66:F66"/>
+    <mergeCell ref="I66:L66"/>
+    <mergeCell ref="O66:R66"/>
+    <mergeCell ref="A62:R62"/>
+    <mergeCell ref="A63:F63"/>
+    <mergeCell ref="G63:L63"/>
+    <mergeCell ref="M63:R63"/>
+    <mergeCell ref="B64:F64"/>
+    <mergeCell ref="N64:R64"/>
+    <mergeCell ref="O65:R65"/>
+    <mergeCell ref="I65:L65"/>
+    <mergeCell ref="M65:M78"/>
+    <mergeCell ref="N67:N78"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A6:D6"/>
+    <mergeCell ref="A22:I22"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="D23:F23"/>
+    <mergeCell ref="G23:I23"/>
+    <mergeCell ref="B24:C24"/>
     <mergeCell ref="H26:I26"/>
     <mergeCell ref="H27:I27"/>
     <mergeCell ref="G65:G78"/>
@@ -3749,77 +3738,17 @@
     <mergeCell ref="B67:B78"/>
     <mergeCell ref="D28:D35"/>
     <mergeCell ref="G28:G35"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A6:D6"/>
-    <mergeCell ref="A22:I22"/>
-    <mergeCell ref="A23:C23"/>
-    <mergeCell ref="D23:F23"/>
-    <mergeCell ref="G23:I23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="C65:F65"/>
-    <mergeCell ref="C66:F66"/>
-    <mergeCell ref="I66:L66"/>
-    <mergeCell ref="O66:R66"/>
-    <mergeCell ref="A62:R62"/>
-    <mergeCell ref="A63:F63"/>
-    <mergeCell ref="G63:L63"/>
-    <mergeCell ref="M63:R63"/>
-    <mergeCell ref="B64:F64"/>
-    <mergeCell ref="N64:R64"/>
-    <mergeCell ref="O65:R65"/>
-    <mergeCell ref="I65:L65"/>
-    <mergeCell ref="M65:M78"/>
-    <mergeCell ref="N67:N78"/>
-    <mergeCell ref="A81:A83"/>
-    <mergeCell ref="B81:B83"/>
-    <mergeCell ref="G81:G83"/>
-    <mergeCell ref="H81:H83"/>
-    <mergeCell ref="M81:M83"/>
-    <mergeCell ref="P81:R81"/>
-    <mergeCell ref="P82:R82"/>
-    <mergeCell ref="P83:R83"/>
-    <mergeCell ref="D80:F80"/>
-    <mergeCell ref="B79:F79"/>
-    <mergeCell ref="J80:L80"/>
-    <mergeCell ref="H79:L79"/>
-    <mergeCell ref="P80:R80"/>
-    <mergeCell ref="N79:R79"/>
-    <mergeCell ref="N81:N83"/>
-    <mergeCell ref="D81:F81"/>
-    <mergeCell ref="D82:F82"/>
-    <mergeCell ref="D83:F83"/>
-    <mergeCell ref="J81:L81"/>
-    <mergeCell ref="J82:L82"/>
-    <mergeCell ref="J83:L83"/>
-    <mergeCell ref="A85:E85"/>
-    <mergeCell ref="B86:E86"/>
-    <mergeCell ref="A87:A88"/>
-    <mergeCell ref="C87:E87"/>
-    <mergeCell ref="C88:E88"/>
-    <mergeCell ref="D89:E89"/>
-    <mergeCell ref="A90:A94"/>
-    <mergeCell ref="B90:C90"/>
-    <mergeCell ref="D90:E90"/>
-    <mergeCell ref="B91:C91"/>
-    <mergeCell ref="D91:E91"/>
-    <mergeCell ref="B92:C92"/>
-    <mergeCell ref="D92:E92"/>
-    <mergeCell ref="B93:C93"/>
-    <mergeCell ref="D93:E93"/>
-    <mergeCell ref="B94:C94"/>
-    <mergeCell ref="D94:E94"/>
-    <mergeCell ref="B99:E99"/>
-    <mergeCell ref="A95:A98"/>
-    <mergeCell ref="B95:C95"/>
-    <mergeCell ref="D95:E95"/>
-    <mergeCell ref="B96:C96"/>
-    <mergeCell ref="D96:E96"/>
-    <mergeCell ref="B97:C97"/>
-    <mergeCell ref="D97:E97"/>
-    <mergeCell ref="B98:C98"/>
-    <mergeCell ref="D98:E98"/>
+    <mergeCell ref="A28:A35"/>
+    <mergeCell ref="A41:A48"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="H36:I36"/>
+    <mergeCell ref="A38:C38"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="H64:L64"/>
   </mergeCells>
   <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="B20" xr:uid="{00000000-0002-0000-0000-000000000000}">
@@ -3872,421 +3801,421 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:175" x14ac:dyDescent="0.25">
-      <c r="A1" s="185" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="151"/>
-      <c r="C1" s="152"/>
-      <c r="D1" s="185" t="s">
+      <c r="A1" s="161" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="112"/>
+      <c r="C1" s="113"/>
+      <c r="D1" s="161" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="151"/>
-      <c r="F1" s="151"/>
-      <c r="G1" s="151"/>
-      <c r="H1" s="151"/>
-      <c r="I1" s="151"/>
-      <c r="J1" s="151"/>
-      <c r="K1" s="151"/>
-      <c r="L1" s="151"/>
-      <c r="M1" s="151"/>
-      <c r="N1" s="151"/>
-      <c r="O1" s="152"/>
-      <c r="P1" s="185" t="s">
+      <c r="E1" s="112"/>
+      <c r="F1" s="112"/>
+      <c r="G1" s="112"/>
+      <c r="H1" s="112"/>
+      <c r="I1" s="112"/>
+      <c r="J1" s="112"/>
+      <c r="K1" s="112"/>
+      <c r="L1" s="112"/>
+      <c r="M1" s="112"/>
+      <c r="N1" s="112"/>
+      <c r="O1" s="113"/>
+      <c r="P1" s="161" t="s">
         <v>82</v>
       </c>
-      <c r="Q1" s="151"/>
-      <c r="R1" s="151"/>
-      <c r="S1" s="152"/>
-      <c r="T1" s="182" t="s">
+      <c r="Q1" s="112"/>
+      <c r="R1" s="112"/>
+      <c r="S1" s="113"/>
+      <c r="T1" s="160" t="s">
         <v>83</v>
       </c>
-      <c r="U1" s="151"/>
-      <c r="V1" s="151"/>
-      <c r="W1" s="151"/>
-      <c r="X1" s="151"/>
-      <c r="Y1" s="151"/>
-      <c r="Z1" s="151"/>
-      <c r="AA1" s="151"/>
-      <c r="AB1" s="151"/>
-      <c r="AC1" s="151"/>
-      <c r="AD1" s="151"/>
-      <c r="AE1" s="151"/>
-      <c r="AF1" s="152"/>
-      <c r="AG1" s="182" t="s">
+      <c r="U1" s="112"/>
+      <c r="V1" s="112"/>
+      <c r="W1" s="112"/>
+      <c r="X1" s="112"/>
+      <c r="Y1" s="112"/>
+      <c r="Z1" s="112"/>
+      <c r="AA1" s="112"/>
+      <c r="AB1" s="112"/>
+      <c r="AC1" s="112"/>
+      <c r="AD1" s="112"/>
+      <c r="AE1" s="112"/>
+      <c r="AF1" s="113"/>
+      <c r="AG1" s="160" t="s">
         <v>84</v>
       </c>
-      <c r="AH1" s="151"/>
-      <c r="AI1" s="151"/>
-      <c r="AJ1" s="151"/>
-      <c r="AK1" s="151"/>
-      <c r="AL1" s="151"/>
-      <c r="AM1" s="151"/>
-      <c r="AN1" s="151"/>
-      <c r="AO1" s="151"/>
-      <c r="AP1" s="151"/>
-      <c r="AQ1" s="151"/>
-      <c r="AR1" s="151"/>
-      <c r="AS1" s="152"/>
-      <c r="AT1" s="182" t="s">
+      <c r="AH1" s="112"/>
+      <c r="AI1" s="112"/>
+      <c r="AJ1" s="112"/>
+      <c r="AK1" s="112"/>
+      <c r="AL1" s="112"/>
+      <c r="AM1" s="112"/>
+      <c r="AN1" s="112"/>
+      <c r="AO1" s="112"/>
+      <c r="AP1" s="112"/>
+      <c r="AQ1" s="112"/>
+      <c r="AR1" s="112"/>
+      <c r="AS1" s="113"/>
+      <c r="AT1" s="160" t="s">
         <v>48</v>
       </c>
-      <c r="AU1" s="151"/>
-      <c r="AV1" s="151"/>
-      <c r="AW1" s="151"/>
-      <c r="AX1" s="151"/>
-      <c r="AY1" s="151"/>
-      <c r="AZ1" s="152"/>
-      <c r="BA1" s="182" t="s">
+      <c r="AU1" s="112"/>
+      <c r="AV1" s="112"/>
+      <c r="AW1" s="112"/>
+      <c r="AX1" s="112"/>
+      <c r="AY1" s="112"/>
+      <c r="AZ1" s="113"/>
+      <c r="BA1" s="160" t="s">
         <v>85</v>
       </c>
-      <c r="BB1" s="151"/>
-      <c r="BC1" s="151"/>
-      <c r="BD1" s="151"/>
-      <c r="BE1" s="151"/>
-      <c r="BF1" s="151"/>
-      <c r="BG1" s="151"/>
-      <c r="BH1" s="151"/>
-      <c r="BI1" s="151"/>
-      <c r="BJ1" s="151"/>
-      <c r="BK1" s="151"/>
-      <c r="BL1" s="151"/>
-      <c r="BM1" s="151"/>
-      <c r="BN1" s="151"/>
-      <c r="BO1" s="151"/>
-      <c r="BP1" s="151"/>
-      <c r="BQ1" s="151"/>
-      <c r="BR1" s="151"/>
-      <c r="BS1" s="151"/>
-      <c r="BT1" s="151"/>
-      <c r="BU1" s="151"/>
-      <c r="BV1" s="151"/>
-      <c r="BW1" s="151"/>
-      <c r="BX1" s="151"/>
-      <c r="BY1" s="151"/>
-      <c r="BZ1" s="151"/>
-      <c r="CA1" s="151"/>
-      <c r="CB1" s="151"/>
-      <c r="CC1" s="151"/>
-      <c r="CD1" s="151"/>
-      <c r="CE1" s="151"/>
-      <c r="CF1" s="151"/>
-      <c r="CG1" s="151"/>
-      <c r="CH1" s="151"/>
-      <c r="CI1" s="151"/>
-      <c r="CJ1" s="151"/>
-      <c r="CK1" s="151"/>
-      <c r="CL1" s="151"/>
-      <c r="CM1" s="152"/>
+      <c r="BB1" s="112"/>
+      <c r="BC1" s="112"/>
+      <c r="BD1" s="112"/>
+      <c r="BE1" s="112"/>
+      <c r="BF1" s="112"/>
+      <c r="BG1" s="112"/>
+      <c r="BH1" s="112"/>
+      <c r="BI1" s="112"/>
+      <c r="BJ1" s="112"/>
+      <c r="BK1" s="112"/>
+      <c r="BL1" s="112"/>
+      <c r="BM1" s="112"/>
+      <c r="BN1" s="112"/>
+      <c r="BO1" s="112"/>
+      <c r="BP1" s="112"/>
+      <c r="BQ1" s="112"/>
+      <c r="BR1" s="112"/>
+      <c r="BS1" s="112"/>
+      <c r="BT1" s="112"/>
+      <c r="BU1" s="112"/>
+      <c r="BV1" s="112"/>
+      <c r="BW1" s="112"/>
+      <c r="BX1" s="112"/>
+      <c r="BY1" s="112"/>
+      <c r="BZ1" s="112"/>
+      <c r="CA1" s="112"/>
+      <c r="CB1" s="112"/>
+      <c r="CC1" s="112"/>
+      <c r="CD1" s="112"/>
+      <c r="CE1" s="112"/>
+      <c r="CF1" s="112"/>
+      <c r="CG1" s="112"/>
+      <c r="CH1" s="112"/>
+      <c r="CI1" s="112"/>
+      <c r="CJ1" s="112"/>
+      <c r="CK1" s="112"/>
+      <c r="CL1" s="112"/>
+      <c r="CM1" s="113"/>
     </row>
     <row r="2" spans="1:175" x14ac:dyDescent="0.25">
-      <c r="A2" s="186" t="s">
+      <c r="A2" s="162" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="183" t="s">
+      <c r="B2" s="159" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="183" t="s">
+      <c r="C2" s="159" t="s">
         <v>86</v>
       </c>
-      <c r="D2" s="183" t="s">
+      <c r="D2" s="159" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="183" t="s">
+      <c r="E2" s="159" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="183" t="s">
+      <c r="F2" s="159" t="s">
         <v>87</v>
       </c>
-      <c r="G2" s="183" t="s">
+      <c r="G2" s="159" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="183" t="s">
+      <c r="H2" s="159" t="s">
         <v>10</v>
       </c>
-      <c r="I2" s="183" t="s">
+      <c r="I2" s="159" t="s">
         <v>11</v>
       </c>
-      <c r="J2" s="183" t="s">
+      <c r="J2" s="159" t="s">
         <v>12</v>
       </c>
-      <c r="K2" s="183" t="s">
+      <c r="K2" s="159" t="s">
         <v>13</v>
       </c>
-      <c r="L2" s="183" t="s">
+      <c r="L2" s="159" t="s">
         <v>88</v>
       </c>
-      <c r="M2" s="183" t="s">
+      <c r="M2" s="159" t="s">
         <v>15</v>
       </c>
-      <c r="N2" s="183" t="s">
+      <c r="N2" s="159" t="s">
         <v>16</v>
       </c>
-      <c r="O2" s="183" t="s">
+      <c r="O2" s="159" t="s">
         <v>89</v>
       </c>
-      <c r="P2" s="183" t="s">
+      <c r="P2" s="159" t="s">
         <v>90</v>
       </c>
-      <c r="Q2" s="183" t="s">
+      <c r="Q2" s="159" t="s">
         <v>91</v>
       </c>
-      <c r="R2" s="183" t="s">
+      <c r="R2" s="159" t="s">
         <v>23</v>
       </c>
-      <c r="S2" s="183" t="s">
+      <c r="S2" s="159" t="s">
         <v>25</v>
       </c>
-      <c r="T2" s="183" t="s">
+      <c r="T2" s="159" t="s">
         <v>30</v>
       </c>
-      <c r="U2" s="183" t="s">
+      <c r="U2" s="159" t="s">
         <v>6</v>
       </c>
-      <c r="V2" s="183" t="s">
+      <c r="V2" s="159" t="s">
         <v>92</v>
       </c>
-      <c r="W2" s="183" t="s">
+      <c r="W2" s="159" t="s">
         <v>93</v>
       </c>
-      <c r="X2" s="182" t="s">
+      <c r="X2" s="160" t="s">
         <v>32</v>
       </c>
-      <c r="Y2" s="151"/>
-      <c r="Z2" s="151"/>
-      <c r="AA2" s="151"/>
-      <c r="AB2" s="151"/>
-      <c r="AC2" s="151"/>
-      <c r="AD2" s="151"/>
-      <c r="AE2" s="152"/>
-      <c r="AF2" s="183" t="s">
+      <c r="Y2" s="112"/>
+      <c r="Z2" s="112"/>
+      <c r="AA2" s="112"/>
+      <c r="AB2" s="112"/>
+      <c r="AC2" s="112"/>
+      <c r="AD2" s="112"/>
+      <c r="AE2" s="113"/>
+      <c r="AF2" s="159" t="s">
         <v>41</v>
       </c>
-      <c r="AG2" s="183" t="s">
+      <c r="AG2" s="159" t="s">
         <v>94</v>
       </c>
-      <c r="AH2" s="183" t="s">
+      <c r="AH2" s="159" t="s">
         <v>44</v>
       </c>
-      <c r="AI2" s="185" t="s">
+      <c r="AI2" s="161" t="s">
         <v>32</v>
       </c>
-      <c r="AJ2" s="151"/>
-      <c r="AK2" s="151"/>
-      <c r="AL2" s="151"/>
-      <c r="AM2" s="151"/>
-      <c r="AN2" s="151"/>
-      <c r="AO2" s="151"/>
-      <c r="AP2" s="152"/>
-      <c r="AQ2" s="183" t="s">
+      <c r="AJ2" s="112"/>
+      <c r="AK2" s="112"/>
+      <c r="AL2" s="112"/>
+      <c r="AM2" s="112"/>
+      <c r="AN2" s="112"/>
+      <c r="AO2" s="112"/>
+      <c r="AP2" s="113"/>
+      <c r="AQ2" s="159" t="s">
         <v>41</v>
       </c>
-      <c r="AR2" s="183" t="s">
+      <c r="AR2" s="159" t="s">
         <v>46</v>
       </c>
-      <c r="AS2" s="183" t="s">
+      <c r="AS2" s="159" t="s">
         <v>47</v>
       </c>
-      <c r="AT2" s="183" t="s">
+      <c r="AT2" s="159" t="s">
         <v>95</v>
       </c>
-      <c r="AU2" s="183" t="s">
+      <c r="AU2" s="159" t="s">
         <v>50</v>
       </c>
-      <c r="AV2" s="183" t="s">
+      <c r="AV2" s="159" t="s">
         <v>51</v>
       </c>
-      <c r="AW2" s="183" t="s">
+      <c r="AW2" s="159" t="s">
         <v>52</v>
       </c>
-      <c r="AX2" s="183" t="s">
+      <c r="AX2" s="159" t="s">
         <v>22</v>
       </c>
-      <c r="AY2" s="183" t="s">
+      <c r="AY2" s="159" t="s">
         <v>53</v>
       </c>
-      <c r="AZ2" s="183" t="s">
+      <c r="AZ2" s="159" t="s">
         <v>54</v>
       </c>
-      <c r="BA2" s="183" t="s">
+      <c r="BA2" s="159" t="s">
         <v>30</v>
       </c>
-      <c r="BB2" s="182" t="s">
+      <c r="BB2" s="160" t="s">
         <v>59</v>
       </c>
-      <c r="BC2" s="151"/>
-      <c r="BD2" s="151"/>
-      <c r="BE2" s="151"/>
-      <c r="BF2" s="151"/>
-      <c r="BG2" s="151"/>
-      <c r="BH2" s="151"/>
-      <c r="BI2" s="151"/>
-      <c r="BJ2" s="151"/>
-      <c r="BK2" s="151"/>
-      <c r="BL2" s="151"/>
-      <c r="BM2" s="151"/>
-      <c r="BN2" s="151"/>
-      <c r="BO2" s="151"/>
-      <c r="BP2" s="151"/>
-      <c r="BQ2" s="151"/>
-      <c r="BR2" s="151"/>
-      <c r="BS2" s="151"/>
-      <c r="BT2" s="151"/>
-      <c r="BU2" s="151"/>
-      <c r="BV2" s="151"/>
-      <c r="BW2" s="151"/>
-      <c r="BX2" s="151"/>
-      <c r="BY2" s="151"/>
-      <c r="BZ2" s="151"/>
-      <c r="CA2" s="151"/>
-      <c r="CB2" s="151"/>
-      <c r="CC2" s="151"/>
-      <c r="CD2" s="151"/>
-      <c r="CE2" s="151"/>
-      <c r="CF2" s="151"/>
-      <c r="CG2" s="151"/>
-      <c r="CH2" s="151"/>
-      <c r="CI2" s="151"/>
-      <c r="CJ2" s="152"/>
-      <c r="CK2" s="183" t="s">
+      <c r="BC2" s="112"/>
+      <c r="BD2" s="112"/>
+      <c r="BE2" s="112"/>
+      <c r="BF2" s="112"/>
+      <c r="BG2" s="112"/>
+      <c r="BH2" s="112"/>
+      <c r="BI2" s="112"/>
+      <c r="BJ2" s="112"/>
+      <c r="BK2" s="112"/>
+      <c r="BL2" s="112"/>
+      <c r="BM2" s="112"/>
+      <c r="BN2" s="112"/>
+      <c r="BO2" s="112"/>
+      <c r="BP2" s="112"/>
+      <c r="BQ2" s="112"/>
+      <c r="BR2" s="112"/>
+      <c r="BS2" s="112"/>
+      <c r="BT2" s="112"/>
+      <c r="BU2" s="112"/>
+      <c r="BV2" s="112"/>
+      <c r="BW2" s="112"/>
+      <c r="BX2" s="112"/>
+      <c r="BY2" s="112"/>
+      <c r="BZ2" s="112"/>
+      <c r="CA2" s="112"/>
+      <c r="CB2" s="112"/>
+      <c r="CC2" s="112"/>
+      <c r="CD2" s="112"/>
+      <c r="CE2" s="112"/>
+      <c r="CF2" s="112"/>
+      <c r="CG2" s="112"/>
+      <c r="CH2" s="112"/>
+      <c r="CI2" s="112"/>
+      <c r="CJ2" s="113"/>
+      <c r="CK2" s="159" t="s">
         <v>79</v>
       </c>
-      <c r="CL2" s="183" t="s">
+      <c r="CL2" s="159" t="s">
         <v>80</v>
       </c>
-      <c r="CM2" s="183" t="s">
+      <c r="CM2" s="159" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:175" x14ac:dyDescent="0.25">
-      <c r="A3" s="158"/>
-      <c r="B3" s="158"/>
-      <c r="C3" s="158"/>
-      <c r="D3" s="158"/>
-      <c r="E3" s="158"/>
-      <c r="F3" s="158"/>
-      <c r="G3" s="158"/>
-      <c r="H3" s="158"/>
-      <c r="I3" s="158"/>
-      <c r="J3" s="158"/>
-      <c r="K3" s="158"/>
-      <c r="L3" s="158"/>
-      <c r="M3" s="158"/>
-      <c r="N3" s="158"/>
-      <c r="O3" s="158"/>
-      <c r="P3" s="158"/>
-      <c r="Q3" s="158"/>
-      <c r="R3" s="158"/>
-      <c r="S3" s="158"/>
-      <c r="T3" s="158"/>
-      <c r="U3" s="158"/>
-      <c r="V3" s="158"/>
-      <c r="W3" s="158"/>
-      <c r="X3" s="183" t="s">
+      <c r="A3" s="115"/>
+      <c r="B3" s="115"/>
+      <c r="C3" s="115"/>
+      <c r="D3" s="115"/>
+      <c r="E3" s="115"/>
+      <c r="F3" s="115"/>
+      <c r="G3" s="115"/>
+      <c r="H3" s="115"/>
+      <c r="I3" s="115"/>
+      <c r="J3" s="115"/>
+      <c r="K3" s="115"/>
+      <c r="L3" s="115"/>
+      <c r="M3" s="115"/>
+      <c r="N3" s="115"/>
+      <c r="O3" s="115"/>
+      <c r="P3" s="115"/>
+      <c r="Q3" s="115"/>
+      <c r="R3" s="115"/>
+      <c r="S3" s="115"/>
+      <c r="T3" s="115"/>
+      <c r="U3" s="115"/>
+      <c r="V3" s="115"/>
+      <c r="W3" s="115"/>
+      <c r="X3" s="159" t="s">
         <v>96</v>
       </c>
-      <c r="Y3" s="183" t="s">
+      <c r="Y3" s="159" t="s">
         <v>34</v>
       </c>
-      <c r="Z3" s="183" t="s">
+      <c r="Z3" s="159" t="s">
         <v>35</v>
       </c>
-      <c r="AA3" s="183" t="s">
+      <c r="AA3" s="159" t="s">
         <v>36</v>
       </c>
-      <c r="AB3" s="183" t="s">
+      <c r="AB3" s="159" t="s">
         <v>37</v>
       </c>
-      <c r="AC3" s="183" t="s">
+      <c r="AC3" s="159" t="s">
         <v>38</v>
       </c>
-      <c r="AD3" s="183" t="s">
+      <c r="AD3" s="159" t="s">
         <v>39</v>
       </c>
-      <c r="AE3" s="183" t="s">
+      <c r="AE3" s="159" t="s">
         <v>40</v>
       </c>
-      <c r="AF3" s="158"/>
-      <c r="AG3" s="158"/>
-      <c r="AH3" s="158"/>
-      <c r="AI3" s="183" t="s">
+      <c r="AF3" s="115"/>
+      <c r="AG3" s="115"/>
+      <c r="AH3" s="115"/>
+      <c r="AI3" s="159" t="s">
         <v>97</v>
       </c>
-      <c r="AJ3" s="183" t="s">
+      <c r="AJ3" s="159" t="s">
         <v>34</v>
       </c>
-      <c r="AK3" s="183" t="s">
+      <c r="AK3" s="159" t="s">
         <v>35</v>
       </c>
-      <c r="AL3" s="183" t="s">
+      <c r="AL3" s="159" t="s">
         <v>36</v>
       </c>
-      <c r="AM3" s="183" t="s">
+      <c r="AM3" s="159" t="s">
         <v>37</v>
       </c>
-      <c r="AN3" s="183" t="s">
+      <c r="AN3" s="159" t="s">
         <v>98</v>
       </c>
-      <c r="AO3" s="183" t="s">
+      <c r="AO3" s="159" t="s">
         <v>39</v>
       </c>
-      <c r="AP3" s="183" t="s">
+      <c r="AP3" s="159" t="s">
         <v>40</v>
       </c>
-      <c r="AQ3" s="158"/>
-      <c r="AR3" s="158"/>
-      <c r="AS3" s="158"/>
-      <c r="AT3" s="158"/>
-      <c r="AU3" s="158"/>
-      <c r="AV3" s="158"/>
-      <c r="AW3" s="158"/>
-      <c r="AX3" s="158"/>
-      <c r="AY3" s="158"/>
-      <c r="AZ3" s="158"/>
-      <c r="BA3" s="158"/>
-      <c r="BB3" s="184" t="s">
+      <c r="AQ3" s="115"/>
+      <c r="AR3" s="115"/>
+      <c r="AS3" s="115"/>
+      <c r="AT3" s="115"/>
+      <c r="AU3" s="115"/>
+      <c r="AV3" s="115"/>
+      <c r="AW3" s="115"/>
+      <c r="AX3" s="115"/>
+      <c r="AY3" s="115"/>
+      <c r="AZ3" s="115"/>
+      <c r="BA3" s="115"/>
+      <c r="BB3" s="163" t="s">
         <v>60</v>
       </c>
-      <c r="BC3" s="184" t="s">
+      <c r="BC3" s="163" t="s">
         <v>61</v>
       </c>
       <c r="BD3" s="34"/>
-      <c r="BE3" s="176" t="s">
+      <c r="BE3" s="122" t="s">
         <v>62</v>
       </c>
-      <c r="BF3" s="148"/>
-      <c r="BG3" s="148"/>
-      <c r="BH3" s="148"/>
-      <c r="BI3" s="148"/>
-      <c r="BJ3" s="148"/>
-      <c r="BK3" s="148"/>
-      <c r="BL3" s="148"/>
-      <c r="BM3" s="148"/>
-      <c r="BN3" s="148"/>
-      <c r="BO3" s="148"/>
-      <c r="BP3" s="148"/>
-      <c r="BQ3" s="148"/>
-      <c r="BR3" s="148"/>
-      <c r="BS3" s="148"/>
-      <c r="BT3" s="148"/>
-      <c r="BU3" s="148"/>
-      <c r="BV3" s="148"/>
-      <c r="BW3" s="148"/>
-      <c r="BX3" s="148"/>
-      <c r="BY3" s="148"/>
-      <c r="BZ3" s="148"/>
-      <c r="CA3" s="148"/>
-      <c r="CB3" s="148"/>
-      <c r="CC3" s="148"/>
-      <c r="CD3" s="148"/>
-      <c r="CE3" s="148"/>
-      <c r="CF3" s="148"/>
-      <c r="CG3" s="148"/>
-      <c r="CH3" s="148"/>
-      <c r="CI3" s="148"/>
-      <c r="CJ3" s="148"/>
-      <c r="CK3" s="158"/>
-      <c r="CL3" s="158"/>
-      <c r="CM3" s="158"/>
+      <c r="BF3" s="137"/>
+      <c r="BG3" s="137"/>
+      <c r="BH3" s="137"/>
+      <c r="BI3" s="137"/>
+      <c r="BJ3" s="137"/>
+      <c r="BK3" s="137"/>
+      <c r="BL3" s="137"/>
+      <c r="BM3" s="137"/>
+      <c r="BN3" s="137"/>
+      <c r="BO3" s="137"/>
+      <c r="BP3" s="137"/>
+      <c r="BQ3" s="137"/>
+      <c r="BR3" s="137"/>
+      <c r="BS3" s="137"/>
+      <c r="BT3" s="137"/>
+      <c r="BU3" s="137"/>
+      <c r="BV3" s="137"/>
+      <c r="BW3" s="137"/>
+      <c r="BX3" s="137"/>
+      <c r="BY3" s="137"/>
+      <c r="BZ3" s="137"/>
+      <c r="CA3" s="137"/>
+      <c r="CB3" s="137"/>
+      <c r="CC3" s="137"/>
+      <c r="CD3" s="137"/>
+      <c r="CE3" s="137"/>
+      <c r="CF3" s="137"/>
+      <c r="CG3" s="137"/>
+      <c r="CH3" s="137"/>
+      <c r="CI3" s="137"/>
+      <c r="CJ3" s="137"/>
+      <c r="CK3" s="115"/>
+      <c r="CL3" s="115"/>
+      <c r="CM3" s="115"/>
       <c r="CN3" s="21"/>
       <c r="CO3" s="21"/>
       <c r="CP3" s="21"/>
@@ -4372,176 +4301,176 @@
       <c r="FS3" s="21"/>
     </row>
     <row r="4" spans="1:175" x14ac:dyDescent="0.25">
-      <c r="A4" s="158"/>
-      <c r="B4" s="158"/>
-      <c r="C4" s="158"/>
-      <c r="D4" s="158"/>
-      <c r="E4" s="158"/>
-      <c r="F4" s="158"/>
-      <c r="G4" s="158"/>
-      <c r="H4" s="158"/>
-      <c r="I4" s="158"/>
-      <c r="J4" s="158"/>
-      <c r="K4" s="158"/>
-      <c r="L4" s="158"/>
-      <c r="M4" s="158"/>
-      <c r="N4" s="158"/>
-      <c r="O4" s="158"/>
-      <c r="P4" s="158"/>
-      <c r="Q4" s="158"/>
-      <c r="R4" s="158"/>
-      <c r="S4" s="158"/>
-      <c r="T4" s="158"/>
-      <c r="U4" s="158"/>
-      <c r="V4" s="158"/>
-      <c r="W4" s="158"/>
-      <c r="X4" s="158"/>
-      <c r="Y4" s="158"/>
-      <c r="Z4" s="158"/>
-      <c r="AA4" s="158"/>
-      <c r="AB4" s="158"/>
-      <c r="AC4" s="158"/>
-      <c r="AD4" s="158"/>
-      <c r="AE4" s="158"/>
-      <c r="AF4" s="158"/>
-      <c r="AG4" s="158"/>
-      <c r="AH4" s="158"/>
-      <c r="AI4" s="158"/>
-      <c r="AJ4" s="158"/>
-      <c r="AK4" s="158"/>
-      <c r="AL4" s="158"/>
-      <c r="AM4" s="158"/>
-      <c r="AN4" s="158"/>
-      <c r="AO4" s="158"/>
-      <c r="AP4" s="158"/>
-      <c r="AQ4" s="158"/>
-      <c r="AR4" s="158"/>
-      <c r="AS4" s="158"/>
-      <c r="AT4" s="158"/>
-      <c r="AU4" s="158"/>
-      <c r="AV4" s="158"/>
-      <c r="AW4" s="158"/>
-      <c r="AX4" s="158"/>
-      <c r="AY4" s="158"/>
-      <c r="AZ4" s="158"/>
-      <c r="BA4" s="158"/>
-      <c r="BB4" s="158"/>
-      <c r="BC4" s="158"/>
-      <c r="BD4" s="182" t="s">
+      <c r="A4" s="115"/>
+      <c r="B4" s="115"/>
+      <c r="C4" s="115"/>
+      <c r="D4" s="115"/>
+      <c r="E4" s="115"/>
+      <c r="F4" s="115"/>
+      <c r="G4" s="115"/>
+      <c r="H4" s="115"/>
+      <c r="I4" s="115"/>
+      <c r="J4" s="115"/>
+      <c r="K4" s="115"/>
+      <c r="L4" s="115"/>
+      <c r="M4" s="115"/>
+      <c r="N4" s="115"/>
+      <c r="O4" s="115"/>
+      <c r="P4" s="115"/>
+      <c r="Q4" s="115"/>
+      <c r="R4" s="115"/>
+      <c r="S4" s="115"/>
+      <c r="T4" s="115"/>
+      <c r="U4" s="115"/>
+      <c r="V4" s="115"/>
+      <c r="W4" s="115"/>
+      <c r="X4" s="115"/>
+      <c r="Y4" s="115"/>
+      <c r="Z4" s="115"/>
+      <c r="AA4" s="115"/>
+      <c r="AB4" s="115"/>
+      <c r="AC4" s="115"/>
+      <c r="AD4" s="115"/>
+      <c r="AE4" s="115"/>
+      <c r="AF4" s="115"/>
+      <c r="AG4" s="115"/>
+      <c r="AH4" s="115"/>
+      <c r="AI4" s="115"/>
+      <c r="AJ4" s="115"/>
+      <c r="AK4" s="115"/>
+      <c r="AL4" s="115"/>
+      <c r="AM4" s="115"/>
+      <c r="AN4" s="115"/>
+      <c r="AO4" s="115"/>
+      <c r="AP4" s="115"/>
+      <c r="AQ4" s="115"/>
+      <c r="AR4" s="115"/>
+      <c r="AS4" s="115"/>
+      <c r="AT4" s="115"/>
+      <c r="AU4" s="115"/>
+      <c r="AV4" s="115"/>
+      <c r="AW4" s="115"/>
+      <c r="AX4" s="115"/>
+      <c r="AY4" s="115"/>
+      <c r="AZ4" s="115"/>
+      <c r="BA4" s="115"/>
+      <c r="BB4" s="115"/>
+      <c r="BC4" s="115"/>
+      <c r="BD4" s="160" t="s">
         <v>67</v>
       </c>
-      <c r="BE4" s="151"/>
-      <c r="BF4" s="152"/>
-      <c r="BG4" s="182" t="s">
+      <c r="BE4" s="112"/>
+      <c r="BF4" s="113"/>
+      <c r="BG4" s="160" t="s">
         <v>67</v>
       </c>
-      <c r="BH4" s="151"/>
-      <c r="BI4" s="152"/>
-      <c r="BJ4" s="182" t="s">
+      <c r="BH4" s="112"/>
+      <c r="BI4" s="113"/>
+      <c r="BJ4" s="160" t="s">
         <v>70</v>
       </c>
-      <c r="BK4" s="151"/>
-      <c r="BL4" s="152"/>
-      <c r="BM4" s="182" t="s">
+      <c r="BK4" s="112"/>
+      <c r="BL4" s="113"/>
+      <c r="BM4" s="160" t="s">
         <v>71</v>
       </c>
-      <c r="BN4" s="151"/>
-      <c r="BO4" s="152"/>
-      <c r="BP4" s="182" t="s">
+      <c r="BN4" s="112"/>
+      <c r="BO4" s="113"/>
+      <c r="BP4" s="160" t="s">
         <v>72</v>
       </c>
-      <c r="BQ4" s="151"/>
-      <c r="BR4" s="152"/>
-      <c r="BS4" s="182" t="s">
+      <c r="BQ4" s="112"/>
+      <c r="BR4" s="113"/>
+      <c r="BS4" s="160" t="s">
         <v>73</v>
       </c>
-      <c r="BT4" s="151"/>
-      <c r="BU4" s="152"/>
-      <c r="BV4" s="182" t="s">
+      <c r="BT4" s="112"/>
+      <c r="BU4" s="113"/>
+      <c r="BV4" s="160" t="s">
         <v>74</v>
       </c>
-      <c r="BW4" s="151"/>
-      <c r="BX4" s="152"/>
-      <c r="BY4" s="182" t="s">
+      <c r="BW4" s="112"/>
+      <c r="BX4" s="113"/>
+      <c r="BY4" s="160" t="s">
         <v>75</v>
       </c>
-      <c r="BZ4" s="151"/>
-      <c r="CA4" s="152"/>
-      <c r="CB4" s="182" t="s">
+      <c r="BZ4" s="112"/>
+      <c r="CA4" s="113"/>
+      <c r="CB4" s="160" t="s">
         <v>76</v>
       </c>
-      <c r="CC4" s="151"/>
-      <c r="CD4" s="152"/>
-      <c r="CE4" s="182" t="s">
+      <c r="CC4" s="112"/>
+      <c r="CD4" s="113"/>
+      <c r="CE4" s="160" t="s">
         <v>77</v>
       </c>
-      <c r="CF4" s="151"/>
-      <c r="CG4" s="152"/>
-      <c r="CH4" s="182" t="s">
+      <c r="CF4" s="112"/>
+      <c r="CG4" s="113"/>
+      <c r="CH4" s="160" t="s">
         <v>78</v>
       </c>
-      <c r="CI4" s="151"/>
-      <c r="CJ4" s="152"/>
-      <c r="CK4" s="158"/>
-      <c r="CL4" s="158"/>
-      <c r="CM4" s="158"/>
+      <c r="CI4" s="112"/>
+      <c r="CJ4" s="113"/>
+      <c r="CK4" s="115"/>
+      <c r="CL4" s="115"/>
+      <c r="CM4" s="115"/>
     </row>
     <row r="5" spans="1:175" x14ac:dyDescent="0.25">
-      <c r="A5" s="170"/>
-      <c r="B5" s="170"/>
-      <c r="C5" s="170"/>
-      <c r="D5" s="170"/>
-      <c r="E5" s="170"/>
-      <c r="F5" s="170"/>
-      <c r="G5" s="170"/>
-      <c r="H5" s="170"/>
-      <c r="I5" s="170"/>
-      <c r="J5" s="170"/>
-      <c r="K5" s="170"/>
-      <c r="L5" s="170"/>
-      <c r="M5" s="170"/>
-      <c r="N5" s="170"/>
-      <c r="O5" s="170"/>
-      <c r="P5" s="170"/>
-      <c r="Q5" s="170"/>
-      <c r="R5" s="170"/>
-      <c r="S5" s="170"/>
-      <c r="T5" s="170"/>
-      <c r="U5" s="170"/>
-      <c r="V5" s="170"/>
-      <c r="W5" s="170"/>
-      <c r="X5" s="170"/>
-      <c r="Y5" s="170"/>
-      <c r="Z5" s="170"/>
-      <c r="AA5" s="170"/>
-      <c r="AB5" s="170"/>
-      <c r="AC5" s="170"/>
-      <c r="AD5" s="170"/>
-      <c r="AE5" s="170"/>
-      <c r="AF5" s="170"/>
-      <c r="AG5" s="170"/>
-      <c r="AH5" s="170"/>
-      <c r="AI5" s="170"/>
-      <c r="AJ5" s="170"/>
-      <c r="AK5" s="170"/>
-      <c r="AL5" s="170"/>
-      <c r="AM5" s="170"/>
-      <c r="AN5" s="170"/>
-      <c r="AO5" s="170"/>
-      <c r="AP5" s="170"/>
-      <c r="AQ5" s="170"/>
-      <c r="AR5" s="170"/>
-      <c r="AS5" s="170"/>
-      <c r="AT5" s="170"/>
-      <c r="AU5" s="170"/>
-      <c r="AV5" s="170"/>
-      <c r="AW5" s="170"/>
-      <c r="AX5" s="170"/>
-      <c r="AY5" s="170"/>
-      <c r="AZ5" s="170"/>
-      <c r="BA5" s="170"/>
-      <c r="BB5" s="170"/>
-      <c r="BC5" s="170"/>
+      <c r="A5" s="116"/>
+      <c r="B5" s="116"/>
+      <c r="C5" s="116"/>
+      <c r="D5" s="116"/>
+      <c r="E5" s="116"/>
+      <c r="F5" s="116"/>
+      <c r="G5" s="116"/>
+      <c r="H5" s="116"/>
+      <c r="I5" s="116"/>
+      <c r="J5" s="116"/>
+      <c r="K5" s="116"/>
+      <c r="L5" s="116"/>
+      <c r="M5" s="116"/>
+      <c r="N5" s="116"/>
+      <c r="O5" s="116"/>
+      <c r="P5" s="116"/>
+      <c r="Q5" s="116"/>
+      <c r="R5" s="116"/>
+      <c r="S5" s="116"/>
+      <c r="T5" s="116"/>
+      <c r="U5" s="116"/>
+      <c r="V5" s="116"/>
+      <c r="W5" s="116"/>
+      <c r="X5" s="116"/>
+      <c r="Y5" s="116"/>
+      <c r="Z5" s="116"/>
+      <c r="AA5" s="116"/>
+      <c r="AB5" s="116"/>
+      <c r="AC5" s="116"/>
+      <c r="AD5" s="116"/>
+      <c r="AE5" s="116"/>
+      <c r="AF5" s="116"/>
+      <c r="AG5" s="116"/>
+      <c r="AH5" s="116"/>
+      <c r="AI5" s="116"/>
+      <c r="AJ5" s="116"/>
+      <c r="AK5" s="116"/>
+      <c r="AL5" s="116"/>
+      <c r="AM5" s="116"/>
+      <c r="AN5" s="116"/>
+      <c r="AO5" s="116"/>
+      <c r="AP5" s="116"/>
+      <c r="AQ5" s="116"/>
+      <c r="AR5" s="116"/>
+      <c r="AS5" s="116"/>
+      <c r="AT5" s="116"/>
+      <c r="AU5" s="116"/>
+      <c r="AV5" s="116"/>
+      <c r="AW5" s="116"/>
+      <c r="AX5" s="116"/>
+      <c r="AY5" s="116"/>
+      <c r="AZ5" s="116"/>
+      <c r="BA5" s="116"/>
+      <c r="BB5" s="116"/>
+      <c r="BC5" s="116"/>
       <c r="BD5" s="35" t="s">
         <v>99</v>
       </c>
@@ -4641,9 +4570,9 @@
       <c r="CJ5" s="35" t="s">
         <v>65</v>
       </c>
-      <c r="CK5" s="170"/>
-      <c r="CL5" s="170"/>
-      <c r="CM5" s="170"/>
+      <c r="CK5" s="116"/>
+      <c r="CL5" s="116"/>
+      <c r="CM5" s="116"/>
     </row>
     <row r="6" spans="1:175" x14ac:dyDescent="0.25">
       <c r="A6" s="36"/>
@@ -5222,14 +5151,62 @@
     </row>
   </sheetData>
   <mergeCells count="80">
-    <mergeCell ref="X3:X5"/>
-    <mergeCell ref="Y3:Y5"/>
-    <mergeCell ref="AL3:AL5"/>
-    <mergeCell ref="Z3:Z5"/>
-    <mergeCell ref="AA3:AA5"/>
-    <mergeCell ref="AB3:AB5"/>
-    <mergeCell ref="AC3:AC5"/>
-    <mergeCell ref="AD3:AD5"/>
+    <mergeCell ref="BM4:BO4"/>
+    <mergeCell ref="AM3:AM5"/>
+    <mergeCell ref="AN3:AN5"/>
+    <mergeCell ref="AO3:AO5"/>
+    <mergeCell ref="AP3:AP5"/>
+    <mergeCell ref="AT2:AT5"/>
+    <mergeCell ref="AU2:AU5"/>
+    <mergeCell ref="AV2:AV5"/>
+    <mergeCell ref="AW2:AW5"/>
+    <mergeCell ref="CE4:CG4"/>
+    <mergeCell ref="CH4:CJ4"/>
+    <mergeCell ref="AX2:AX5"/>
+    <mergeCell ref="AY2:AY5"/>
+    <mergeCell ref="AZ2:AZ5"/>
+    <mergeCell ref="BB3:BB5"/>
+    <mergeCell ref="BC3:BC5"/>
+    <mergeCell ref="BP4:BR4"/>
+    <mergeCell ref="BS4:BU4"/>
+    <mergeCell ref="BV4:BX4"/>
+    <mergeCell ref="BY4:CA4"/>
+    <mergeCell ref="CB4:CD4"/>
+    <mergeCell ref="BA2:BA5"/>
+    <mergeCell ref="BD4:BF4"/>
+    <mergeCell ref="BG4:BI4"/>
+    <mergeCell ref="BJ4:BL4"/>
+    <mergeCell ref="CK2:CK5"/>
+    <mergeCell ref="CL2:CL5"/>
+    <mergeCell ref="CM2:CM5"/>
+    <mergeCell ref="BE3:CJ3"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D1:O1"/>
+    <mergeCell ref="P1:S1"/>
+    <mergeCell ref="T1:AF1"/>
+    <mergeCell ref="AG1:AS1"/>
+    <mergeCell ref="AT1:AZ1"/>
+    <mergeCell ref="BA1:CM1"/>
+    <mergeCell ref="BB2:CJ2"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="C2:C5"/>
+    <mergeCell ref="D2:D5"/>
+    <mergeCell ref="E2:E5"/>
+    <mergeCell ref="F2:F5"/>
+    <mergeCell ref="G2:G5"/>
+    <mergeCell ref="H2:H5"/>
+    <mergeCell ref="I2:I5"/>
+    <mergeCell ref="J2:J5"/>
+    <mergeCell ref="K2:K5"/>
+    <mergeCell ref="L2:L5"/>
+    <mergeCell ref="M2:M5"/>
+    <mergeCell ref="N2:N5"/>
+    <mergeCell ref="O2:O5"/>
+    <mergeCell ref="P2:P5"/>
+    <mergeCell ref="Q2:Q5"/>
+    <mergeCell ref="R2:R5"/>
+    <mergeCell ref="S2:S5"/>
     <mergeCell ref="T2:T5"/>
     <mergeCell ref="U2:U5"/>
     <mergeCell ref="AQ2:AQ5"/>
@@ -5246,62 +5223,14 @@
     <mergeCell ref="AI3:AI5"/>
     <mergeCell ref="AJ3:AJ5"/>
     <mergeCell ref="AK3:AK5"/>
-    <mergeCell ref="O2:O5"/>
-    <mergeCell ref="P2:P5"/>
-    <mergeCell ref="Q2:Q5"/>
-    <mergeCell ref="R2:R5"/>
-    <mergeCell ref="S2:S5"/>
-    <mergeCell ref="J2:J5"/>
-    <mergeCell ref="K2:K5"/>
-    <mergeCell ref="L2:L5"/>
-    <mergeCell ref="M2:M5"/>
-    <mergeCell ref="N2:N5"/>
-    <mergeCell ref="E2:E5"/>
-    <mergeCell ref="F2:F5"/>
-    <mergeCell ref="G2:G5"/>
-    <mergeCell ref="H2:H5"/>
-    <mergeCell ref="I2:I5"/>
-    <mergeCell ref="CK2:CK5"/>
-    <mergeCell ref="CL2:CL5"/>
-    <mergeCell ref="CM2:CM5"/>
-    <mergeCell ref="BE3:CJ3"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="D1:O1"/>
-    <mergeCell ref="P1:S1"/>
-    <mergeCell ref="T1:AF1"/>
-    <mergeCell ref="AG1:AS1"/>
-    <mergeCell ref="AT1:AZ1"/>
-    <mergeCell ref="BA1:CM1"/>
-    <mergeCell ref="BB2:CJ2"/>
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="B2:B5"/>
-    <mergeCell ref="C2:C5"/>
-    <mergeCell ref="D2:D5"/>
-    <mergeCell ref="CE4:CG4"/>
-    <mergeCell ref="CH4:CJ4"/>
-    <mergeCell ref="AX2:AX5"/>
-    <mergeCell ref="AY2:AY5"/>
-    <mergeCell ref="AZ2:AZ5"/>
-    <mergeCell ref="BB3:BB5"/>
-    <mergeCell ref="BC3:BC5"/>
-    <mergeCell ref="BP4:BR4"/>
-    <mergeCell ref="BS4:BU4"/>
-    <mergeCell ref="BV4:BX4"/>
-    <mergeCell ref="BY4:CA4"/>
-    <mergeCell ref="CB4:CD4"/>
-    <mergeCell ref="BA2:BA5"/>
-    <mergeCell ref="BD4:BF4"/>
-    <mergeCell ref="BG4:BI4"/>
-    <mergeCell ref="BJ4:BL4"/>
-    <mergeCell ref="BM4:BO4"/>
-    <mergeCell ref="AM3:AM5"/>
-    <mergeCell ref="AN3:AN5"/>
-    <mergeCell ref="AO3:AO5"/>
-    <mergeCell ref="AP3:AP5"/>
-    <mergeCell ref="AT2:AT5"/>
-    <mergeCell ref="AU2:AU5"/>
-    <mergeCell ref="AV2:AV5"/>
-    <mergeCell ref="AW2:AW5"/>
+    <mergeCell ref="X3:X5"/>
+    <mergeCell ref="Y3:Y5"/>
+    <mergeCell ref="AL3:AL5"/>
+    <mergeCell ref="Z3:Z5"/>
+    <mergeCell ref="AA3:AA5"/>
+    <mergeCell ref="AB3:AB5"/>
+    <mergeCell ref="AC3:AC5"/>
+    <mergeCell ref="AD3:AD5"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="BB6:BB10" xr:uid="{00000000-0002-0000-0100-000000000000}">
@@ -5335,36 +5264,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="187" t="s">
+      <c r="A1" s="168" t="s">
         <v>100</v>
       </c>
-      <c r="B1" s="148"/>
-      <c r="C1" s="148"/>
-      <c r="D1" s="148"/>
-      <c r="E1" s="148"/>
-      <c r="F1" s="148"/>
-      <c r="G1" s="148"/>
-      <c r="H1" s="148"/>
-      <c r="I1" s="148"/>
-      <c r="J1" s="148"/>
-      <c r="K1" s="148"/>
-      <c r="L1" s="148"/>
+      <c r="B1" s="137"/>
+      <c r="C1" s="137"/>
+      <c r="D1" s="137"/>
+      <c r="E1" s="137"/>
+      <c r="F1" s="137"/>
+      <c r="G1" s="137"/>
+      <c r="H1" s="137"/>
+      <c r="I1" s="137"/>
+      <c r="J1" s="137"/>
+      <c r="K1" s="137"/>
+      <c r="L1" s="137"/>
     </row>
     <row r="3" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A3" s="188" t="s">
+      <c r="A3" s="165" t="s">
         <v>101</v>
       </c>
-      <c r="B3" s="148"/>
-      <c r="C3" s="148"/>
-      <c r="D3" s="148"/>
-      <c r="E3" s="148"/>
-      <c r="F3" s="148"/>
-      <c r="G3" s="148"/>
-      <c r="H3" s="148"/>
-      <c r="I3" s="148"/>
-      <c r="J3" s="148"/>
-      <c r="K3" s="148"/>
-      <c r="L3" s="148"/>
+      <c r="B3" s="137"/>
+      <c r="C3" s="137"/>
+      <c r="D3" s="137"/>
+      <c r="E3" s="137"/>
+      <c r="F3" s="137"/>
+      <c r="G3" s="137"/>
+      <c r="H3" s="137"/>
+      <c r="I3" s="137"/>
+      <c r="J3" s="137"/>
+      <c r="K3" s="137"/>
+      <c r="L3" s="137"/>
     </row>
     <row r="4" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A4" s="38" t="s">
@@ -5401,24 +5330,24 @@
       <c r="L5" s="32"/>
     </row>
     <row r="6" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A6" s="189" t="s">
+      <c r="A6" s="169" t="s">
         <v>105</v>
       </c>
-      <c r="B6" s="145"/>
-      <c r="C6" s="145"/>
-      <c r="D6" s="156"/>
-      <c r="E6" s="189" t="s">
+      <c r="B6" s="107"/>
+      <c r="C6" s="107"/>
+      <c r="D6" s="108"/>
+      <c r="E6" s="169" t="s">
         <v>106</v>
       </c>
-      <c r="F6" s="145"/>
-      <c r="G6" s="145"/>
-      <c r="H6" s="156"/>
-      <c r="I6" s="189" t="s">
+      <c r="F6" s="107"/>
+      <c r="G6" s="107"/>
+      <c r="H6" s="108"/>
+      <c r="I6" s="169" t="s">
         <v>107</v>
       </c>
-      <c r="J6" s="145"/>
-      <c r="K6" s="145"/>
-      <c r="L6" s="156"/>
+      <c r="J6" s="107"/>
+      <c r="K6" s="107"/>
+      <c r="L6" s="108"/>
     </row>
     <row r="7" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A7" s="38" t="s">
@@ -5613,19 +5542,19 @@
       <c r="D16" s="34"/>
     </row>
     <row r="17" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A17" s="188" t="s">
+      <c r="A17" s="165" t="s">
         <v>125</v>
       </c>
-      <c r="B17" s="148"/>
-      <c r="C17" s="148"/>
-      <c r="D17" s="148"/>
+      <c r="B17" s="137"/>
+      <c r="C17" s="137"/>
+      <c r="D17" s="137"/>
       <c r="E17" s="46"/>
-      <c r="F17" s="190" t="s">
+      <c r="F17" s="166" t="s">
         <v>126</v>
       </c>
-      <c r="G17" s="191"/>
-      <c r="H17" s="191"/>
-      <c r="I17" s="191"/>
+      <c r="G17" s="167"/>
+      <c r="H17" s="167"/>
+      <c r="I17" s="167"/>
     </row>
     <row r="18" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A18" s="47" t="s">
@@ -5710,19 +5639,19 @@
       <c r="D24" s="65"/>
     </row>
     <row r="25" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A25" s="188" t="s">
+      <c r="A25" s="165" t="s">
         <v>135</v>
       </c>
-      <c r="B25" s="148"/>
-      <c r="C25" s="148"/>
-      <c r="D25" s="148"/>
+      <c r="B25" s="137"/>
+      <c r="C25" s="137"/>
+      <c r="D25" s="137"/>
       <c r="E25" s="66"/>
-      <c r="F25" s="188" t="s">
+      <c r="F25" s="165" t="s">
         <v>136</v>
       </c>
-      <c r="G25" s="148"/>
-      <c r="H25" s="148"/>
-      <c r="I25" s="148"/>
+      <c r="G25" s="137"/>
+      <c r="H25" s="137"/>
+      <c r="I25" s="137"/>
     </row>
     <row r="26" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A26" s="38" t="s">
@@ -6055,16 +5984,16 @@
       <c r="D53" s="32"/>
     </row>
     <row r="55" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A55" s="188" t="s">
+      <c r="A55" s="165" t="s">
         <v>172</v>
       </c>
-      <c r="B55" s="148"/>
-      <c r="C55" s="148"/>
-      <c r="D55" s="148"/>
-      <c r="E55" s="148"/>
-      <c r="F55" s="148"/>
-      <c r="G55" s="148"/>
-      <c r="H55" s="148"/>
+      <c r="B55" s="137"/>
+      <c r="C55" s="137"/>
+      <c r="D55" s="137"/>
+      <c r="E55" s="137"/>
+      <c r="F55" s="137"/>
+      <c r="G55" s="137"/>
+      <c r="H55" s="137"/>
     </row>
     <row r="56" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A56" s="38" t="s">
@@ -6103,18 +6032,18 @@
       <c r="H59" s="32"/>
     </row>
     <row r="60" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A60" s="192" t="s">
+      <c r="A60" s="164" t="s">
         <v>174</v>
       </c>
-      <c r="B60" s="151"/>
-      <c r="C60" s="151"/>
-      <c r="D60" s="152"/>
-      <c r="E60" s="192" t="s">
+      <c r="B60" s="112"/>
+      <c r="C60" s="112"/>
+      <c r="D60" s="113"/>
+      <c r="E60" s="164" t="s">
         <v>175</v>
       </c>
-      <c r="F60" s="151"/>
-      <c r="G60" s="151"/>
-      <c r="H60" s="152"/>
+      <c r="F60" s="112"/>
+      <c r="G60" s="112"/>
+      <c r="H60" s="113"/>
     </row>
     <row r="61" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A61" s="44" t="s">
@@ -6160,16 +6089,16 @@
       <c r="H62" s="32"/>
     </row>
     <row r="63" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A63" s="192" t="s">
+      <c r="A63" s="164" t="s">
         <v>186</v>
       </c>
-      <c r="B63" s="151"/>
-      <c r="C63" s="151"/>
-      <c r="D63" s="151"/>
-      <c r="E63" s="151"/>
-      <c r="F63" s="151"/>
-      <c r="G63" s="151"/>
-      <c r="H63" s="152"/>
+      <c r="B63" s="112"/>
+      <c r="C63" s="112"/>
+      <c r="D63" s="112"/>
+      <c r="E63" s="112"/>
+      <c r="F63" s="112"/>
+      <c r="G63" s="112"/>
+      <c r="H63" s="113"/>
     </row>
     <row r="64" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A64" s="38" t="s">
@@ -6232,18 +6161,18 @@
       <c r="H67" s="7"/>
     </row>
     <row r="68" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A68" s="192" t="s">
+      <c r="A68" s="164" t="s">
         <v>197</v>
       </c>
-      <c r="B68" s="151"/>
-      <c r="C68" s="151"/>
-      <c r="D68" s="152"/>
-      <c r="E68" s="192" t="s">
+      <c r="B68" s="112"/>
+      <c r="C68" s="112"/>
+      <c r="D68" s="113"/>
+      <c r="E68" s="164" t="s">
         <v>198</v>
       </c>
-      <c r="F68" s="151"/>
-      <c r="G68" s="151"/>
-      <c r="H68" s="152"/>
+      <c r="F68" s="112"/>
+      <c r="G68" s="112"/>
+      <c r="H68" s="113"/>
     </row>
     <row r="69" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A69" s="47" t="s">
@@ -6336,18 +6265,18 @@
       <c r="H74" s="32"/>
     </row>
     <row r="75" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A75" s="192" t="s">
+      <c r="A75" s="164" t="s">
         <v>202</v>
       </c>
-      <c r="B75" s="151"/>
-      <c r="C75" s="151"/>
-      <c r="D75" s="152"/>
-      <c r="E75" s="192" t="s">
+      <c r="B75" s="112"/>
+      <c r="C75" s="112"/>
+      <c r="D75" s="113"/>
+      <c r="E75" s="164" t="s">
         <v>203</v>
       </c>
-      <c r="F75" s="151"/>
-      <c r="G75" s="151"/>
-      <c r="H75" s="152"/>
+      <c r="F75" s="112"/>
+      <c r="G75" s="112"/>
+      <c r="H75" s="113"/>
     </row>
     <row r="76" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A76" s="47" t="s">
@@ -6440,18 +6369,18 @@
       <c r="H81" s="32"/>
     </row>
     <row r="82" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A82" s="192" t="s">
+      <c r="A82" s="164" t="s">
         <v>204</v>
       </c>
-      <c r="B82" s="151"/>
-      <c r="C82" s="151"/>
-      <c r="D82" s="152"/>
-      <c r="E82" s="192" t="s">
+      <c r="B82" s="112"/>
+      <c r="C82" s="112"/>
+      <c r="D82" s="113"/>
+      <c r="E82" s="164" t="s">
         <v>205</v>
       </c>
-      <c r="F82" s="151"/>
-      <c r="G82" s="151"/>
-      <c r="H82" s="152"/>
+      <c r="F82" s="112"/>
+      <c r="G82" s="112"/>
+      <c r="H82" s="113"/>
     </row>
     <row r="83" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A83" s="47" t="s">
@@ -6629,6 +6558,16 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A3:L3"/>
+    <mergeCell ref="A6:D6"/>
+    <mergeCell ref="E6:H6"/>
+    <mergeCell ref="I6:L6"/>
+    <mergeCell ref="A17:D17"/>
+    <mergeCell ref="F17:I17"/>
+    <mergeCell ref="A68:D68"/>
+    <mergeCell ref="A75:D75"/>
+    <mergeCell ref="E75:H75"/>
     <mergeCell ref="A82:D82"/>
     <mergeCell ref="E82:H82"/>
     <mergeCell ref="A25:D25"/>
@@ -6638,16 +6577,6 @@
     <mergeCell ref="E60:H60"/>
     <mergeCell ref="A63:H63"/>
     <mergeCell ref="E68:H68"/>
-    <mergeCell ref="A17:D17"/>
-    <mergeCell ref="F17:I17"/>
-    <mergeCell ref="A68:D68"/>
-    <mergeCell ref="A75:D75"/>
-    <mergeCell ref="E75:H75"/>
-    <mergeCell ref="A1:L1"/>
-    <mergeCell ref="A3:L3"/>
-    <mergeCell ref="A6:D6"/>
-    <mergeCell ref="E6:H6"/>
-    <mergeCell ref="I6:L6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Finished read excel data
</commit_message>
<xml_diff>
--- a/attachments/Input Merchant Acquisition (1).xlsx
+++ b/attachments/Input Merchant Acquisition (1).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kuliah\Asisten\Icstar Indonesia Lomba\MerchantAcquisition\attachments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB1060B7-87CA-439C-8676-6E6655174921}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C461624B-450F-4BD5-BE77-83E467A1DE38}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="648" uniqueCount="319">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="650" uniqueCount="321">
   <si>
     <t>Sales Chanel</t>
   </si>
@@ -987,6 +987,12 @@
   </si>
   <si>
     <t>parent merchant</t>
+  </si>
+  <si>
+    <t>asdasd</t>
+  </si>
+  <si>
+    <t>Sarang Lebah</t>
   </si>
 </sst>
 </file>
@@ -1905,133 +1911,146 @@
     <xf numFmtId="49" fontId="8" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
@@ -2039,15 +2058,18 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="49" fontId="8" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -2056,173 +2078,157 @@
     <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2445,8 +2451,8 @@
   </sheetPr>
   <dimension ref="A1:W132"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
-      <selection activeCell="A128" sqref="A128:D128"/>
+    <sheetView tabSelected="1" topLeftCell="F62" workbookViewId="0">
+      <selection activeCell="I66" sqref="I66:L66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2467,10 +2473,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1" s="174" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="162"/>
+      <c r="A1" s="183" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="158"/>
     </row>
     <row r="2" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -2497,12 +2503,12 @@
       </c>
     </row>
     <row r="6" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A6" s="175" t="s">
+      <c r="A6" s="151" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="155"/>
-      <c r="C6" s="155"/>
-      <c r="D6" s="166"/>
+      <c r="B6" s="152"/>
+      <c r="C6" s="152"/>
+      <c r="D6" s="153"/>
     </row>
     <row r="7" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
@@ -2679,38 +2685,38 @@
       <c r="D20" s="79"/>
     </row>
     <row r="22" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A22" s="176" t="s">
+      <c r="A22" s="184" t="s">
         <v>26</v>
       </c>
-      <c r="B22" s="177"/>
-      <c r="C22" s="177"/>
-      <c r="D22" s="177"/>
-      <c r="E22" s="177"/>
-      <c r="F22" s="177"/>
-      <c r="G22" s="177"/>
-      <c r="H22" s="177"/>
-      <c r="I22" s="178"/>
+      <c r="B22" s="185"/>
+      <c r="C22" s="185"/>
+      <c r="D22" s="185"/>
+      <c r="E22" s="185"/>
+      <c r="F22" s="185"/>
+      <c r="G22" s="185"/>
+      <c r="H22" s="185"/>
+      <c r="I22" s="186"/>
       <c r="J22" s="16"/>
       <c r="K22" s="16"/>
       <c r="L22" s="16"/>
       <c r="M22" s="16"/>
     </row>
     <row r="23" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A23" s="179" t="s">
+      <c r="A23" s="187" t="s">
         <v>27</v>
       </c>
-      <c r="B23" s="177"/>
-      <c r="C23" s="177"/>
-      <c r="D23" s="179" t="s">
+      <c r="B23" s="185"/>
+      <c r="C23" s="185"/>
+      <c r="D23" s="187" t="s">
         <v>28</v>
       </c>
-      <c r="E23" s="177"/>
-      <c r="F23" s="177"/>
-      <c r="G23" s="179" t="s">
+      <c r="E23" s="185"/>
+      <c r="F23" s="185"/>
+      <c r="G23" s="187" t="s">
         <v>29</v>
       </c>
-      <c r="H23" s="177"/>
-      <c r="I23" s="178"/>
+      <c r="H23" s="185"/>
+      <c r="I23" s="186"/>
       <c r="L23" s="16"/>
       <c r="M23" s="16"/>
     </row>
@@ -2718,82 +2724,84 @@
       <c r="A24" s="105" t="s">
         <v>30</v>
       </c>
-      <c r="B24" s="173" t="s">
+      <c r="B24" s="182" t="s">
         <v>239</v>
       </c>
-      <c r="C24" s="172"/>
+      <c r="C24" s="181"/>
       <c r="D24" s="105" t="s">
         <v>30</v>
       </c>
-      <c r="E24" s="171" t="s">
+      <c r="E24" s="180" t="s">
         <v>282</v>
       </c>
-      <c r="F24" s="172"/>
+      <c r="F24" s="181"/>
       <c r="G24" s="105" t="s">
         <v>30</v>
       </c>
-      <c r="H24" s="173"/>
-      <c r="I24" s="172"/>
+      <c r="H24" s="182" t="s">
+        <v>319</v>
+      </c>
+      <c r="I24" s="181"/>
     </row>
     <row r="25" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A25" s="106" t="s">
         <v>6</v>
       </c>
-      <c r="B25" s="180" t="s">
+      <c r="B25" s="172" t="s">
         <v>240</v>
       </c>
-      <c r="C25" s="181"/>
+      <c r="C25" s="173"/>
       <c r="D25" s="106" t="s">
         <v>6</v>
       </c>
-      <c r="E25" s="180"/>
-      <c r="F25" s="181"/>
+      <c r="E25" s="172"/>
+      <c r="F25" s="173"/>
       <c r="G25" s="106" t="s">
         <v>6</v>
       </c>
-      <c r="H25" s="180"/>
-      <c r="I25" s="181"/>
+      <c r="H25" s="172"/>
+      <c r="I25" s="173"/>
     </row>
     <row r="26" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A26" s="106" t="s">
         <v>31</v>
       </c>
-      <c r="B26" s="183" t="s">
+      <c r="B26" s="178" t="s">
         <v>246</v>
       </c>
-      <c r="C26" s="184"/>
+      <c r="C26" s="179"/>
       <c r="D26" s="106" t="s">
         <v>31</v>
       </c>
-      <c r="E26" s="180"/>
-      <c r="F26" s="181"/>
+      <c r="E26" s="172"/>
+      <c r="F26" s="173"/>
       <c r="G26" s="106" t="s">
         <v>31</v>
       </c>
-      <c r="H26" s="180"/>
-      <c r="I26" s="181"/>
+      <c r="H26" s="172"/>
+      <c r="I26" s="173"/>
     </row>
     <row r="27" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A27" s="106" t="s">
         <v>8</v>
       </c>
-      <c r="B27" s="183" t="s">
+      <c r="B27" s="178" t="s">
         <v>245</v>
       </c>
-      <c r="C27" s="184"/>
+      <c r="C27" s="179"/>
       <c r="D27" s="106" t="s">
         <v>8</v>
       </c>
-      <c r="E27" s="180"/>
-      <c r="F27" s="181"/>
+      <c r="E27" s="172"/>
+      <c r="F27" s="173"/>
       <c r="G27" s="106" t="s">
         <v>8</v>
       </c>
-      <c r="H27" s="180"/>
-      <c r="I27" s="181"/>
+      <c r="H27" s="172"/>
+      <c r="I27" s="173"/>
     </row>
     <row r="28" spans="1:13" ht="35.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="185" t="s">
+      <c r="A28" s="159" t="s">
         <v>32</v>
       </c>
       <c r="B28" s="107" t="s">
@@ -2802,14 +2810,14 @@
       <c r="C28" s="108" t="s">
         <v>241</v>
       </c>
-      <c r="D28" s="185" t="s">
+      <c r="D28" s="159" t="s">
         <v>32</v>
       </c>
       <c r="E28" s="107" t="s">
         <v>33</v>
       </c>
       <c r="F28" s="109"/>
-      <c r="G28" s="185" t="s">
+      <c r="G28" s="159" t="s">
         <v>32</v>
       </c>
       <c r="H28" s="107" t="s">
@@ -2818,38 +2826,38 @@
       <c r="I28" s="109"/>
     </row>
     <row r="29" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A29" s="186"/>
+      <c r="A29" s="160"/>
       <c r="B29" s="110" t="s">
         <v>34</v>
       </c>
       <c r="C29" s="104" t="s">
         <v>242</v>
       </c>
-      <c r="D29" s="186"/>
+      <c r="D29" s="160"/>
       <c r="E29" s="110" t="s">
         <v>34</v>
       </c>
       <c r="F29" s="111"/>
-      <c r="G29" s="186"/>
+      <c r="G29" s="160"/>
       <c r="H29" s="110" t="s">
         <v>34</v>
       </c>
       <c r="I29" s="111"/>
     </row>
     <row r="30" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A30" s="186"/>
+      <c r="A30" s="160"/>
       <c r="B30" s="110" t="s">
         <v>35</v>
       </c>
       <c r="C30" s="116" t="s">
         <v>281</v>
       </c>
-      <c r="D30" s="186"/>
+      <c r="D30" s="160"/>
       <c r="E30" s="110" t="s">
         <v>35</v>
       </c>
       <c r="F30" s="111"/>
-      <c r="G30" s="186"/>
+      <c r="G30" s="160"/>
       <c r="H30" s="110" t="s">
         <v>35</v>
       </c>
@@ -2857,19 +2865,19 @@
       <c r="M30" s="18"/>
     </row>
     <row r="31" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A31" s="186"/>
+      <c r="A31" s="160"/>
       <c r="B31" s="110" t="s">
         <v>36</v>
       </c>
       <c r="C31" s="104" t="s">
         <v>243</v>
       </c>
-      <c r="D31" s="186"/>
+      <c r="D31" s="160"/>
       <c r="E31" s="110" t="s">
         <v>36</v>
       </c>
       <c r="F31" s="111"/>
-      <c r="G31" s="186"/>
+      <c r="G31" s="160"/>
       <c r="H31" s="110" t="s">
         <v>36</v>
       </c>
@@ -2877,19 +2885,19 @@
       <c r="M31" s="18"/>
     </row>
     <row r="32" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A32" s="186"/>
+      <c r="A32" s="160"/>
       <c r="B32" s="110" t="s">
         <v>37</v>
       </c>
       <c r="C32" s="104">
         <v>123123</v>
       </c>
-      <c r="D32" s="186"/>
+      <c r="D32" s="160"/>
       <c r="E32" s="110" t="s">
         <v>37</v>
       </c>
       <c r="F32" s="111"/>
-      <c r="G32" s="186"/>
+      <c r="G32" s="160"/>
       <c r="H32" s="110" t="s">
         <v>37</v>
       </c>
@@ -2897,19 +2905,19 @@
       <c r="M32" s="18"/>
     </row>
     <row r="33" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A33" s="186"/>
+      <c r="A33" s="160"/>
       <c r="B33" s="110" t="s">
         <v>38</v>
       </c>
       <c r="C33" s="104" t="s">
         <v>244</v>
       </c>
-      <c r="D33" s="186"/>
+      <c r="D33" s="160"/>
       <c r="E33" s="110" t="s">
         <v>38</v>
       </c>
       <c r="F33" s="111"/>
-      <c r="G33" s="186"/>
+      <c r="G33" s="160"/>
       <c r="H33" s="110" t="s">
         <v>38</v>
       </c>
@@ -2917,19 +2925,19 @@
       <c r="M33" s="18"/>
     </row>
     <row r="34" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A34" s="186"/>
+      <c r="A34" s="160"/>
       <c r="B34" s="110" t="s">
         <v>39</v>
       </c>
       <c r="C34" s="104">
         <v>111</v>
       </c>
-      <c r="D34" s="186"/>
+      <c r="D34" s="160"/>
       <c r="E34" s="110" t="s">
         <v>39</v>
       </c>
       <c r="F34" s="111"/>
-      <c r="G34" s="186"/>
+      <c r="G34" s="160"/>
       <c r="H34" s="110" t="s">
         <v>39</v>
       </c>
@@ -2937,19 +2945,19 @@
       <c r="M34" s="18"/>
     </row>
     <row r="35" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A35" s="187"/>
+      <c r="A35" s="161"/>
       <c r="B35" s="112" t="s">
         <v>40</v>
       </c>
       <c r="C35" s="113">
         <v>32231</v>
       </c>
-      <c r="D35" s="187"/>
+      <c r="D35" s="161"/>
       <c r="E35" s="112" t="s">
         <v>40</v>
       </c>
       <c r="F35" s="114"/>
-      <c r="G35" s="187"/>
+      <c r="G35" s="161"/>
       <c r="H35" s="112" t="s">
         <v>40</v>
       </c>
@@ -2960,27 +2968,27 @@
       <c r="A36" s="115" t="s">
         <v>41</v>
       </c>
-      <c r="B36" s="197" t="s">
+      <c r="B36" s="171" t="s">
         <v>280</v>
       </c>
-      <c r="C36" s="198"/>
+      <c r="C36" s="150"/>
       <c r="D36" s="115" t="s">
         <v>41</v>
       </c>
-      <c r="E36" s="199"/>
-      <c r="F36" s="198"/>
+      <c r="E36" s="149"/>
+      <c r="F36" s="150"/>
       <c r="G36" s="115" t="s">
         <v>41</v>
       </c>
-      <c r="H36" s="199"/>
-      <c r="I36" s="198"/>
+      <c r="H36" s="149"/>
+      <c r="I36" s="150"/>
     </row>
     <row r="38" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A38" s="175" t="s">
+      <c r="A38" s="151" t="s">
         <v>42</v>
       </c>
-      <c r="B38" s="155"/>
-      <c r="C38" s="166"/>
+      <c r="B38" s="152"/>
+      <c r="C38" s="153"/>
     </row>
     <row r="39" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A39" s="9" t="s">
@@ -2995,13 +3003,13 @@
       <c r="A40" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="B40" s="157" t="s">
+      <c r="B40" s="154" t="s">
         <v>219</v>
       </c>
-      <c r="C40" s="159"/>
+      <c r="C40" s="155"/>
     </row>
     <row r="41" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A41" s="188" t="s">
+      <c r="A41" s="162" t="s">
         <v>32</v>
       </c>
       <c r="B41" s="9" t="s">
@@ -3012,7 +3020,7 @@
       </c>
     </row>
     <row r="42" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A42" s="189"/>
+      <c r="A42" s="163"/>
       <c r="B42" s="7" t="s">
         <v>34</v>
       </c>
@@ -3021,7 +3029,7 @@
       </c>
     </row>
     <row r="43" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A43" s="189"/>
+      <c r="A43" s="163"/>
       <c r="B43" s="7" t="s">
         <v>35</v>
       </c>
@@ -3030,7 +3038,7 @@
       </c>
     </row>
     <row r="44" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A44" s="189"/>
+      <c r="A44" s="163"/>
       <c r="B44" s="7" t="s">
         <v>36</v>
       </c>
@@ -3039,7 +3047,7 @@
       </c>
     </row>
     <row r="45" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A45" s="189"/>
+      <c r="A45" s="163"/>
       <c r="B45" s="7" t="s">
         <v>37</v>
       </c>
@@ -3048,7 +3056,7 @@
       </c>
     </row>
     <row r="46" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A46" s="189"/>
+      <c r="A46" s="163"/>
       <c r="B46" s="7" t="s">
         <v>38</v>
       </c>
@@ -3057,7 +3065,7 @@
       </c>
     </row>
     <row r="47" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A47" s="189"/>
+      <c r="A47" s="163"/>
       <c r="B47" s="7" t="s">
         <v>39</v>
       </c>
@@ -3066,7 +3074,7 @@
       </c>
     </row>
     <row r="48" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A48" s="190"/>
+      <c r="A48" s="164"/>
       <c r="B48" s="7" t="s">
         <v>40</v>
       </c>
@@ -3078,34 +3086,34 @@
       <c r="A49" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="B49" s="191">
+      <c r="B49" s="165">
         <v>23586598</v>
       </c>
-      <c r="C49" s="192"/>
+      <c r="C49" s="166"/>
     </row>
     <row r="50" spans="1:18" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A50" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="B50" s="193">
+      <c r="B50" s="167">
         <v>8123456789</v>
       </c>
-      <c r="C50" s="194"/>
+      <c r="C50" s="168"/>
     </row>
     <row r="51" spans="1:18" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A51" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="B51" s="195" t="s">
+      <c r="B51" s="169" t="s">
         <v>225</v>
       </c>
-      <c r="C51" s="196"/>
+      <c r="C51" s="170"/>
     </row>
     <row r="53" spans="1:18" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A53" s="175" t="s">
+      <c r="A53" s="151" t="s">
         <v>48</v>
       </c>
-      <c r="B53" s="166"/>
+      <c r="B53" s="153"/>
     </row>
     <row r="54" spans="1:18" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A54" s="9" t="s">
@@ -3162,146 +3170,148 @@
       <c r="B60" s="89"/>
     </row>
     <row r="62" spans="1:18" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A62" s="160" t="s">
+      <c r="A62" s="191" t="s">
         <v>55</v>
       </c>
-      <c r="B62" s="161"/>
-      <c r="C62" s="161"/>
-      <c r="D62" s="161"/>
-      <c r="E62" s="161"/>
-      <c r="F62" s="161"/>
-      <c r="G62" s="161"/>
-      <c r="H62" s="161"/>
-      <c r="I62" s="161"/>
-      <c r="J62" s="161"/>
-      <c r="K62" s="161"/>
-      <c r="L62" s="161"/>
-      <c r="M62" s="161"/>
-      <c r="N62" s="161"/>
-      <c r="O62" s="161"/>
-      <c r="P62" s="161"/>
-      <c r="Q62" s="161"/>
-      <c r="R62" s="162"/>
+      <c r="B62" s="157"/>
+      <c r="C62" s="157"/>
+      <c r="D62" s="157"/>
+      <c r="E62" s="157"/>
+      <c r="F62" s="157"/>
+      <c r="G62" s="157"/>
+      <c r="H62" s="157"/>
+      <c r="I62" s="157"/>
+      <c r="J62" s="157"/>
+      <c r="K62" s="157"/>
+      <c r="L62" s="157"/>
+      <c r="M62" s="157"/>
+      <c r="N62" s="157"/>
+      <c r="O62" s="157"/>
+      <c r="P62" s="157"/>
+      <c r="Q62" s="157"/>
+      <c r="R62" s="158"/>
     </row>
     <row r="63" spans="1:18" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A63" s="163" t="s">
+      <c r="A63" s="192" t="s">
         <v>56</v>
       </c>
-      <c r="B63" s="161"/>
-      <c r="C63" s="161"/>
-      <c r="D63" s="161"/>
-      <c r="E63" s="161"/>
-      <c r="F63" s="162"/>
-      <c r="G63" s="163" t="s">
+      <c r="B63" s="157"/>
+      <c r="C63" s="157"/>
+      <c r="D63" s="157"/>
+      <c r="E63" s="157"/>
+      <c r="F63" s="158"/>
+      <c r="G63" s="192" t="s">
         <v>57</v>
       </c>
-      <c r="H63" s="161"/>
-      <c r="I63" s="161"/>
-      <c r="J63" s="161"/>
-      <c r="K63" s="161"/>
-      <c r="L63" s="161"/>
-      <c r="M63" s="163" t="s">
+      <c r="H63" s="157"/>
+      <c r="I63" s="157"/>
+      <c r="J63" s="157"/>
+      <c r="K63" s="157"/>
+      <c r="L63" s="157"/>
+      <c r="M63" s="192" t="s">
         <v>58</v>
       </c>
-      <c r="N63" s="161"/>
-      <c r="O63" s="161"/>
-      <c r="P63" s="161"/>
-      <c r="Q63" s="161"/>
-      <c r="R63" s="162"/>
+      <c r="N63" s="157"/>
+      <c r="O63" s="157"/>
+      <c r="P63" s="157"/>
+      <c r="Q63" s="157"/>
+      <c r="R63" s="158"/>
     </row>
     <row r="64" spans="1:18" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A64" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B64" s="164" t="s">
+      <c r="B64" s="156" t="s">
         <v>234</v>
       </c>
-      <c r="C64" s="161"/>
-      <c r="D64" s="161"/>
-      <c r="E64" s="161"/>
-      <c r="F64" s="162"/>
+      <c r="C64" s="157"/>
+      <c r="D64" s="157"/>
+      <c r="E64" s="157"/>
+      <c r="F64" s="158"/>
       <c r="G64" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="H64" s="164"/>
-      <c r="I64" s="161"/>
-      <c r="J64" s="161"/>
-      <c r="K64" s="161"/>
-      <c r="L64" s="162"/>
+      <c r="H64" s="156" t="s">
+        <v>320</v>
+      </c>
+      <c r="I64" s="157"/>
+      <c r="J64" s="157"/>
+      <c r="K64" s="157"/>
+      <c r="L64" s="158"/>
       <c r="M64" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="N64" s="164"/>
-      <c r="O64" s="161"/>
-      <c r="P64" s="161"/>
-      <c r="Q64" s="161"/>
-      <c r="R64" s="162"/>
+      <c r="N64" s="156"/>
+      <c r="O64" s="157"/>
+      <c r="P64" s="157"/>
+      <c r="Q64" s="157"/>
+      <c r="R64" s="158"/>
     </row>
     <row r="65" spans="1:18" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A65" s="182" t="s">
+      <c r="A65" s="174" t="s">
         <v>59</v>
       </c>
       <c r="B65" s="23" t="s">
         <v>60</v>
       </c>
-      <c r="C65" s="154" t="s">
+      <c r="C65" s="188" t="s">
         <v>264</v>
       </c>
-      <c r="D65" s="155"/>
-      <c r="E65" s="155"/>
-      <c r="F65" s="155"/>
-      <c r="G65" s="182" t="s">
+      <c r="D65" s="152"/>
+      <c r="E65" s="152"/>
+      <c r="F65" s="152"/>
+      <c r="G65" s="174" t="s">
         <v>59</v>
       </c>
       <c r="H65" s="23" t="s">
         <v>60</v>
       </c>
-      <c r="I65" s="165"/>
-      <c r="J65" s="155"/>
-      <c r="K65" s="155"/>
-      <c r="L65" s="166"/>
-      <c r="M65" s="167" t="s">
+      <c r="I65" s="193"/>
+      <c r="J65" s="152"/>
+      <c r="K65" s="152"/>
+      <c r="L65" s="153"/>
+      <c r="M65" s="194" t="s">
         <v>59</v>
       </c>
       <c r="N65" s="23" t="s">
         <v>60</v>
       </c>
-      <c r="O65" s="165"/>
-      <c r="P65" s="155"/>
-      <c r="Q65" s="155"/>
-      <c r="R65" s="166"/>
+      <c r="O65" s="193"/>
+      <c r="P65" s="152"/>
+      <c r="Q65" s="152"/>
+      <c r="R65" s="153"/>
     </row>
     <row r="66" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="168"/>
+      <c r="A66" s="175"/>
       <c r="B66" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="C66" s="156">
+      <c r="C66" s="189">
         <v>12</v>
       </c>
-      <c r="D66" s="156"/>
-      <c r="E66" s="156"/>
-      <c r="F66" s="156"/>
-      <c r="G66" s="168"/>
+      <c r="D66" s="189"/>
+      <c r="E66" s="189"/>
+      <c r="F66" s="189"/>
+      <c r="G66" s="175"/>
       <c r="H66" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="I66" s="157"/>
-      <c r="J66" s="158"/>
-      <c r="K66" s="158"/>
-      <c r="L66" s="159"/>
-      <c r="M66" s="168"/>
+      <c r="I66" s="154"/>
+      <c r="J66" s="190"/>
+      <c r="K66" s="190"/>
+      <c r="L66" s="155"/>
+      <c r="M66" s="175"/>
       <c r="N66" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="O66" s="157"/>
-      <c r="P66" s="158"/>
-      <c r="Q66" s="158"/>
-      <c r="R66" s="159"/>
+      <c r="O66" s="154"/>
+      <c r="P66" s="190"/>
+      <c r="Q66" s="190"/>
+      <c r="R66" s="155"/>
     </row>
     <row r="67" spans="1:18" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A67" s="168"/>
-      <c r="B67" s="169" t="s">
+      <c r="A67" s="175"/>
+      <c r="B67" s="176" t="s">
         <v>62</v>
       </c>
       <c r="C67" s="26" t="s">
@@ -3316,8 +3326,8 @@
       <c r="F67" s="26" t="s">
         <v>65</v>
       </c>
-      <c r="G67" s="168"/>
-      <c r="H67" s="169" t="s">
+      <c r="G67" s="175"/>
+      <c r="H67" s="176" t="s">
         <v>62</v>
       </c>
       <c r="I67" s="26" t="s">
@@ -3332,8 +3342,8 @@
       <c r="L67" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="M67" s="168"/>
-      <c r="N67" s="169" t="s">
+      <c r="M67" s="175"/>
+      <c r="N67" s="176" t="s">
         <v>62</v>
       </c>
       <c r="O67" s="26" t="s">
@@ -3350,8 +3360,8 @@
       </c>
     </row>
     <row r="68" spans="1:18" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A68" s="168"/>
-      <c r="B68" s="159"/>
+      <c r="A68" s="175"/>
+      <c r="B68" s="155"/>
       <c r="C68" s="25" t="s">
         <v>66</v>
       </c>
@@ -3364,8 +3374,8 @@
       <c r="F68" t="s">
         <v>233</v>
       </c>
-      <c r="G68" s="168"/>
-      <c r="H68" s="159"/>
+      <c r="G68" s="175"/>
+      <c r="H68" s="155"/>
       <c r="I68" s="25" t="s">
         <v>67</v>
       </c>
@@ -3374,8 +3384,8 @@
       </c>
       <c r="K68" s="2"/>
       <c r="L68" s="2"/>
-      <c r="M68" s="168"/>
-      <c r="N68" s="159"/>
+      <c r="M68" s="175"/>
+      <c r="N68" s="155"/>
       <c r="O68" s="25" t="s">
         <v>67</v>
       </c>
@@ -3386,8 +3396,8 @@
       <c r="R68" s="2"/>
     </row>
     <row r="69" spans="1:18" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A69" s="168"/>
-      <c r="B69" s="159"/>
+      <c r="A69" s="175"/>
+      <c r="B69" s="155"/>
       <c r="C69" s="25" t="s">
         <v>68</v>
       </c>
@@ -3397,8 +3407,8 @@
       <c r="E69" s="2">
         <v>2231</v>
       </c>
-      <c r="G69" s="168"/>
-      <c r="H69" s="159"/>
+      <c r="G69" s="175"/>
+      <c r="H69" s="155"/>
       <c r="I69" s="25" t="s">
         <v>69</v>
       </c>
@@ -3407,8 +3417,8 @@
       </c>
       <c r="K69" s="2"/>
       <c r="L69" s="2"/>
-      <c r="M69" s="168"/>
-      <c r="N69" s="159"/>
+      <c r="M69" s="175"/>
+      <c r="N69" s="155"/>
       <c r="O69" s="25" t="s">
         <v>69</v>
       </c>
@@ -3419,8 +3429,8 @@
       <c r="R69" s="2"/>
     </row>
     <row r="70" spans="1:18" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A70" s="168"/>
-      <c r="B70" s="159"/>
+      <c r="A70" s="175"/>
+      <c r="B70" s="155"/>
       <c r="C70" s="25" t="s">
         <v>70</v>
       </c>
@@ -3428,8 +3438,8 @@
         <v>0</v>
       </c>
       <c r="E70" s="2"/>
-      <c r="G70" s="168"/>
-      <c r="H70" s="159"/>
+      <c r="G70" s="175"/>
+      <c r="H70" s="155"/>
       <c r="I70" s="25" t="s">
         <v>70</v>
       </c>
@@ -3438,8 +3448,8 @@
       </c>
       <c r="K70" s="2"/>
       <c r="L70" s="2"/>
-      <c r="M70" s="168"/>
-      <c r="N70" s="159"/>
+      <c r="M70" s="175"/>
+      <c r="N70" s="155"/>
       <c r="O70" s="25" t="s">
         <v>70</v>
       </c>
@@ -3450,8 +3460,8 @@
       <c r="R70" s="2"/>
     </row>
     <row r="71" spans="1:18" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A71" s="168"/>
-      <c r="B71" s="159"/>
+      <c r="A71" s="175"/>
+      <c r="B71" s="155"/>
       <c r="C71" s="25" t="s">
         <v>71</v>
       </c>
@@ -3459,8 +3469,8 @@
         <v>0</v>
       </c>
       <c r="E71" s="2"/>
-      <c r="G71" s="168"/>
-      <c r="H71" s="159"/>
+      <c r="G71" s="175"/>
+      <c r="H71" s="155"/>
       <c r="I71" s="25" t="s">
         <v>71</v>
       </c>
@@ -3469,8 +3479,8 @@
       </c>
       <c r="K71" s="2"/>
       <c r="L71" s="2"/>
-      <c r="M71" s="168"/>
-      <c r="N71" s="159"/>
+      <c r="M71" s="175"/>
+      <c r="N71" s="155"/>
       <c r="O71" s="25" t="s">
         <v>71</v>
       </c>
@@ -3481,8 +3491,8 @@
       <c r="R71" s="2"/>
     </row>
     <row r="72" spans="1:18" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A72" s="168"/>
-      <c r="B72" s="159"/>
+      <c r="A72" s="175"/>
+      <c r="B72" s="155"/>
       <c r="C72" s="25" t="s">
         <v>72</v>
       </c>
@@ -3492,8 +3502,8 @@
       <c r="E72" s="2">
         <v>232</v>
       </c>
-      <c r="G72" s="168"/>
-      <c r="H72" s="159"/>
+      <c r="G72" s="175"/>
+      <c r="H72" s="155"/>
       <c r="I72" s="25" t="s">
         <v>72</v>
       </c>
@@ -3502,8 +3512,8 @@
       </c>
       <c r="K72" s="2"/>
       <c r="L72" s="2"/>
-      <c r="M72" s="168"/>
-      <c r="N72" s="159"/>
+      <c r="M72" s="175"/>
+      <c r="N72" s="155"/>
       <c r="O72" s="25" t="s">
         <v>72</v>
       </c>
@@ -3514,8 +3524,8 @@
       <c r="R72" s="2"/>
     </row>
     <row r="73" spans="1:18" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A73" s="168"/>
-      <c r="B73" s="159"/>
+      <c r="A73" s="175"/>
+      <c r="B73" s="155"/>
       <c r="C73" s="25" t="s">
         <v>73</v>
       </c>
@@ -3528,18 +3538,20 @@
       <c r="F73" t="s">
         <v>279</v>
       </c>
-      <c r="G73" s="168"/>
-      <c r="H73" s="159"/>
+      <c r="G73" s="175"/>
+      <c r="H73" s="155"/>
       <c r="I73" s="25" t="s">
         <v>73</v>
       </c>
       <c r="J73" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="K73" s="2"/>
+        <v>1</v>
+      </c>
+      <c r="K73" s="2">
+        <v>123</v>
+      </c>
       <c r="L73" s="2"/>
-      <c r="M73" s="168"/>
-      <c r="N73" s="159"/>
+      <c r="M73" s="175"/>
+      <c r="N73" s="155"/>
       <c r="O73" s="25" t="s">
         <v>73</v>
       </c>
@@ -3550,8 +3562,8 @@
       <c r="R73" s="2"/>
     </row>
     <row r="74" spans="1:18" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A74" s="168"/>
-      <c r="B74" s="159"/>
+      <c r="A74" s="175"/>
+      <c r="B74" s="155"/>
       <c r="C74" s="25" t="s">
         <v>74</v>
       </c>
@@ -3559,8 +3571,8 @@
         <v>0</v>
       </c>
       <c r="E74" s="2"/>
-      <c r="G74" s="168"/>
-      <c r="H74" s="159"/>
+      <c r="G74" s="175"/>
+      <c r="H74" s="155"/>
       <c r="I74" s="25" t="s">
         <v>74</v>
       </c>
@@ -3569,8 +3581,8 @@
       </c>
       <c r="K74" s="2"/>
       <c r="L74" s="2"/>
-      <c r="M74" s="168"/>
-      <c r="N74" s="159"/>
+      <c r="M74" s="175"/>
+      <c r="N74" s="155"/>
       <c r="O74" s="25" t="s">
         <v>74</v>
       </c>
@@ -3581,8 +3593,8 @@
       <c r="R74" s="2"/>
     </row>
     <row r="75" spans="1:18" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A75" s="168"/>
-      <c r="B75" s="159"/>
+      <c r="A75" s="175"/>
+      <c r="B75" s="155"/>
       <c r="C75" s="25" t="s">
         <v>75</v>
       </c>
@@ -3590,8 +3602,8 @@
         <v>0</v>
       </c>
       <c r="E75" s="2"/>
-      <c r="G75" s="168"/>
-      <c r="H75" s="159"/>
+      <c r="G75" s="175"/>
+      <c r="H75" s="155"/>
       <c r="I75" s="25" t="s">
         <v>75</v>
       </c>
@@ -3600,8 +3612,8 @@
       </c>
       <c r="K75" s="2"/>
       <c r="L75" s="2"/>
-      <c r="M75" s="168"/>
-      <c r="N75" s="159"/>
+      <c r="M75" s="175"/>
+      <c r="N75" s="155"/>
       <c r="O75" s="25" t="s">
         <v>75</v>
       </c>
@@ -3612,8 +3624,8 @@
       <c r="R75" s="2"/>
     </row>
     <row r="76" spans="1:18" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A76" s="168"/>
-      <c r="B76" s="159"/>
+      <c r="A76" s="175"/>
+      <c r="B76" s="155"/>
       <c r="C76" s="25" t="s">
         <v>76</v>
       </c>
@@ -3621,8 +3633,8 @@
         <v>0</v>
       </c>
       <c r="E76" s="2"/>
-      <c r="G76" s="168"/>
-      <c r="H76" s="159"/>
+      <c r="G76" s="175"/>
+      <c r="H76" s="155"/>
       <c r="I76" s="25" t="s">
         <v>76</v>
       </c>
@@ -3631,8 +3643,8 @@
       </c>
       <c r="K76" s="2"/>
       <c r="L76" s="2"/>
-      <c r="M76" s="168"/>
-      <c r="N76" s="159"/>
+      <c r="M76" s="175"/>
+      <c r="N76" s="155"/>
       <c r="O76" s="25" t="s">
         <v>76</v>
       </c>
@@ -3643,8 +3655,8 @@
       <c r="R76" s="2"/>
     </row>
     <row r="77" spans="1:18" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A77" s="168"/>
-      <c r="B77" s="159"/>
+      <c r="A77" s="175"/>
+      <c r="B77" s="155"/>
       <c r="C77" s="25" t="s">
         <v>77</v>
       </c>
@@ -3652,8 +3664,8 @@
         <v>0</v>
       </c>
       <c r="E77" s="2"/>
-      <c r="G77" s="168"/>
-      <c r="H77" s="159"/>
+      <c r="G77" s="175"/>
+      <c r="H77" s="155"/>
       <c r="I77" s="25" t="s">
         <v>77</v>
       </c>
@@ -3662,8 +3674,8 @@
       </c>
       <c r="K77" s="2"/>
       <c r="L77" s="2"/>
-      <c r="M77" s="168"/>
-      <c r="N77" s="159"/>
+      <c r="M77" s="175"/>
+      <c r="N77" s="155"/>
       <c r="O77" s="25" t="s">
         <v>77</v>
       </c>
@@ -3674,8 +3686,8 @@
       <c r="R77" s="2"/>
     </row>
     <row r="78" spans="1:18" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A78" s="168"/>
-      <c r="B78" s="159"/>
+      <c r="A78" s="175"/>
+      <c r="B78" s="155"/>
       <c r="C78" s="25" t="s">
         <v>78</v>
       </c>
@@ -3683,8 +3695,8 @@
         <v>0</v>
       </c>
       <c r="E78" s="2"/>
-      <c r="G78" s="168"/>
-      <c r="H78" s="170"/>
+      <c r="G78" s="175"/>
+      <c r="H78" s="177"/>
       <c r="I78" s="25" t="s">
         <v>78</v>
       </c>
@@ -3693,8 +3705,8 @@
       </c>
       <c r="K78" s="2"/>
       <c r="L78" s="2"/>
-      <c r="M78" s="168"/>
-      <c r="N78" s="170"/>
+      <c r="M78" s="175"/>
+      <c r="N78" s="177"/>
       <c r="O78" s="25" t="s">
         <v>78</v>
       </c>
@@ -3708,29 +3720,29 @@
       <c r="A79" s="92" t="s">
         <v>80</v>
       </c>
-      <c r="B79" s="141" t="s">
+      <c r="B79" s="203" t="s">
         <v>278</v>
       </c>
-      <c r="C79" s="142"/>
-      <c r="D79" s="142"/>
-      <c r="E79" s="142"/>
-      <c r="F79" s="143"/>
+      <c r="C79" s="204"/>
+      <c r="D79" s="204"/>
+      <c r="E79" s="204"/>
+      <c r="F79" s="205"/>
       <c r="G79" s="92" t="s">
         <v>80</v>
       </c>
-      <c r="H79" s="144"/>
-      <c r="I79" s="145"/>
-      <c r="J79" s="145"/>
-      <c r="K79" s="145"/>
-      <c r="L79" s="146"/>
+      <c r="H79" s="206"/>
+      <c r="I79" s="207"/>
+      <c r="J79" s="207"/>
+      <c r="K79" s="207"/>
+      <c r="L79" s="208"/>
       <c r="M79" s="92" t="s">
         <v>80</v>
       </c>
-      <c r="N79" s="144"/>
-      <c r="O79" s="145"/>
-      <c r="P79" s="145"/>
-      <c r="Q79" s="145"/>
-      <c r="R79" s="146"/>
+      <c r="N79" s="206"/>
+      <c r="O79" s="207"/>
+      <c r="P79" s="207"/>
+      <c r="Q79" s="207"/>
+      <c r="R79" s="208"/>
     </row>
     <row r="80" spans="1:18" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A80" s="92" t="s">
@@ -3742,11 +3754,11 @@
       <c r="C80" s="94" t="s">
         <v>238</v>
       </c>
-      <c r="D80" s="139" t="s">
+      <c r="D80" s="201" t="s">
         <v>265</v>
       </c>
-      <c r="E80" s="140"/>
-      <c r="F80" s="140"/>
+      <c r="E80" s="202"/>
+      <c r="F80" s="202"/>
       <c r="G80" s="92" t="s">
         <v>79</v>
       </c>
@@ -3756,9 +3768,9 @@
       <c r="I80" s="94" t="s">
         <v>238</v>
       </c>
-      <c r="J80" s="137"/>
-      <c r="K80" s="137"/>
-      <c r="L80" s="137"/>
+      <c r="J80" s="199"/>
+      <c r="K80" s="199"/>
+      <c r="L80" s="199"/>
       <c r="M80" s="92" t="s">
         <v>79</v>
       </c>
@@ -3768,49 +3780,49 @@
       <c r="O80" s="94" t="s">
         <v>238</v>
       </c>
-      <c r="P80" s="137"/>
-      <c r="Q80" s="137"/>
-      <c r="R80" s="137"/>
+      <c r="P80" s="199"/>
+      <c r="Q80" s="199"/>
+      <c r="R80" s="199"/>
     </row>
     <row r="81" spans="1:23" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A81" s="153" t="s">
+      <c r="A81" s="195" t="s">
         <v>81</v>
       </c>
-      <c r="B81" s="147" t="b">
+      <c r="B81" s="196" t="b">
         <v>1</v>
       </c>
       <c r="C81" s="95" t="s">
         <v>235</v>
       </c>
-      <c r="D81" s="150" t="s">
+      <c r="D81" s="209" t="s">
         <v>266</v>
       </c>
-      <c r="E81" s="140"/>
-      <c r="F81" s="140"/>
-      <c r="G81" s="153" t="s">
+      <c r="E81" s="202"/>
+      <c r="F81" s="202"/>
+      <c r="G81" s="195" t="s">
         <v>81</v>
       </c>
-      <c r="H81" s="147" t="b">
+      <c r="H81" s="196" t="b">
         <v>0</v>
       </c>
       <c r="I81" s="95" t="s">
         <v>235</v>
       </c>
-      <c r="J81" s="137"/>
-      <c r="K81" s="137"/>
-      <c r="L81" s="137"/>
-      <c r="M81" s="153" t="s">
+      <c r="J81" s="199"/>
+      <c r="K81" s="199"/>
+      <c r="L81" s="199"/>
+      <c r="M81" s="195" t="s">
         <v>81</v>
       </c>
-      <c r="N81" s="147" t="b">
+      <c r="N81" s="196" t="b">
         <v>0</v>
       </c>
       <c r="O81" s="95" t="s">
         <v>235</v>
       </c>
-      <c r="P81" s="137"/>
-      <c r="Q81" s="137"/>
-      <c r="R81" s="137"/>
+      <c r="P81" s="199"/>
+      <c r="Q81" s="199"/>
+      <c r="R81" s="199"/>
       <c r="S81" s="90"/>
       <c r="T81" s="90"/>
       <c r="U81" s="90"/>
@@ -3818,32 +3830,32 @@
       <c r="W81" s="90"/>
     </row>
     <row r="82" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="153"/>
-      <c r="B82" s="148"/>
+      <c r="A82" s="195"/>
+      <c r="B82" s="197"/>
       <c r="C82" s="96" t="s">
         <v>236</v>
       </c>
-      <c r="D82" s="151" t="s">
+      <c r="D82" s="210" t="s">
         <v>267</v>
       </c>
-      <c r="E82" s="152"/>
-      <c r="F82" s="152"/>
-      <c r="G82" s="153"/>
-      <c r="H82" s="148"/>
+      <c r="E82" s="211"/>
+      <c r="F82" s="211"/>
+      <c r="G82" s="195"/>
+      <c r="H82" s="197"/>
       <c r="I82" s="96" t="s">
         <v>236</v>
       </c>
-      <c r="J82" s="138"/>
-      <c r="K82" s="138"/>
-      <c r="L82" s="138"/>
-      <c r="M82" s="153"/>
-      <c r="N82" s="148"/>
+      <c r="J82" s="200"/>
+      <c r="K82" s="200"/>
+      <c r="L82" s="200"/>
+      <c r="M82" s="195"/>
+      <c r="N82" s="197"/>
       <c r="O82" s="96" t="s">
         <v>236</v>
       </c>
-      <c r="P82" s="138"/>
-      <c r="Q82" s="138"/>
-      <c r="R82" s="138"/>
+      <c r="P82" s="200"/>
+      <c r="Q82" s="200"/>
+      <c r="R82" s="200"/>
       <c r="S82" s="90"/>
       <c r="T82" s="90"/>
       <c r="U82" s="90"/>
@@ -3851,32 +3863,32 @@
       <c r="W82" s="90"/>
     </row>
     <row r="83" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="153"/>
-      <c r="B83" s="149"/>
+      <c r="A83" s="195"/>
+      <c r="B83" s="198"/>
       <c r="C83" s="97" t="s">
         <v>237</v>
       </c>
-      <c r="D83" s="151" t="s">
+      <c r="D83" s="210" t="s">
         <v>268</v>
       </c>
-      <c r="E83" s="152"/>
-      <c r="F83" s="152"/>
-      <c r="G83" s="153"/>
-      <c r="H83" s="149"/>
+      <c r="E83" s="211"/>
+      <c r="F83" s="211"/>
+      <c r="G83" s="195"/>
+      <c r="H83" s="198"/>
       <c r="I83" s="97" t="s">
         <v>237</v>
       </c>
-      <c r="J83" s="138"/>
-      <c r="K83" s="138"/>
-      <c r="L83" s="138"/>
-      <c r="M83" s="153"/>
-      <c r="N83" s="149"/>
+      <c r="J83" s="200"/>
+      <c r="K83" s="200"/>
+      <c r="L83" s="200"/>
+      <c r="M83" s="195"/>
+      <c r="N83" s="198"/>
       <c r="O83" s="97" t="s">
         <v>237</v>
       </c>
-      <c r="P83" s="138"/>
-      <c r="Q83" s="138"/>
-      <c r="R83" s="138"/>
+      <c r="P83" s="200"/>
+      <c r="Q83" s="200"/>
+      <c r="R83" s="200"/>
       <c r="S83" s="90"/>
       <c r="T83" s="90"/>
       <c r="U83" s="90"/>
@@ -3900,13 +3912,13 @@
       <c r="N84" s="91"/>
     </row>
     <row r="85" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="132" t="s">
+      <c r="A85" s="212" t="s">
         <v>247</v>
       </c>
-      <c r="B85" s="133"/>
-      <c r="C85" s="133"/>
-      <c r="D85" s="133"/>
-      <c r="E85" s="134"/>
+      <c r="B85" s="213"/>
+      <c r="C85" s="213"/>
+      <c r="D85" s="213"/>
+      <c r="E85" s="214"/>
       <c r="F85" s="90"/>
       <c r="G85" s="90"/>
       <c r="H85" s="90"/>
@@ -3921,12 +3933,12 @@
       <c r="A86" s="103" t="s">
         <v>146</v>
       </c>
-      <c r="B86" s="135">
+      <c r="B86" s="215">
         <v>1231</v>
       </c>
-      <c r="C86" s="135"/>
-      <c r="D86" s="135"/>
-      <c r="E86" s="136"/>
+      <c r="C86" s="215"/>
+      <c r="D86" s="215"/>
+      <c r="E86" s="216"/>
       <c r="F86" s="90"/>
       <c r="G86" s="90"/>
       <c r="H86" s="90"/>
@@ -3938,17 +3950,17 @@
       <c r="N86" s="90"/>
     </row>
     <row r="87" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="119" t="s">
+      <c r="A87" s="217" t="s">
         <v>248</v>
       </c>
       <c r="B87" s="101" t="s">
         <v>249</v>
       </c>
-      <c r="C87" s="122" t="s">
+      <c r="C87" s="218" t="s">
         <v>272</v>
       </c>
-      <c r="D87" s="122"/>
-      <c r="E87" s="123"/>
+      <c r="D87" s="218"/>
+      <c r="E87" s="219"/>
       <c r="F87" s="90"/>
       <c r="G87" s="90"/>
       <c r="H87" s="90"/>
@@ -3960,15 +3972,15 @@
       <c r="N87" s="90"/>
     </row>
     <row r="88" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="119"/>
+      <c r="A88" s="217"/>
       <c r="B88" s="102" t="s">
         <v>250</v>
       </c>
-      <c r="C88" s="122" t="s">
+      <c r="C88" s="218" t="s">
         <v>271</v>
       </c>
-      <c r="D88" s="122"/>
-      <c r="E88" s="123"/>
+      <c r="D88" s="218"/>
+      <c r="E88" s="219"/>
     </row>
     <row r="89" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="103" t="s">
@@ -3980,546 +3992,476 @@
       <c r="C89" s="100" t="s">
         <v>252</v>
       </c>
-      <c r="D89" s="128" t="s">
+      <c r="D89" s="220" t="s">
         <v>270</v>
       </c>
-      <c r="E89" s="129"/>
+      <c r="E89" s="221"/>
     </row>
     <row r="90" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="119" t="s">
+      <c r="A90" s="217" t="s">
         <v>253</v>
       </c>
-      <c r="B90" s="120" t="s">
+      <c r="B90" s="222" t="s">
         <v>254</v>
       </c>
-      <c r="C90" s="121"/>
-      <c r="D90" s="130" t="b">
-        <v>0</v>
-      </c>
-      <c r="E90" s="131"/>
+      <c r="C90" s="223"/>
+      <c r="D90" s="224" t="b">
+        <v>0</v>
+      </c>
+      <c r="E90" s="225"/>
     </row>
     <row r="91" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="119"/>
-      <c r="B91" s="124" t="s">
+      <c r="A91" s="217"/>
+      <c r="B91" s="226" t="s">
         <v>255</v>
       </c>
-      <c r="C91" s="125"/>
-      <c r="D91" s="130" t="b">
+      <c r="C91" s="227"/>
+      <c r="D91" s="224" t="b">
         <v>1</v>
       </c>
-      <c r="E91" s="131"/>
+      <c r="E91" s="225"/>
     </row>
     <row r="92" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="119"/>
-      <c r="B92" s="124" t="s">
+      <c r="A92" s="217"/>
+      <c r="B92" s="226" t="s">
         <v>256</v>
       </c>
-      <c r="C92" s="125"/>
-      <c r="D92" s="130" t="b">
-        <v>0</v>
-      </c>
-      <c r="E92" s="131"/>
+      <c r="C92" s="227"/>
+      <c r="D92" s="224" t="b">
+        <v>0</v>
+      </c>
+      <c r="E92" s="225"/>
     </row>
     <row r="93" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="119"/>
-      <c r="B93" s="124" t="s">
+      <c r="A93" s="217"/>
+      <c r="B93" s="226" t="s">
         <v>73</v>
       </c>
-      <c r="C93" s="125"/>
-      <c r="D93" s="130" t="b">
-        <v>0</v>
-      </c>
-      <c r="E93" s="131"/>
+      <c r="C93" s="227"/>
+      <c r="D93" s="224" t="b">
+        <v>0</v>
+      </c>
+      <c r="E93" s="225"/>
     </row>
     <row r="94" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="119"/>
-      <c r="B94" s="126" t="s">
+      <c r="A94" s="217"/>
+      <c r="B94" s="228" t="s">
         <v>257</v>
       </c>
-      <c r="C94" s="127"/>
-      <c r="D94" s="130" t="b">
-        <v>0</v>
-      </c>
-      <c r="E94" s="131"/>
+      <c r="C94" s="229"/>
+      <c r="D94" s="224" t="b">
+        <v>0</v>
+      </c>
+      <c r="E94" s="225"/>
     </row>
     <row r="95" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="119" t="s">
+      <c r="A95" s="217" t="s">
         <v>258</v>
       </c>
-      <c r="B95" s="120" t="s">
+      <c r="B95" s="222" t="s">
         <v>259</v>
       </c>
-      <c r="C95" s="121"/>
-      <c r="D95" s="122" t="s">
+      <c r="C95" s="223"/>
+      <c r="D95" s="218" t="s">
         <v>273</v>
       </c>
-      <c r="E95" s="123"/>
+      <c r="E95" s="219"/>
     </row>
     <row r="96" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="119"/>
-      <c r="B96" s="124" t="s">
+      <c r="A96" s="217"/>
+      <c r="B96" s="226" t="s">
         <v>260</v>
       </c>
-      <c r="C96" s="125"/>
-      <c r="D96" s="122" t="s">
+      <c r="C96" s="227"/>
+      <c r="D96" s="218" t="s">
         <v>274</v>
       </c>
-      <c r="E96" s="123"/>
+      <c r="E96" s="219"/>
     </row>
     <row r="97" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="119"/>
-      <c r="B97" s="124" t="s">
+      <c r="A97" s="217"/>
+      <c r="B97" s="226" t="s">
         <v>261</v>
       </c>
-      <c r="C97" s="125"/>
-      <c r="D97" s="122" t="s">
+      <c r="C97" s="227"/>
+      <c r="D97" s="218" t="s">
         <v>275</v>
       </c>
-      <c r="E97" s="123"/>
+      <c r="E97" s="219"/>
     </row>
     <row r="98" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="119"/>
-      <c r="B98" s="126" t="s">
+      <c r="A98" s="217"/>
+      <c r="B98" s="228" t="s">
         <v>262</v>
       </c>
-      <c r="C98" s="127"/>
-      <c r="D98" s="122" t="s">
+      <c r="C98" s="229"/>
+      <c r="D98" s="218" t="s">
         <v>276</v>
       </c>
-      <c r="E98" s="123"/>
+      <c r="E98" s="219"/>
     </row>
     <row r="99" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="103" t="s">
         <v>263</v>
       </c>
-      <c r="B99" s="117" t="s">
+      <c r="B99" s="230" t="s">
         <v>277</v>
       </c>
-      <c r="C99" s="117"/>
-      <c r="D99" s="117"/>
-      <c r="E99" s="118"/>
+      <c r="C99" s="230"/>
+      <c r="D99" s="230"/>
+      <c r="E99" s="231"/>
     </row>
     <row r="100" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="101" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A101" s="228" t="s">
+      <c r="A101" s="144" t="s">
         <v>283</v>
       </c>
-      <c r="B101" s="229"/>
-      <c r="C101" s="229"/>
-      <c r="D101" s="230"/>
+      <c r="B101" s="145"/>
+      <c r="C101" s="145"/>
+      <c r="D101" s="146"/>
     </row>
     <row r="102" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A102" s="231" t="s">
+      <c r="A102" s="147" t="s">
         <v>101</v>
       </c>
-      <c r="B102" s="232"/>
-      <c r="C102" s="232"/>
-      <c r="D102" s="233"/>
+      <c r="B102" s="142"/>
+      <c r="C102" s="142"/>
+      <c r="D102" s="148"/>
     </row>
     <row r="103" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A103" s="212" t="s">
+      <c r="A103" s="117" t="s">
         <v>102</v>
       </c>
-      <c r="B103" s="213" t="s">
+      <c r="B103" s="118" t="s">
         <v>296</v>
       </c>
-      <c r="C103" s="213"/>
-      <c r="D103" s="214"/>
+      <c r="C103" s="118"/>
+      <c r="D103" s="119"/>
     </row>
     <row r="104" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A104" s="215" t="s">
+      <c r="A104" s="120" t="s">
         <v>284</v>
       </c>
-      <c r="B104" s="216" t="s">
+      <c r="B104" s="121" t="s">
         <v>297</v>
       </c>
-      <c r="C104" s="216"/>
-      <c r="D104" s="217"/>
+      <c r="C104" s="121"/>
+      <c r="D104" s="122"/>
     </row>
     <row r="105" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A105" s="231" t="s">
+      <c r="A105" s="147" t="s">
         <v>125</v>
       </c>
-      <c r="B105" s="232"/>
-      <c r="C105" s="232"/>
-      <c r="D105" s="233"/>
+      <c r="B105" s="142"/>
+      <c r="C105" s="142"/>
+      <c r="D105" s="148"/>
     </row>
     <row r="106" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A106" s="212" t="s">
+      <c r="A106" s="117" t="s">
         <v>134</v>
       </c>
-      <c r="B106" s="213" t="s">
+      <c r="B106" s="118" t="s">
         <v>298</v>
       </c>
-      <c r="C106" s="213"/>
-      <c r="D106" s="214"/>
+      <c r="C106" s="118"/>
+      <c r="D106" s="119"/>
     </row>
     <row r="107" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A107" s="218" t="s">
+      <c r="A107" s="123" t="s">
         <v>130</v>
       </c>
-      <c r="B107" s="219" t="s">
+      <c r="B107" s="124" t="s">
         <v>299</v>
       </c>
-      <c r="C107" s="219"/>
-      <c r="D107" s="220"/>
+      <c r="C107" s="124"/>
+      <c r="D107" s="125"/>
     </row>
     <row r="108" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A108" s="231" t="s">
+      <c r="A108" s="147" t="s">
         <v>126</v>
       </c>
-      <c r="B108" s="232"/>
-      <c r="C108" s="232"/>
-      <c r="D108" s="233"/>
+      <c r="B108" s="142"/>
+      <c r="C108" s="142"/>
+      <c r="D108" s="148"/>
     </row>
     <row r="109" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A109" s="212" t="s">
+      <c r="A109" s="117" t="s">
         <v>285</v>
       </c>
-      <c r="B109" s="213" t="s">
+      <c r="B109" s="118" t="s">
         <v>300</v>
       </c>
-      <c r="C109" s="213"/>
-      <c r="D109" s="214"/>
+      <c r="C109" s="118"/>
+      <c r="D109" s="119"/>
     </row>
     <row r="110" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A110" s="212" t="s">
+      <c r="A110" s="117" t="s">
         <v>130</v>
       </c>
-      <c r="B110" s="213" t="s">
+      <c r="B110" s="118" t="s">
         <v>301</v>
       </c>
-      <c r="C110" s="213"/>
-      <c r="D110" s="214"/>
+      <c r="C110" s="118"/>
+      <c r="D110" s="119"/>
     </row>
     <row r="111" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A111" s="215" t="s">
+      <c r="A111" s="120" t="s">
         <v>109</v>
       </c>
-      <c r="B111" s="216" t="s">
+      <c r="B111" s="121" t="s">
         <v>302</v>
       </c>
-      <c r="C111" s="216"/>
-      <c r="D111" s="217"/>
+      <c r="C111" s="121"/>
+      <c r="D111" s="122"/>
     </row>
     <row r="112" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A112" s="231" t="s">
+      <c r="A112" s="147" t="s">
         <v>135</v>
       </c>
-      <c r="B112" s="232"/>
-      <c r="C112" s="232"/>
-      <c r="D112" s="233"/>
+      <c r="B112" s="142"/>
+      <c r="C112" s="142"/>
+      <c r="D112" s="148"/>
     </row>
     <row r="113" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A113" s="215" t="s">
+      <c r="A113" s="120" t="s">
         <v>103</v>
       </c>
-      <c r="B113" s="239">
+      <c r="B113" s="133">
         <v>123123</v>
       </c>
-      <c r="C113" s="216"/>
-      <c r="D113" s="217"/>
+      <c r="C113" s="121"/>
+      <c r="D113" s="122"/>
     </row>
     <row r="114" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A114" s="212" t="s">
+      <c r="A114" s="117" t="s">
         <v>286</v>
       </c>
-      <c r="B114" s="240" t="s">
+      <c r="B114" s="134" t="s">
         <v>303</v>
       </c>
-      <c r="C114" s="221" t="s">
+      <c r="C114" s="126" t="s">
         <v>287</v>
       </c>
-      <c r="D114" s="240" t="s">
+      <c r="D114" s="134" t="s">
         <v>305</v>
       </c>
     </row>
     <row r="115" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A115" s="215" t="s">
+      <c r="A115" s="120" t="s">
         <v>288</v>
       </c>
-      <c r="B115" s="241" t="s">
+      <c r="B115" s="135" t="s">
         <v>304</v>
       </c>
-      <c r="C115" s="218" t="s">
+      <c r="C115" s="123" t="s">
         <v>147</v>
       </c>
-      <c r="D115" s="241" t="s">
+      <c r="D115" s="135" t="s">
         <v>306</v>
       </c>
     </row>
     <row r="116" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A116" s="212" t="s">
+      <c r="A116" s="117" t="s">
         <v>289</v>
       </c>
-      <c r="B116" s="242">
+      <c r="B116" s="136">
         <v>12313</v>
       </c>
-      <c r="C116" s="213"/>
-      <c r="D116" s="214"/>
+      <c r="C116" s="118"/>
+      <c r="D116" s="119"/>
     </row>
     <row r="117" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A117" s="212" t="s">
+      <c r="A117" s="117" t="s">
         <v>154</v>
       </c>
-      <c r="B117" s="242" t="s">
+      <c r="B117" s="136" t="s">
         <v>307</v>
       </c>
-      <c r="C117" s="213"/>
-      <c r="D117" s="214"/>
+      <c r="C117" s="118"/>
+      <c r="D117" s="119"/>
     </row>
     <row r="118" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A118" s="222" t="s">
+      <c r="A118" s="127" t="s">
         <v>156</v>
       </c>
-      <c r="B118" s="242">
+      <c r="B118" s="136">
         <v>21321</v>
       </c>
-      <c r="C118" s="213"/>
-      <c r="D118" s="214"/>
+      <c r="C118" s="118"/>
+      <c r="D118" s="119"/>
     </row>
     <row r="119" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A119" s="215" t="s">
+      <c r="A119" s="120" t="s">
         <v>159</v>
       </c>
-      <c r="B119" s="239" t="s">
+      <c r="B119" s="133" t="s">
         <v>317</v>
       </c>
-      <c r="C119" s="216"/>
-      <c r="D119" s="217"/>
+      <c r="C119" s="121"/>
+      <c r="D119" s="122"/>
     </row>
     <row r="120" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A120" s="234" t="s">
+      <c r="A120" s="138" t="s">
         <v>290</v>
       </c>
-      <c r="B120" s="235"/>
-      <c r="C120" s="235"/>
-      <c r="D120" s="236"/>
+      <c r="B120" s="139"/>
+      <c r="C120" s="139"/>
+      <c r="D120" s="140"/>
     </row>
     <row r="121" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A121" s="212" t="s">
+      <c r="A121" s="117" t="s">
         <v>291</v>
       </c>
-      <c r="B121" s="243">
+      <c r="B121" s="137">
         <v>3211223</v>
       </c>
-      <c r="C121" s="221" t="s">
+      <c r="C121" s="126" t="s">
         <v>292</v>
       </c>
-      <c r="D121" s="243">
+      <c r="D121" s="137">
         <v>2132312</v>
       </c>
     </row>
     <row r="122" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A122" s="215" t="s">
+      <c r="A122" s="120" t="s">
         <v>293</v>
       </c>
-      <c r="B122" s="241">
+      <c r="B122" s="135">
         <v>1221213</v>
       </c>
-      <c r="C122" s="218" t="s">
+      <c r="C122" s="123" t="s">
         <v>294</v>
       </c>
-      <c r="D122" s="241" t="s">
+      <c r="D122" s="135" t="s">
         <v>318</v>
       </c>
     </row>
     <row r="123" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A123" s="234" t="s">
+      <c r="A123" s="138" t="s">
         <v>175</v>
       </c>
-      <c r="B123" s="235"/>
-      <c r="C123" s="235"/>
-      <c r="D123" s="236"/>
+      <c r="B123" s="139"/>
+      <c r="C123" s="139"/>
+      <c r="D123" s="140"/>
     </row>
     <row r="124" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A124" s="224" t="s">
+      <c r="A124" s="129" t="s">
         <v>295</v>
       </c>
-      <c r="B124" s="219" t="s">
+      <c r="B124" s="124" t="s">
         <v>308</v>
       </c>
-      <c r="C124" s="219"/>
-      <c r="D124" s="220"/>
+      <c r="C124" s="124"/>
+      <c r="D124" s="125"/>
     </row>
     <row r="125" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A125" s="237" t="s">
+      <c r="A125" s="141" t="s">
         <v>172</v>
       </c>
-      <c r="B125" s="232"/>
-      <c r="C125" s="232"/>
-      <c r="D125" s="238"/>
+      <c r="B125" s="142"/>
+      <c r="C125" s="142"/>
+      <c r="D125" s="143"/>
     </row>
     <row r="126" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A126" s="222" t="s">
+      <c r="A126" s="127" t="s">
         <v>176</v>
       </c>
-      <c r="B126" s="223" t="s">
+      <c r="B126" s="128" t="s">
         <v>309</v>
       </c>
-      <c r="C126" s="225" t="s">
+      <c r="C126" s="130" t="s">
         <v>178</v>
       </c>
-      <c r="D126" s="240">
+      <c r="D126" s="134">
         <v>123</v>
       </c>
     </row>
     <row r="127" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A127" s="226" t="s">
+      <c r="A127" s="131" t="s">
         <v>182</v>
       </c>
-      <c r="B127" s="217" t="s">
+      <c r="B127" s="122" t="s">
         <v>310</v>
       </c>
-      <c r="C127" s="227" t="s">
+      <c r="C127" s="132" t="s">
         <v>183</v>
       </c>
-      <c r="D127" s="241" t="s">
+      <c r="D127" s="135" t="s">
         <v>315</v>
       </c>
     </row>
     <row r="128" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A128" s="234" t="s">
+      <c r="A128" s="138" t="s">
         <v>186</v>
       </c>
-      <c r="B128" s="235"/>
-      <c r="C128" s="235"/>
-      <c r="D128" s="236"/>
+      <c r="B128" s="139"/>
+      <c r="C128" s="139"/>
+      <c r="D128" s="140"/>
     </row>
     <row r="129" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A129" s="222" t="s">
+      <c r="A129" s="127" t="s">
         <v>187</v>
       </c>
-      <c r="B129" s="214" t="s">
+      <c r="B129" s="119" t="s">
         <v>313</v>
       </c>
-      <c r="C129" s="225" t="s">
+      <c r="C129" s="130" t="s">
         <v>189</v>
       </c>
-      <c r="D129" s="214" t="s">
+      <c r="D129" s="119" t="s">
         <v>314</v>
       </c>
     </row>
     <row r="130" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A130" s="226" t="s">
+      <c r="A130" s="131" t="s">
         <v>191</v>
       </c>
-      <c r="B130" s="220" t="s">
+      <c r="B130" s="125" t="s">
         <v>311</v>
       </c>
-      <c r="C130" s="227" t="s">
+      <c r="C130" s="132" t="s">
         <v>193</v>
       </c>
-      <c r="D130" s="217" t="s">
+      <c r="D130" s="122" t="s">
         <v>315</v>
       </c>
     </row>
     <row r="131" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A131" s="226" t="s">
+      <c r="A131" s="131" t="s">
         <v>102</v>
       </c>
-      <c r="B131" s="217" t="s">
+      <c r="B131" s="122" t="s">
         <v>296</v>
       </c>
-      <c r="C131" s="227" t="s">
+      <c r="C131" s="132" t="s">
         <v>195</v>
       </c>
-      <c r="D131" s="217" t="s">
+      <c r="D131" s="122" t="s">
         <v>316</v>
       </c>
     </row>
     <row r="132" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A132" s="226" t="s">
+      <c r="A132" s="131" t="s">
         <v>196</v>
       </c>
-      <c r="B132" s="216" t="s">
+      <c r="B132" s="121" t="s">
         <v>312</v>
       </c>
-      <c r="C132" s="216"/>
-      <c r="D132" s="217"/>
+      <c r="C132" s="121"/>
+      <c r="D132" s="122"/>
     </row>
   </sheetData>
   <mergeCells count="107">
-    <mergeCell ref="A120:D120"/>
-    <mergeCell ref="A123:D123"/>
-    <mergeCell ref="A125:D125"/>
-    <mergeCell ref="A128:D128"/>
-    <mergeCell ref="A101:D101"/>
-    <mergeCell ref="A102:D102"/>
-    <mergeCell ref="A105:D105"/>
-    <mergeCell ref="A108:D108"/>
-    <mergeCell ref="A112:D112"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="H36:I36"/>
-    <mergeCell ref="A38:C38"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="H64:L64"/>
-    <mergeCell ref="A28:A35"/>
-    <mergeCell ref="A41:A48"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="H26:I26"/>
-    <mergeCell ref="H27:I27"/>
-    <mergeCell ref="G65:G78"/>
-    <mergeCell ref="H67:H78"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="H25:I25"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="A65:A78"/>
-    <mergeCell ref="B67:B78"/>
-    <mergeCell ref="D28:D35"/>
-    <mergeCell ref="G28:G35"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A6:D6"/>
-    <mergeCell ref="A22:I22"/>
-    <mergeCell ref="A23:C23"/>
-    <mergeCell ref="D23:F23"/>
-    <mergeCell ref="G23:I23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="C65:F65"/>
-    <mergeCell ref="C66:F66"/>
-    <mergeCell ref="I66:L66"/>
-    <mergeCell ref="O66:R66"/>
-    <mergeCell ref="A62:R62"/>
-    <mergeCell ref="A63:F63"/>
-    <mergeCell ref="G63:L63"/>
-    <mergeCell ref="M63:R63"/>
-    <mergeCell ref="B64:F64"/>
-    <mergeCell ref="N64:R64"/>
-    <mergeCell ref="O65:R65"/>
-    <mergeCell ref="I65:L65"/>
-    <mergeCell ref="M65:M78"/>
-    <mergeCell ref="N67:N78"/>
-    <mergeCell ref="A81:A83"/>
-    <mergeCell ref="B81:B83"/>
-    <mergeCell ref="G81:G83"/>
-    <mergeCell ref="H81:H83"/>
-    <mergeCell ref="M81:M83"/>
-    <mergeCell ref="P81:R81"/>
-    <mergeCell ref="P82:R82"/>
-    <mergeCell ref="P83:R83"/>
-    <mergeCell ref="D80:F80"/>
-    <mergeCell ref="B79:F79"/>
-    <mergeCell ref="J80:L80"/>
-    <mergeCell ref="H79:L79"/>
-    <mergeCell ref="P80:R80"/>
-    <mergeCell ref="N79:R79"/>
-    <mergeCell ref="N81:N83"/>
-    <mergeCell ref="D81:F81"/>
-    <mergeCell ref="D82:F82"/>
-    <mergeCell ref="D83:F83"/>
-    <mergeCell ref="J81:L81"/>
-    <mergeCell ref="J82:L82"/>
-    <mergeCell ref="J83:L83"/>
+    <mergeCell ref="B99:E99"/>
+    <mergeCell ref="A95:A98"/>
+    <mergeCell ref="B95:C95"/>
+    <mergeCell ref="D95:E95"/>
+    <mergeCell ref="B96:C96"/>
+    <mergeCell ref="D96:E96"/>
+    <mergeCell ref="B97:C97"/>
+    <mergeCell ref="D97:E97"/>
+    <mergeCell ref="B98:C98"/>
+    <mergeCell ref="D98:E98"/>
     <mergeCell ref="A85:E85"/>
     <mergeCell ref="B86:E86"/>
     <mergeCell ref="A87:A88"/>
@@ -4537,16 +4479,86 @@
     <mergeCell ref="D93:E93"/>
     <mergeCell ref="B94:C94"/>
     <mergeCell ref="D94:E94"/>
-    <mergeCell ref="B99:E99"/>
-    <mergeCell ref="A95:A98"/>
-    <mergeCell ref="B95:C95"/>
-    <mergeCell ref="D95:E95"/>
-    <mergeCell ref="B96:C96"/>
-    <mergeCell ref="D96:E96"/>
-    <mergeCell ref="B97:C97"/>
-    <mergeCell ref="D97:E97"/>
-    <mergeCell ref="B98:C98"/>
-    <mergeCell ref="D98:E98"/>
+    <mergeCell ref="B79:F79"/>
+    <mergeCell ref="J80:L80"/>
+    <mergeCell ref="H79:L79"/>
+    <mergeCell ref="P80:R80"/>
+    <mergeCell ref="N79:R79"/>
+    <mergeCell ref="N81:N83"/>
+    <mergeCell ref="D81:F81"/>
+    <mergeCell ref="D82:F82"/>
+    <mergeCell ref="D83:F83"/>
+    <mergeCell ref="J81:L81"/>
+    <mergeCell ref="J82:L82"/>
+    <mergeCell ref="J83:L83"/>
+    <mergeCell ref="A81:A83"/>
+    <mergeCell ref="B81:B83"/>
+    <mergeCell ref="G81:G83"/>
+    <mergeCell ref="H81:H83"/>
+    <mergeCell ref="M81:M83"/>
+    <mergeCell ref="P81:R81"/>
+    <mergeCell ref="P82:R82"/>
+    <mergeCell ref="P83:R83"/>
+    <mergeCell ref="D80:F80"/>
+    <mergeCell ref="O66:R66"/>
+    <mergeCell ref="A62:R62"/>
+    <mergeCell ref="A63:F63"/>
+    <mergeCell ref="G63:L63"/>
+    <mergeCell ref="M63:R63"/>
+    <mergeCell ref="B64:F64"/>
+    <mergeCell ref="N64:R64"/>
+    <mergeCell ref="O65:R65"/>
+    <mergeCell ref="I65:L65"/>
+    <mergeCell ref="M65:M78"/>
+    <mergeCell ref="N67:N78"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A6:D6"/>
+    <mergeCell ref="A22:I22"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="D23:F23"/>
+    <mergeCell ref="G23:I23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="G65:G78"/>
+    <mergeCell ref="H67:H78"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="A65:A78"/>
+    <mergeCell ref="B67:B78"/>
+    <mergeCell ref="D28:D35"/>
+    <mergeCell ref="G28:G35"/>
+    <mergeCell ref="C65:F65"/>
+    <mergeCell ref="C66:F66"/>
+    <mergeCell ref="I66:L66"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="H36:I36"/>
+    <mergeCell ref="A38:C38"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="H64:L64"/>
+    <mergeCell ref="A28:A35"/>
+    <mergeCell ref="A41:A48"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="A120:D120"/>
+    <mergeCell ref="A123:D123"/>
+    <mergeCell ref="A125:D125"/>
+    <mergeCell ref="A128:D128"/>
+    <mergeCell ref="A101:D101"/>
+    <mergeCell ref="A102:D102"/>
+    <mergeCell ref="A105:D105"/>
+    <mergeCell ref="A108:D108"/>
+    <mergeCell ref="A112:D112"/>
   </mergeCells>
   <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="B20" xr:uid="{00000000-0002-0000-0000-000000000000}">
@@ -4599,421 +4611,421 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:175" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="204" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="161"/>
-      <c r="C1" s="162"/>
-      <c r="D1" s="204" t="s">
+      <c r="A1" s="235" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="157"/>
+      <c r="C1" s="158"/>
+      <c r="D1" s="235" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="161"/>
-      <c r="F1" s="161"/>
-      <c r="G1" s="161"/>
-      <c r="H1" s="161"/>
-      <c r="I1" s="161"/>
-      <c r="J1" s="161"/>
-      <c r="K1" s="161"/>
-      <c r="L1" s="161"/>
-      <c r="M1" s="161"/>
-      <c r="N1" s="161"/>
-      <c r="O1" s="162"/>
-      <c r="P1" s="204" t="s">
+      <c r="E1" s="157"/>
+      <c r="F1" s="157"/>
+      <c r="G1" s="157"/>
+      <c r="H1" s="157"/>
+      <c r="I1" s="157"/>
+      <c r="J1" s="157"/>
+      <c r="K1" s="157"/>
+      <c r="L1" s="157"/>
+      <c r="M1" s="157"/>
+      <c r="N1" s="157"/>
+      <c r="O1" s="158"/>
+      <c r="P1" s="235" t="s">
         <v>82</v>
       </c>
-      <c r="Q1" s="161"/>
-      <c r="R1" s="161"/>
-      <c r="S1" s="162"/>
-      <c r="T1" s="200" t="s">
+      <c r="Q1" s="157"/>
+      <c r="R1" s="157"/>
+      <c r="S1" s="158"/>
+      <c r="T1" s="234" t="s">
         <v>83</v>
       </c>
-      <c r="U1" s="161"/>
-      <c r="V1" s="161"/>
-      <c r="W1" s="161"/>
-      <c r="X1" s="161"/>
-      <c r="Y1" s="161"/>
-      <c r="Z1" s="161"/>
-      <c r="AA1" s="161"/>
-      <c r="AB1" s="161"/>
-      <c r="AC1" s="161"/>
-      <c r="AD1" s="161"/>
-      <c r="AE1" s="161"/>
-      <c r="AF1" s="162"/>
-      <c r="AG1" s="200" t="s">
+      <c r="U1" s="157"/>
+      <c r="V1" s="157"/>
+      <c r="W1" s="157"/>
+      <c r="X1" s="157"/>
+      <c r="Y1" s="157"/>
+      <c r="Z1" s="157"/>
+      <c r="AA1" s="157"/>
+      <c r="AB1" s="157"/>
+      <c r="AC1" s="157"/>
+      <c r="AD1" s="157"/>
+      <c r="AE1" s="157"/>
+      <c r="AF1" s="158"/>
+      <c r="AG1" s="234" t="s">
         <v>84</v>
       </c>
-      <c r="AH1" s="161"/>
-      <c r="AI1" s="161"/>
-      <c r="AJ1" s="161"/>
-      <c r="AK1" s="161"/>
-      <c r="AL1" s="161"/>
-      <c r="AM1" s="161"/>
-      <c r="AN1" s="161"/>
-      <c r="AO1" s="161"/>
-      <c r="AP1" s="161"/>
-      <c r="AQ1" s="161"/>
-      <c r="AR1" s="161"/>
-      <c r="AS1" s="162"/>
-      <c r="AT1" s="200" t="s">
+      <c r="AH1" s="157"/>
+      <c r="AI1" s="157"/>
+      <c r="AJ1" s="157"/>
+      <c r="AK1" s="157"/>
+      <c r="AL1" s="157"/>
+      <c r="AM1" s="157"/>
+      <c r="AN1" s="157"/>
+      <c r="AO1" s="157"/>
+      <c r="AP1" s="157"/>
+      <c r="AQ1" s="157"/>
+      <c r="AR1" s="157"/>
+      <c r="AS1" s="158"/>
+      <c r="AT1" s="234" t="s">
         <v>48</v>
       </c>
-      <c r="AU1" s="161"/>
-      <c r="AV1" s="161"/>
-      <c r="AW1" s="161"/>
-      <c r="AX1" s="161"/>
-      <c r="AY1" s="161"/>
-      <c r="AZ1" s="162"/>
-      <c r="BA1" s="200" t="s">
+      <c r="AU1" s="157"/>
+      <c r="AV1" s="157"/>
+      <c r="AW1" s="157"/>
+      <c r="AX1" s="157"/>
+      <c r="AY1" s="157"/>
+      <c r="AZ1" s="158"/>
+      <c r="BA1" s="234" t="s">
         <v>85</v>
       </c>
-      <c r="BB1" s="161"/>
-      <c r="BC1" s="161"/>
-      <c r="BD1" s="161"/>
-      <c r="BE1" s="161"/>
-      <c r="BF1" s="161"/>
-      <c r="BG1" s="161"/>
-      <c r="BH1" s="161"/>
-      <c r="BI1" s="161"/>
-      <c r="BJ1" s="161"/>
-      <c r="BK1" s="161"/>
-      <c r="BL1" s="161"/>
-      <c r="BM1" s="161"/>
-      <c r="BN1" s="161"/>
-      <c r="BO1" s="161"/>
-      <c r="BP1" s="161"/>
-      <c r="BQ1" s="161"/>
-      <c r="BR1" s="161"/>
-      <c r="BS1" s="161"/>
-      <c r="BT1" s="161"/>
-      <c r="BU1" s="161"/>
-      <c r="BV1" s="161"/>
-      <c r="BW1" s="161"/>
-      <c r="BX1" s="161"/>
-      <c r="BY1" s="161"/>
-      <c r="BZ1" s="161"/>
-      <c r="CA1" s="161"/>
-      <c r="CB1" s="161"/>
-      <c r="CC1" s="161"/>
-      <c r="CD1" s="161"/>
-      <c r="CE1" s="161"/>
-      <c r="CF1" s="161"/>
-      <c r="CG1" s="161"/>
-      <c r="CH1" s="161"/>
-      <c r="CI1" s="161"/>
-      <c r="CJ1" s="161"/>
-      <c r="CK1" s="161"/>
-      <c r="CL1" s="161"/>
-      <c r="CM1" s="162"/>
+      <c r="BB1" s="157"/>
+      <c r="BC1" s="157"/>
+      <c r="BD1" s="157"/>
+      <c r="BE1" s="157"/>
+      <c r="BF1" s="157"/>
+      <c r="BG1" s="157"/>
+      <c r="BH1" s="157"/>
+      <c r="BI1" s="157"/>
+      <c r="BJ1" s="157"/>
+      <c r="BK1" s="157"/>
+      <c r="BL1" s="157"/>
+      <c r="BM1" s="157"/>
+      <c r="BN1" s="157"/>
+      <c r="BO1" s="157"/>
+      <c r="BP1" s="157"/>
+      <c r="BQ1" s="157"/>
+      <c r="BR1" s="157"/>
+      <c r="BS1" s="157"/>
+      <c r="BT1" s="157"/>
+      <c r="BU1" s="157"/>
+      <c r="BV1" s="157"/>
+      <c r="BW1" s="157"/>
+      <c r="BX1" s="157"/>
+      <c r="BY1" s="157"/>
+      <c r="BZ1" s="157"/>
+      <c r="CA1" s="157"/>
+      <c r="CB1" s="157"/>
+      <c r="CC1" s="157"/>
+      <c r="CD1" s="157"/>
+      <c r="CE1" s="157"/>
+      <c r="CF1" s="157"/>
+      <c r="CG1" s="157"/>
+      <c r="CH1" s="157"/>
+      <c r="CI1" s="157"/>
+      <c r="CJ1" s="157"/>
+      <c r="CK1" s="157"/>
+      <c r="CL1" s="157"/>
+      <c r="CM1" s="158"/>
     </row>
     <row r="2" spans="1:175" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="205" t="s">
+      <c r="A2" s="236" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="201" t="s">
+      <c r="B2" s="232" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="201" t="s">
+      <c r="C2" s="232" t="s">
         <v>86</v>
       </c>
-      <c r="D2" s="201" t="s">
+      <c r="D2" s="232" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="201" t="s">
+      <c r="E2" s="232" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="201" t="s">
+      <c r="F2" s="232" t="s">
         <v>87</v>
       </c>
-      <c r="G2" s="201" t="s">
+      <c r="G2" s="232" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="201" t="s">
+      <c r="H2" s="232" t="s">
         <v>10</v>
       </c>
-      <c r="I2" s="201" t="s">
+      <c r="I2" s="232" t="s">
         <v>11</v>
       </c>
-      <c r="J2" s="201" t="s">
+      <c r="J2" s="232" t="s">
         <v>12</v>
       </c>
-      <c r="K2" s="201" t="s">
+      <c r="K2" s="232" t="s">
         <v>13</v>
       </c>
-      <c r="L2" s="201" t="s">
+      <c r="L2" s="232" t="s">
         <v>88</v>
       </c>
-      <c r="M2" s="201" t="s">
+      <c r="M2" s="232" t="s">
         <v>15</v>
       </c>
-      <c r="N2" s="201" t="s">
+      <c r="N2" s="232" t="s">
         <v>16</v>
       </c>
-      <c r="O2" s="201" t="s">
+      <c r="O2" s="232" t="s">
         <v>89</v>
       </c>
-      <c r="P2" s="201" t="s">
+      <c r="P2" s="232" t="s">
         <v>90</v>
       </c>
-      <c r="Q2" s="201" t="s">
+      <c r="Q2" s="232" t="s">
         <v>91</v>
       </c>
-      <c r="R2" s="201" t="s">
+      <c r="R2" s="232" t="s">
         <v>23</v>
       </c>
-      <c r="S2" s="201" t="s">
+      <c r="S2" s="232" t="s">
         <v>25</v>
       </c>
-      <c r="T2" s="201" t="s">
+      <c r="T2" s="232" t="s">
         <v>30</v>
       </c>
-      <c r="U2" s="201" t="s">
+      <c r="U2" s="232" t="s">
         <v>6</v>
       </c>
-      <c r="V2" s="201" t="s">
+      <c r="V2" s="232" t="s">
         <v>92</v>
       </c>
-      <c r="W2" s="201" t="s">
+      <c r="W2" s="232" t="s">
         <v>93</v>
       </c>
-      <c r="X2" s="200" t="s">
+      <c r="X2" s="234" t="s">
         <v>32</v>
       </c>
-      <c r="Y2" s="161"/>
-      <c r="Z2" s="161"/>
-      <c r="AA2" s="161"/>
-      <c r="AB2" s="161"/>
-      <c r="AC2" s="161"/>
-      <c r="AD2" s="161"/>
-      <c r="AE2" s="162"/>
-      <c r="AF2" s="201" t="s">
+      <c r="Y2" s="157"/>
+      <c r="Z2" s="157"/>
+      <c r="AA2" s="157"/>
+      <c r="AB2" s="157"/>
+      <c r="AC2" s="157"/>
+      <c r="AD2" s="157"/>
+      <c r="AE2" s="158"/>
+      <c r="AF2" s="232" t="s">
         <v>41</v>
       </c>
-      <c r="AG2" s="201" t="s">
+      <c r="AG2" s="232" t="s">
         <v>94</v>
       </c>
-      <c r="AH2" s="201" t="s">
+      <c r="AH2" s="232" t="s">
         <v>44</v>
       </c>
-      <c r="AI2" s="204" t="s">
+      <c r="AI2" s="235" t="s">
         <v>32</v>
       </c>
-      <c r="AJ2" s="161"/>
-      <c r="AK2" s="161"/>
-      <c r="AL2" s="161"/>
-      <c r="AM2" s="161"/>
-      <c r="AN2" s="161"/>
-      <c r="AO2" s="161"/>
-      <c r="AP2" s="162"/>
-      <c r="AQ2" s="201" t="s">
+      <c r="AJ2" s="157"/>
+      <c r="AK2" s="157"/>
+      <c r="AL2" s="157"/>
+      <c r="AM2" s="157"/>
+      <c r="AN2" s="157"/>
+      <c r="AO2" s="157"/>
+      <c r="AP2" s="158"/>
+      <c r="AQ2" s="232" t="s">
         <v>41</v>
       </c>
-      <c r="AR2" s="201" t="s">
+      <c r="AR2" s="232" t="s">
         <v>46</v>
       </c>
-      <c r="AS2" s="201" t="s">
+      <c r="AS2" s="232" t="s">
         <v>47</v>
       </c>
-      <c r="AT2" s="201" t="s">
+      <c r="AT2" s="232" t="s">
         <v>95</v>
       </c>
-      <c r="AU2" s="201" t="s">
+      <c r="AU2" s="232" t="s">
         <v>50</v>
       </c>
-      <c r="AV2" s="201" t="s">
+      <c r="AV2" s="232" t="s">
         <v>51</v>
       </c>
-      <c r="AW2" s="201" t="s">
+      <c r="AW2" s="232" t="s">
         <v>52</v>
       </c>
-      <c r="AX2" s="201" t="s">
+      <c r="AX2" s="232" t="s">
         <v>22</v>
       </c>
-      <c r="AY2" s="201" t="s">
+      <c r="AY2" s="232" t="s">
         <v>53</v>
       </c>
-      <c r="AZ2" s="201" t="s">
+      <c r="AZ2" s="232" t="s">
         <v>54</v>
       </c>
-      <c r="BA2" s="201" t="s">
+      <c r="BA2" s="232" t="s">
         <v>30</v>
       </c>
-      <c r="BB2" s="200" t="s">
+      <c r="BB2" s="234" t="s">
         <v>59</v>
       </c>
-      <c r="BC2" s="161"/>
-      <c r="BD2" s="161"/>
-      <c r="BE2" s="161"/>
-      <c r="BF2" s="161"/>
-      <c r="BG2" s="161"/>
-      <c r="BH2" s="161"/>
-      <c r="BI2" s="161"/>
-      <c r="BJ2" s="161"/>
-      <c r="BK2" s="161"/>
-      <c r="BL2" s="161"/>
-      <c r="BM2" s="161"/>
-      <c r="BN2" s="161"/>
-      <c r="BO2" s="161"/>
-      <c r="BP2" s="161"/>
-      <c r="BQ2" s="161"/>
-      <c r="BR2" s="161"/>
-      <c r="BS2" s="161"/>
-      <c r="BT2" s="161"/>
-      <c r="BU2" s="161"/>
-      <c r="BV2" s="161"/>
-      <c r="BW2" s="161"/>
-      <c r="BX2" s="161"/>
-      <c r="BY2" s="161"/>
-      <c r="BZ2" s="161"/>
-      <c r="CA2" s="161"/>
-      <c r="CB2" s="161"/>
-      <c r="CC2" s="161"/>
-      <c r="CD2" s="161"/>
-      <c r="CE2" s="161"/>
-      <c r="CF2" s="161"/>
-      <c r="CG2" s="161"/>
-      <c r="CH2" s="161"/>
-      <c r="CI2" s="161"/>
-      <c r="CJ2" s="162"/>
-      <c r="CK2" s="201" t="s">
+      <c r="BC2" s="157"/>
+      <c r="BD2" s="157"/>
+      <c r="BE2" s="157"/>
+      <c r="BF2" s="157"/>
+      <c r="BG2" s="157"/>
+      <c r="BH2" s="157"/>
+      <c r="BI2" s="157"/>
+      <c r="BJ2" s="157"/>
+      <c r="BK2" s="157"/>
+      <c r="BL2" s="157"/>
+      <c r="BM2" s="157"/>
+      <c r="BN2" s="157"/>
+      <c r="BO2" s="157"/>
+      <c r="BP2" s="157"/>
+      <c r="BQ2" s="157"/>
+      <c r="BR2" s="157"/>
+      <c r="BS2" s="157"/>
+      <c r="BT2" s="157"/>
+      <c r="BU2" s="157"/>
+      <c r="BV2" s="157"/>
+      <c r="BW2" s="157"/>
+      <c r="BX2" s="157"/>
+      <c r="BY2" s="157"/>
+      <c r="BZ2" s="157"/>
+      <c r="CA2" s="157"/>
+      <c r="CB2" s="157"/>
+      <c r="CC2" s="157"/>
+      <c r="CD2" s="157"/>
+      <c r="CE2" s="157"/>
+      <c r="CF2" s="157"/>
+      <c r="CG2" s="157"/>
+      <c r="CH2" s="157"/>
+      <c r="CI2" s="157"/>
+      <c r="CJ2" s="158"/>
+      <c r="CK2" s="232" t="s">
         <v>79</v>
       </c>
-      <c r="CL2" s="201" t="s">
+      <c r="CL2" s="232" t="s">
         <v>80</v>
       </c>
-      <c r="CM2" s="201" t="s">
+      <c r="CM2" s="232" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:175" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="168"/>
-      <c r="B3" s="168"/>
-      <c r="C3" s="168"/>
-      <c r="D3" s="168"/>
-      <c r="E3" s="168"/>
-      <c r="F3" s="168"/>
-      <c r="G3" s="168"/>
-      <c r="H3" s="168"/>
-      <c r="I3" s="168"/>
-      <c r="J3" s="168"/>
-      <c r="K3" s="168"/>
-      <c r="L3" s="168"/>
-      <c r="M3" s="168"/>
-      <c r="N3" s="168"/>
-      <c r="O3" s="168"/>
-      <c r="P3" s="168"/>
-      <c r="Q3" s="168"/>
-      <c r="R3" s="168"/>
-      <c r="S3" s="168"/>
-      <c r="T3" s="168"/>
-      <c r="U3" s="168"/>
-      <c r="V3" s="168"/>
-      <c r="W3" s="168"/>
-      <c r="X3" s="201" t="s">
+      <c r="A3" s="175"/>
+      <c r="B3" s="175"/>
+      <c r="C3" s="175"/>
+      <c r="D3" s="175"/>
+      <c r="E3" s="175"/>
+      <c r="F3" s="175"/>
+      <c r="G3" s="175"/>
+      <c r="H3" s="175"/>
+      <c r="I3" s="175"/>
+      <c r="J3" s="175"/>
+      <c r="K3" s="175"/>
+      <c r="L3" s="175"/>
+      <c r="M3" s="175"/>
+      <c r="N3" s="175"/>
+      <c r="O3" s="175"/>
+      <c r="P3" s="175"/>
+      <c r="Q3" s="175"/>
+      <c r="R3" s="175"/>
+      <c r="S3" s="175"/>
+      <c r="T3" s="175"/>
+      <c r="U3" s="175"/>
+      <c r="V3" s="175"/>
+      <c r="W3" s="175"/>
+      <c r="X3" s="232" t="s">
         <v>96</v>
       </c>
-      <c r="Y3" s="201" t="s">
+      <c r="Y3" s="232" t="s">
         <v>34</v>
       </c>
-      <c r="Z3" s="201" t="s">
+      <c r="Z3" s="232" t="s">
         <v>35</v>
       </c>
-      <c r="AA3" s="201" t="s">
+      <c r="AA3" s="232" t="s">
         <v>36</v>
       </c>
-      <c r="AB3" s="201" t="s">
+      <c r="AB3" s="232" t="s">
         <v>37</v>
       </c>
-      <c r="AC3" s="201" t="s">
+      <c r="AC3" s="232" t="s">
         <v>38</v>
       </c>
-      <c r="AD3" s="201" t="s">
+      <c r="AD3" s="232" t="s">
         <v>39</v>
       </c>
-      <c r="AE3" s="201" t="s">
+      <c r="AE3" s="232" t="s">
         <v>40</v>
       </c>
-      <c r="AF3" s="168"/>
-      <c r="AG3" s="168"/>
-      <c r="AH3" s="168"/>
-      <c r="AI3" s="201" t="s">
+      <c r="AF3" s="175"/>
+      <c r="AG3" s="175"/>
+      <c r="AH3" s="175"/>
+      <c r="AI3" s="232" t="s">
         <v>97</v>
       </c>
-      <c r="AJ3" s="201" t="s">
+      <c r="AJ3" s="232" t="s">
         <v>34</v>
       </c>
-      <c r="AK3" s="201" t="s">
+      <c r="AK3" s="232" t="s">
         <v>35</v>
       </c>
-      <c r="AL3" s="201" t="s">
+      <c r="AL3" s="232" t="s">
         <v>36</v>
       </c>
-      <c r="AM3" s="201" t="s">
+      <c r="AM3" s="232" t="s">
         <v>37</v>
       </c>
-      <c r="AN3" s="201" t="s">
+      <c r="AN3" s="232" t="s">
         <v>98</v>
       </c>
-      <c r="AO3" s="201" t="s">
+      <c r="AO3" s="232" t="s">
         <v>39</v>
       </c>
-      <c r="AP3" s="201" t="s">
+      <c r="AP3" s="232" t="s">
         <v>40</v>
       </c>
-      <c r="AQ3" s="168"/>
-      <c r="AR3" s="168"/>
-      <c r="AS3" s="168"/>
-      <c r="AT3" s="168"/>
-      <c r="AU3" s="168"/>
-      <c r="AV3" s="168"/>
-      <c r="AW3" s="168"/>
-      <c r="AX3" s="168"/>
-      <c r="AY3" s="168"/>
-      <c r="AZ3" s="168"/>
-      <c r="BA3" s="168"/>
-      <c r="BB3" s="203" t="s">
+      <c r="AQ3" s="175"/>
+      <c r="AR3" s="175"/>
+      <c r="AS3" s="175"/>
+      <c r="AT3" s="175"/>
+      <c r="AU3" s="175"/>
+      <c r="AV3" s="175"/>
+      <c r="AW3" s="175"/>
+      <c r="AX3" s="175"/>
+      <c r="AY3" s="175"/>
+      <c r="AZ3" s="175"/>
+      <c r="BA3" s="175"/>
+      <c r="BB3" s="237" t="s">
         <v>60</v>
       </c>
-      <c r="BC3" s="203" t="s">
+      <c r="BC3" s="237" t="s">
         <v>61</v>
       </c>
       <c r="BD3" s="31"/>
-      <c r="BE3" s="193" t="s">
+      <c r="BE3" s="167" t="s">
         <v>62</v>
       </c>
-      <c r="BF3" s="158"/>
-      <c r="BG3" s="158"/>
-      <c r="BH3" s="158"/>
-      <c r="BI3" s="158"/>
-      <c r="BJ3" s="158"/>
-      <c r="BK3" s="158"/>
-      <c r="BL3" s="158"/>
-      <c r="BM3" s="158"/>
-      <c r="BN3" s="158"/>
-      <c r="BO3" s="158"/>
-      <c r="BP3" s="158"/>
-      <c r="BQ3" s="158"/>
-      <c r="BR3" s="158"/>
-      <c r="BS3" s="158"/>
-      <c r="BT3" s="158"/>
-      <c r="BU3" s="158"/>
-      <c r="BV3" s="158"/>
-      <c r="BW3" s="158"/>
-      <c r="BX3" s="158"/>
-      <c r="BY3" s="158"/>
-      <c r="BZ3" s="158"/>
-      <c r="CA3" s="158"/>
-      <c r="CB3" s="158"/>
-      <c r="CC3" s="158"/>
-      <c r="CD3" s="158"/>
-      <c r="CE3" s="158"/>
-      <c r="CF3" s="158"/>
-      <c r="CG3" s="158"/>
-      <c r="CH3" s="158"/>
-      <c r="CI3" s="158"/>
-      <c r="CJ3" s="158"/>
-      <c r="CK3" s="168"/>
-      <c r="CL3" s="168"/>
-      <c r="CM3" s="168"/>
+      <c r="BF3" s="190"/>
+      <c r="BG3" s="190"/>
+      <c r="BH3" s="190"/>
+      <c r="BI3" s="190"/>
+      <c r="BJ3" s="190"/>
+      <c r="BK3" s="190"/>
+      <c r="BL3" s="190"/>
+      <c r="BM3" s="190"/>
+      <c r="BN3" s="190"/>
+      <c r="BO3" s="190"/>
+      <c r="BP3" s="190"/>
+      <c r="BQ3" s="190"/>
+      <c r="BR3" s="190"/>
+      <c r="BS3" s="190"/>
+      <c r="BT3" s="190"/>
+      <c r="BU3" s="190"/>
+      <c r="BV3" s="190"/>
+      <c r="BW3" s="190"/>
+      <c r="BX3" s="190"/>
+      <c r="BY3" s="190"/>
+      <c r="BZ3" s="190"/>
+      <c r="CA3" s="190"/>
+      <c r="CB3" s="190"/>
+      <c r="CC3" s="190"/>
+      <c r="CD3" s="190"/>
+      <c r="CE3" s="190"/>
+      <c r="CF3" s="190"/>
+      <c r="CG3" s="190"/>
+      <c r="CH3" s="190"/>
+      <c r="CI3" s="190"/>
+      <c r="CJ3" s="190"/>
+      <c r="CK3" s="175"/>
+      <c r="CL3" s="175"/>
+      <c r="CM3" s="175"/>
       <c r="CN3" s="18"/>
       <c r="CO3" s="18"/>
       <c r="CP3" s="18"/>
@@ -5099,176 +5111,176 @@
       <c r="FS3" s="18"/>
     </row>
     <row r="4" spans="1:175" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="168"/>
-      <c r="B4" s="168"/>
-      <c r="C4" s="168"/>
-      <c r="D4" s="168"/>
-      <c r="E4" s="168"/>
-      <c r="F4" s="168"/>
-      <c r="G4" s="168"/>
-      <c r="H4" s="168"/>
-      <c r="I4" s="168"/>
-      <c r="J4" s="168"/>
-      <c r="K4" s="168"/>
-      <c r="L4" s="168"/>
-      <c r="M4" s="168"/>
-      <c r="N4" s="168"/>
-      <c r="O4" s="168"/>
-      <c r="P4" s="168"/>
-      <c r="Q4" s="168"/>
-      <c r="R4" s="168"/>
-      <c r="S4" s="168"/>
-      <c r="T4" s="168"/>
-      <c r="U4" s="168"/>
-      <c r="V4" s="168"/>
-      <c r="W4" s="168"/>
-      <c r="X4" s="168"/>
-      <c r="Y4" s="168"/>
-      <c r="Z4" s="168"/>
-      <c r="AA4" s="168"/>
-      <c r="AB4" s="168"/>
-      <c r="AC4" s="168"/>
-      <c r="AD4" s="168"/>
-      <c r="AE4" s="168"/>
-      <c r="AF4" s="168"/>
-      <c r="AG4" s="168"/>
-      <c r="AH4" s="168"/>
-      <c r="AI4" s="168"/>
-      <c r="AJ4" s="168"/>
-      <c r="AK4" s="168"/>
-      <c r="AL4" s="168"/>
-      <c r="AM4" s="168"/>
-      <c r="AN4" s="168"/>
-      <c r="AO4" s="168"/>
-      <c r="AP4" s="168"/>
-      <c r="AQ4" s="168"/>
-      <c r="AR4" s="168"/>
-      <c r="AS4" s="168"/>
-      <c r="AT4" s="168"/>
-      <c r="AU4" s="168"/>
-      <c r="AV4" s="168"/>
-      <c r="AW4" s="168"/>
-      <c r="AX4" s="168"/>
-      <c r="AY4" s="168"/>
-      <c r="AZ4" s="168"/>
-      <c r="BA4" s="168"/>
-      <c r="BB4" s="168"/>
-      <c r="BC4" s="168"/>
-      <c r="BD4" s="200" t="s">
+      <c r="A4" s="175"/>
+      <c r="B4" s="175"/>
+      <c r="C4" s="175"/>
+      <c r="D4" s="175"/>
+      <c r="E4" s="175"/>
+      <c r="F4" s="175"/>
+      <c r="G4" s="175"/>
+      <c r="H4" s="175"/>
+      <c r="I4" s="175"/>
+      <c r="J4" s="175"/>
+      <c r="K4" s="175"/>
+      <c r="L4" s="175"/>
+      <c r="M4" s="175"/>
+      <c r="N4" s="175"/>
+      <c r="O4" s="175"/>
+      <c r="P4" s="175"/>
+      <c r="Q4" s="175"/>
+      <c r="R4" s="175"/>
+      <c r="S4" s="175"/>
+      <c r="T4" s="175"/>
+      <c r="U4" s="175"/>
+      <c r="V4" s="175"/>
+      <c r="W4" s="175"/>
+      <c r="X4" s="175"/>
+      <c r="Y4" s="175"/>
+      <c r="Z4" s="175"/>
+      <c r="AA4" s="175"/>
+      <c r="AB4" s="175"/>
+      <c r="AC4" s="175"/>
+      <c r="AD4" s="175"/>
+      <c r="AE4" s="175"/>
+      <c r="AF4" s="175"/>
+      <c r="AG4" s="175"/>
+      <c r="AH4" s="175"/>
+      <c r="AI4" s="175"/>
+      <c r="AJ4" s="175"/>
+      <c r="AK4" s="175"/>
+      <c r="AL4" s="175"/>
+      <c r="AM4" s="175"/>
+      <c r="AN4" s="175"/>
+      <c r="AO4" s="175"/>
+      <c r="AP4" s="175"/>
+      <c r="AQ4" s="175"/>
+      <c r="AR4" s="175"/>
+      <c r="AS4" s="175"/>
+      <c r="AT4" s="175"/>
+      <c r="AU4" s="175"/>
+      <c r="AV4" s="175"/>
+      <c r="AW4" s="175"/>
+      <c r="AX4" s="175"/>
+      <c r="AY4" s="175"/>
+      <c r="AZ4" s="175"/>
+      <c r="BA4" s="175"/>
+      <c r="BB4" s="175"/>
+      <c r="BC4" s="175"/>
+      <c r="BD4" s="234" t="s">
         <v>67</v>
       </c>
-      <c r="BE4" s="161"/>
-      <c r="BF4" s="162"/>
-      <c r="BG4" s="200" t="s">
+      <c r="BE4" s="157"/>
+      <c r="BF4" s="158"/>
+      <c r="BG4" s="234" t="s">
         <v>67</v>
       </c>
-      <c r="BH4" s="161"/>
-      <c r="BI4" s="162"/>
-      <c r="BJ4" s="200" t="s">
+      <c r="BH4" s="157"/>
+      <c r="BI4" s="158"/>
+      <c r="BJ4" s="234" t="s">
         <v>70</v>
       </c>
-      <c r="BK4" s="161"/>
-      <c r="BL4" s="162"/>
-      <c r="BM4" s="200" t="s">
+      <c r="BK4" s="157"/>
+      <c r="BL4" s="158"/>
+      <c r="BM4" s="234" t="s">
         <v>71</v>
       </c>
-      <c r="BN4" s="161"/>
-      <c r="BO4" s="162"/>
-      <c r="BP4" s="200" t="s">
+      <c r="BN4" s="157"/>
+      <c r="BO4" s="158"/>
+      <c r="BP4" s="234" t="s">
         <v>72</v>
       </c>
-      <c r="BQ4" s="161"/>
-      <c r="BR4" s="162"/>
-      <c r="BS4" s="200" t="s">
+      <c r="BQ4" s="157"/>
+      <c r="BR4" s="158"/>
+      <c r="BS4" s="234" t="s">
         <v>73</v>
       </c>
-      <c r="BT4" s="161"/>
-      <c r="BU4" s="162"/>
-      <c r="BV4" s="200" t="s">
+      <c r="BT4" s="157"/>
+      <c r="BU4" s="158"/>
+      <c r="BV4" s="234" t="s">
         <v>74</v>
       </c>
-      <c r="BW4" s="161"/>
-      <c r="BX4" s="162"/>
-      <c r="BY4" s="200" t="s">
+      <c r="BW4" s="157"/>
+      <c r="BX4" s="158"/>
+      <c r="BY4" s="234" t="s">
         <v>75</v>
       </c>
-      <c r="BZ4" s="161"/>
-      <c r="CA4" s="162"/>
-      <c r="CB4" s="200" t="s">
+      <c r="BZ4" s="157"/>
+      <c r="CA4" s="158"/>
+      <c r="CB4" s="234" t="s">
         <v>76</v>
       </c>
-      <c r="CC4" s="161"/>
-      <c r="CD4" s="162"/>
-      <c r="CE4" s="200" t="s">
+      <c r="CC4" s="157"/>
+      <c r="CD4" s="158"/>
+      <c r="CE4" s="234" t="s">
         <v>77</v>
       </c>
-      <c r="CF4" s="161"/>
-      <c r="CG4" s="162"/>
-      <c r="CH4" s="200" t="s">
+      <c r="CF4" s="157"/>
+      <c r="CG4" s="158"/>
+      <c r="CH4" s="234" t="s">
         <v>78</v>
       </c>
-      <c r="CI4" s="161"/>
-      <c r="CJ4" s="162"/>
-      <c r="CK4" s="168"/>
-      <c r="CL4" s="168"/>
-      <c r="CM4" s="168"/>
+      <c r="CI4" s="157"/>
+      <c r="CJ4" s="158"/>
+      <c r="CK4" s="175"/>
+      <c r="CL4" s="175"/>
+      <c r="CM4" s="175"/>
     </row>
     <row r="5" spans="1:175" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="202"/>
-      <c r="B5" s="202"/>
-      <c r="C5" s="202"/>
-      <c r="D5" s="202"/>
-      <c r="E5" s="202"/>
-      <c r="F5" s="202"/>
-      <c r="G5" s="202"/>
-      <c r="H5" s="202"/>
-      <c r="I5" s="202"/>
-      <c r="J5" s="202"/>
-      <c r="K5" s="202"/>
-      <c r="L5" s="202"/>
-      <c r="M5" s="202"/>
-      <c r="N5" s="202"/>
-      <c r="O5" s="202"/>
-      <c r="P5" s="202"/>
-      <c r="Q5" s="202"/>
-      <c r="R5" s="202"/>
-      <c r="S5" s="202"/>
-      <c r="T5" s="202"/>
-      <c r="U5" s="202"/>
-      <c r="V5" s="202"/>
-      <c r="W5" s="202"/>
-      <c r="X5" s="202"/>
-      <c r="Y5" s="202"/>
-      <c r="Z5" s="202"/>
-      <c r="AA5" s="202"/>
-      <c r="AB5" s="202"/>
-      <c r="AC5" s="202"/>
-      <c r="AD5" s="202"/>
-      <c r="AE5" s="202"/>
-      <c r="AF5" s="202"/>
-      <c r="AG5" s="202"/>
-      <c r="AH5" s="202"/>
-      <c r="AI5" s="202"/>
-      <c r="AJ5" s="202"/>
-      <c r="AK5" s="202"/>
-      <c r="AL5" s="202"/>
-      <c r="AM5" s="202"/>
-      <c r="AN5" s="202"/>
-      <c r="AO5" s="202"/>
-      <c r="AP5" s="202"/>
-      <c r="AQ5" s="202"/>
-      <c r="AR5" s="202"/>
-      <c r="AS5" s="202"/>
-      <c r="AT5" s="202"/>
-      <c r="AU5" s="202"/>
-      <c r="AV5" s="202"/>
-      <c r="AW5" s="202"/>
-      <c r="AX5" s="202"/>
-      <c r="AY5" s="202"/>
-      <c r="AZ5" s="202"/>
-      <c r="BA5" s="202"/>
-      <c r="BB5" s="202"/>
-      <c r="BC5" s="202"/>
+      <c r="A5" s="233"/>
+      <c r="B5" s="233"/>
+      <c r="C5" s="233"/>
+      <c r="D5" s="233"/>
+      <c r="E5" s="233"/>
+      <c r="F5" s="233"/>
+      <c r="G5" s="233"/>
+      <c r="H5" s="233"/>
+      <c r="I5" s="233"/>
+      <c r="J5" s="233"/>
+      <c r="K5" s="233"/>
+      <c r="L5" s="233"/>
+      <c r="M5" s="233"/>
+      <c r="N5" s="233"/>
+      <c r="O5" s="233"/>
+      <c r="P5" s="233"/>
+      <c r="Q5" s="233"/>
+      <c r="R5" s="233"/>
+      <c r="S5" s="233"/>
+      <c r="T5" s="233"/>
+      <c r="U5" s="233"/>
+      <c r="V5" s="233"/>
+      <c r="W5" s="233"/>
+      <c r="X5" s="233"/>
+      <c r="Y5" s="233"/>
+      <c r="Z5" s="233"/>
+      <c r="AA5" s="233"/>
+      <c r="AB5" s="233"/>
+      <c r="AC5" s="233"/>
+      <c r="AD5" s="233"/>
+      <c r="AE5" s="233"/>
+      <c r="AF5" s="233"/>
+      <c r="AG5" s="233"/>
+      <c r="AH5" s="233"/>
+      <c r="AI5" s="233"/>
+      <c r="AJ5" s="233"/>
+      <c r="AK5" s="233"/>
+      <c r="AL5" s="233"/>
+      <c r="AM5" s="233"/>
+      <c r="AN5" s="233"/>
+      <c r="AO5" s="233"/>
+      <c r="AP5" s="233"/>
+      <c r="AQ5" s="233"/>
+      <c r="AR5" s="233"/>
+      <c r="AS5" s="233"/>
+      <c r="AT5" s="233"/>
+      <c r="AU5" s="233"/>
+      <c r="AV5" s="233"/>
+      <c r="AW5" s="233"/>
+      <c r="AX5" s="233"/>
+      <c r="AY5" s="233"/>
+      <c r="AZ5" s="233"/>
+      <c r="BA5" s="233"/>
+      <c r="BB5" s="233"/>
+      <c r="BC5" s="233"/>
       <c r="BD5" s="32" t="s">
         <v>99</v>
       </c>
@@ -5368,9 +5380,9 @@
       <c r="CJ5" s="32" t="s">
         <v>65</v>
       </c>
-      <c r="CK5" s="202"/>
-      <c r="CL5" s="202"/>
-      <c r="CM5" s="202"/>
+      <c r="CK5" s="233"/>
+      <c r="CL5" s="233"/>
+      <c r="CM5" s="233"/>
     </row>
     <row r="6" spans="1:175" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="33"/>
@@ -5949,14 +5961,62 @@
     </row>
   </sheetData>
   <mergeCells count="80">
-    <mergeCell ref="X3:X5"/>
-    <mergeCell ref="Y3:Y5"/>
-    <mergeCell ref="AL3:AL5"/>
-    <mergeCell ref="Z3:Z5"/>
-    <mergeCell ref="AA3:AA5"/>
-    <mergeCell ref="AB3:AB5"/>
-    <mergeCell ref="AC3:AC5"/>
-    <mergeCell ref="AD3:AD5"/>
+    <mergeCell ref="BM4:BO4"/>
+    <mergeCell ref="AM3:AM5"/>
+    <mergeCell ref="AN3:AN5"/>
+    <mergeCell ref="AO3:AO5"/>
+    <mergeCell ref="AP3:AP5"/>
+    <mergeCell ref="AT2:AT5"/>
+    <mergeCell ref="AU2:AU5"/>
+    <mergeCell ref="AV2:AV5"/>
+    <mergeCell ref="AW2:AW5"/>
+    <mergeCell ref="CE4:CG4"/>
+    <mergeCell ref="CH4:CJ4"/>
+    <mergeCell ref="AX2:AX5"/>
+    <mergeCell ref="AY2:AY5"/>
+    <mergeCell ref="AZ2:AZ5"/>
+    <mergeCell ref="BB3:BB5"/>
+    <mergeCell ref="BC3:BC5"/>
+    <mergeCell ref="BP4:BR4"/>
+    <mergeCell ref="BS4:BU4"/>
+    <mergeCell ref="BV4:BX4"/>
+    <mergeCell ref="BY4:CA4"/>
+    <mergeCell ref="CB4:CD4"/>
+    <mergeCell ref="BA2:BA5"/>
+    <mergeCell ref="BD4:BF4"/>
+    <mergeCell ref="BG4:BI4"/>
+    <mergeCell ref="BJ4:BL4"/>
+    <mergeCell ref="CK2:CK5"/>
+    <mergeCell ref="CL2:CL5"/>
+    <mergeCell ref="CM2:CM5"/>
+    <mergeCell ref="BE3:CJ3"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D1:O1"/>
+    <mergeCell ref="P1:S1"/>
+    <mergeCell ref="T1:AF1"/>
+    <mergeCell ref="AG1:AS1"/>
+    <mergeCell ref="AT1:AZ1"/>
+    <mergeCell ref="BA1:CM1"/>
+    <mergeCell ref="BB2:CJ2"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="C2:C5"/>
+    <mergeCell ref="D2:D5"/>
+    <mergeCell ref="E2:E5"/>
+    <mergeCell ref="F2:F5"/>
+    <mergeCell ref="G2:G5"/>
+    <mergeCell ref="H2:H5"/>
+    <mergeCell ref="I2:I5"/>
+    <mergeCell ref="J2:J5"/>
+    <mergeCell ref="K2:K5"/>
+    <mergeCell ref="L2:L5"/>
+    <mergeCell ref="M2:M5"/>
+    <mergeCell ref="N2:N5"/>
+    <mergeCell ref="O2:O5"/>
+    <mergeCell ref="P2:P5"/>
+    <mergeCell ref="Q2:Q5"/>
+    <mergeCell ref="R2:R5"/>
+    <mergeCell ref="S2:S5"/>
     <mergeCell ref="T2:T5"/>
     <mergeCell ref="U2:U5"/>
     <mergeCell ref="AQ2:AQ5"/>
@@ -5973,62 +6033,14 @@
     <mergeCell ref="AI3:AI5"/>
     <mergeCell ref="AJ3:AJ5"/>
     <mergeCell ref="AK3:AK5"/>
-    <mergeCell ref="O2:O5"/>
-    <mergeCell ref="P2:P5"/>
-    <mergeCell ref="Q2:Q5"/>
-    <mergeCell ref="R2:R5"/>
-    <mergeCell ref="S2:S5"/>
-    <mergeCell ref="J2:J5"/>
-    <mergeCell ref="K2:K5"/>
-    <mergeCell ref="L2:L5"/>
-    <mergeCell ref="M2:M5"/>
-    <mergeCell ref="N2:N5"/>
-    <mergeCell ref="E2:E5"/>
-    <mergeCell ref="F2:F5"/>
-    <mergeCell ref="G2:G5"/>
-    <mergeCell ref="H2:H5"/>
-    <mergeCell ref="I2:I5"/>
-    <mergeCell ref="CK2:CK5"/>
-    <mergeCell ref="CL2:CL5"/>
-    <mergeCell ref="CM2:CM5"/>
-    <mergeCell ref="BE3:CJ3"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="D1:O1"/>
-    <mergeCell ref="P1:S1"/>
-    <mergeCell ref="T1:AF1"/>
-    <mergeCell ref="AG1:AS1"/>
-    <mergeCell ref="AT1:AZ1"/>
-    <mergeCell ref="BA1:CM1"/>
-    <mergeCell ref="BB2:CJ2"/>
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="B2:B5"/>
-    <mergeCell ref="C2:C5"/>
-    <mergeCell ref="D2:D5"/>
-    <mergeCell ref="CE4:CG4"/>
-    <mergeCell ref="CH4:CJ4"/>
-    <mergeCell ref="AX2:AX5"/>
-    <mergeCell ref="AY2:AY5"/>
-    <mergeCell ref="AZ2:AZ5"/>
-    <mergeCell ref="BB3:BB5"/>
-    <mergeCell ref="BC3:BC5"/>
-    <mergeCell ref="BP4:BR4"/>
-    <mergeCell ref="BS4:BU4"/>
-    <mergeCell ref="BV4:BX4"/>
-    <mergeCell ref="BY4:CA4"/>
-    <mergeCell ref="CB4:CD4"/>
-    <mergeCell ref="BA2:BA5"/>
-    <mergeCell ref="BD4:BF4"/>
-    <mergeCell ref="BG4:BI4"/>
-    <mergeCell ref="BJ4:BL4"/>
-    <mergeCell ref="BM4:BO4"/>
-    <mergeCell ref="AM3:AM5"/>
-    <mergeCell ref="AN3:AN5"/>
-    <mergeCell ref="AO3:AO5"/>
-    <mergeCell ref="AP3:AP5"/>
-    <mergeCell ref="AT2:AT5"/>
-    <mergeCell ref="AU2:AU5"/>
-    <mergeCell ref="AV2:AV5"/>
-    <mergeCell ref="AW2:AW5"/>
+    <mergeCell ref="X3:X5"/>
+    <mergeCell ref="Y3:Y5"/>
+    <mergeCell ref="AL3:AL5"/>
+    <mergeCell ref="Z3:Z5"/>
+    <mergeCell ref="AA3:AA5"/>
+    <mergeCell ref="AB3:AB5"/>
+    <mergeCell ref="AC3:AC5"/>
+    <mergeCell ref="AD3:AD5"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="BB6:BB10" xr:uid="{00000000-0002-0000-0100-000000000000}">
@@ -6062,36 +6074,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="206" t="s">
+      <c r="A1" s="242" t="s">
         <v>100</v>
       </c>
-      <c r="B1" s="158"/>
-      <c r="C1" s="158"/>
-      <c r="D1" s="158"/>
-      <c r="E1" s="158"/>
-      <c r="F1" s="158"/>
-      <c r="G1" s="158"/>
-      <c r="H1" s="158"/>
-      <c r="I1" s="158"/>
-      <c r="J1" s="158"/>
-      <c r="K1" s="158"/>
-      <c r="L1" s="158"/>
+      <c r="B1" s="190"/>
+      <c r="C1" s="190"/>
+      <c r="D1" s="190"/>
+      <c r="E1" s="190"/>
+      <c r="F1" s="190"/>
+      <c r="G1" s="190"/>
+      <c r="H1" s="190"/>
+      <c r="I1" s="190"/>
+      <c r="J1" s="190"/>
+      <c r="K1" s="190"/>
+      <c r="L1" s="190"/>
     </row>
     <row r="3" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A3" s="207" t="s">
+      <c r="A3" s="239" t="s">
         <v>101</v>
       </c>
-      <c r="B3" s="158"/>
-      <c r="C3" s="158"/>
-      <c r="D3" s="158"/>
-      <c r="E3" s="158"/>
-      <c r="F3" s="158"/>
-      <c r="G3" s="158"/>
-      <c r="H3" s="158"/>
-      <c r="I3" s="158"/>
-      <c r="J3" s="158"/>
-      <c r="K3" s="158"/>
-      <c r="L3" s="158"/>
+      <c r="B3" s="190"/>
+      <c r="C3" s="190"/>
+      <c r="D3" s="190"/>
+      <c r="E3" s="190"/>
+      <c r="F3" s="190"/>
+      <c r="G3" s="190"/>
+      <c r="H3" s="190"/>
+      <c r="I3" s="190"/>
+      <c r="J3" s="190"/>
+      <c r="K3" s="190"/>
+      <c r="L3" s="190"/>
     </row>
     <row r="4" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A4" s="35" t="s">
@@ -6128,24 +6140,24 @@
       <c r="L5" s="29"/>
     </row>
     <row r="6" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A6" s="208" t="s">
+      <c r="A6" s="243" t="s">
         <v>105</v>
       </c>
-      <c r="B6" s="155"/>
-      <c r="C6" s="155"/>
-      <c r="D6" s="166"/>
-      <c r="E6" s="208" t="s">
+      <c r="B6" s="152"/>
+      <c r="C6" s="152"/>
+      <c r="D6" s="153"/>
+      <c r="E6" s="243" t="s">
         <v>106</v>
       </c>
-      <c r="F6" s="155"/>
-      <c r="G6" s="155"/>
-      <c r="H6" s="166"/>
-      <c r="I6" s="208" t="s">
+      <c r="F6" s="152"/>
+      <c r="G6" s="152"/>
+      <c r="H6" s="153"/>
+      <c r="I6" s="243" t="s">
         <v>107</v>
       </c>
-      <c r="J6" s="155"/>
-      <c r="K6" s="155"/>
-      <c r="L6" s="166"/>
+      <c r="J6" s="152"/>
+      <c r="K6" s="152"/>
+      <c r="L6" s="153"/>
     </row>
     <row r="7" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A7" s="35" t="s">
@@ -6340,19 +6352,19 @@
       <c r="D16" s="31"/>
     </row>
     <row r="17" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A17" s="207" t="s">
+      <c r="A17" s="239" t="s">
         <v>125</v>
       </c>
-      <c r="B17" s="158"/>
-      <c r="C17" s="158"/>
-      <c r="D17" s="158"/>
+      <c r="B17" s="190"/>
+      <c r="C17" s="190"/>
+      <c r="D17" s="190"/>
       <c r="E17" s="43"/>
-      <c r="F17" s="209" t="s">
+      <c r="F17" s="240" t="s">
         <v>126</v>
       </c>
-      <c r="G17" s="210"/>
-      <c r="H17" s="210"/>
-      <c r="I17" s="210"/>
+      <c r="G17" s="241"/>
+      <c r="H17" s="241"/>
+      <c r="I17" s="241"/>
     </row>
     <row r="18" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A18" s="44" t="s">
@@ -6437,19 +6449,19 @@
       <c r="D24" s="62"/>
     </row>
     <row r="25" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A25" s="207" t="s">
+      <c r="A25" s="239" t="s">
         <v>135</v>
       </c>
-      <c r="B25" s="158"/>
-      <c r="C25" s="158"/>
-      <c r="D25" s="158"/>
+      <c r="B25" s="190"/>
+      <c r="C25" s="190"/>
+      <c r="D25" s="190"/>
       <c r="E25" s="63"/>
-      <c r="F25" s="207" t="s">
+      <c r="F25" s="239" t="s">
         <v>136</v>
       </c>
-      <c r="G25" s="158"/>
-      <c r="H25" s="158"/>
-      <c r="I25" s="158"/>
+      <c r="G25" s="190"/>
+      <c r="H25" s="190"/>
+      <c r="I25" s="190"/>
     </row>
     <row r="26" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A26" s="35" t="s">
@@ -6782,16 +6794,16 @@
       <c r="D53" s="29"/>
     </row>
     <row r="55" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A55" s="207" t="s">
+      <c r="A55" s="239" t="s">
         <v>172</v>
       </c>
-      <c r="B55" s="158"/>
-      <c r="C55" s="158"/>
-      <c r="D55" s="158"/>
-      <c r="E55" s="158"/>
-      <c r="F55" s="158"/>
-      <c r="G55" s="158"/>
-      <c r="H55" s="158"/>
+      <c r="B55" s="190"/>
+      <c r="C55" s="190"/>
+      <c r="D55" s="190"/>
+      <c r="E55" s="190"/>
+      <c r="F55" s="190"/>
+      <c r="G55" s="190"/>
+      <c r="H55" s="190"/>
     </row>
     <row r="56" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A56" s="35" t="s">
@@ -6830,18 +6842,18 @@
       <c r="H59" s="29"/>
     </row>
     <row r="60" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A60" s="211" t="s">
+      <c r="A60" s="238" t="s">
         <v>174</v>
       </c>
-      <c r="B60" s="161"/>
-      <c r="C60" s="161"/>
-      <c r="D60" s="162"/>
-      <c r="E60" s="211" t="s">
+      <c r="B60" s="157"/>
+      <c r="C60" s="157"/>
+      <c r="D60" s="158"/>
+      <c r="E60" s="238" t="s">
         <v>175</v>
       </c>
-      <c r="F60" s="161"/>
-      <c r="G60" s="161"/>
-      <c r="H60" s="162"/>
+      <c r="F60" s="157"/>
+      <c r="G60" s="157"/>
+      <c r="H60" s="158"/>
     </row>
     <row r="61" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A61" s="41" t="s">
@@ -6887,16 +6899,16 @@
       <c r="H62" s="29"/>
     </row>
     <row r="63" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A63" s="211" t="s">
+      <c r="A63" s="238" t="s">
         <v>186</v>
       </c>
-      <c r="B63" s="161"/>
-      <c r="C63" s="161"/>
-      <c r="D63" s="161"/>
-      <c r="E63" s="161"/>
-      <c r="F63" s="161"/>
-      <c r="G63" s="161"/>
-      <c r="H63" s="162"/>
+      <c r="B63" s="157"/>
+      <c r="C63" s="157"/>
+      <c r="D63" s="157"/>
+      <c r="E63" s="157"/>
+      <c r="F63" s="157"/>
+      <c r="G63" s="157"/>
+      <c r="H63" s="158"/>
     </row>
     <row r="64" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A64" s="35" t="s">
@@ -6959,18 +6971,18 @@
       <c r="H67" s="6"/>
     </row>
     <row r="68" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A68" s="211" t="s">
+      <c r="A68" s="238" t="s">
         <v>197</v>
       </c>
-      <c r="B68" s="161"/>
-      <c r="C68" s="161"/>
-      <c r="D68" s="162"/>
-      <c r="E68" s="211" t="s">
+      <c r="B68" s="157"/>
+      <c r="C68" s="157"/>
+      <c r="D68" s="158"/>
+      <c r="E68" s="238" t="s">
         <v>198</v>
       </c>
-      <c r="F68" s="161"/>
-      <c r="G68" s="161"/>
-      <c r="H68" s="162"/>
+      <c r="F68" s="157"/>
+      <c r="G68" s="157"/>
+      <c r="H68" s="158"/>
     </row>
     <row r="69" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A69" s="44" t="s">
@@ -7063,18 +7075,18 @@
       <c r="H74" s="29"/>
     </row>
     <row r="75" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A75" s="211" t="s">
+      <c r="A75" s="238" t="s">
         <v>202</v>
       </c>
-      <c r="B75" s="161"/>
-      <c r="C75" s="161"/>
-      <c r="D75" s="162"/>
-      <c r="E75" s="211" t="s">
+      <c r="B75" s="157"/>
+      <c r="C75" s="157"/>
+      <c r="D75" s="158"/>
+      <c r="E75" s="238" t="s">
         <v>203</v>
       </c>
-      <c r="F75" s="161"/>
-      <c r="G75" s="161"/>
-      <c r="H75" s="162"/>
+      <c r="F75" s="157"/>
+      <c r="G75" s="157"/>
+      <c r="H75" s="158"/>
     </row>
     <row r="76" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A76" s="44" t="s">
@@ -7167,18 +7179,18 @@
       <c r="H81" s="29"/>
     </row>
     <row r="82" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A82" s="211" t="s">
+      <c r="A82" s="238" t="s">
         <v>204</v>
       </c>
-      <c r="B82" s="161"/>
-      <c r="C82" s="161"/>
-      <c r="D82" s="162"/>
-      <c r="E82" s="211" t="s">
+      <c r="B82" s="157"/>
+      <c r="C82" s="157"/>
+      <c r="D82" s="158"/>
+      <c r="E82" s="238" t="s">
         <v>205</v>
       </c>
-      <c r="F82" s="161"/>
-      <c r="G82" s="161"/>
-      <c r="H82" s="162"/>
+      <c r="F82" s="157"/>
+      <c r="G82" s="157"/>
+      <c r="H82" s="158"/>
     </row>
     <row r="83" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A83" s="44" t="s">
@@ -7356,6 +7368,16 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A3:L3"/>
+    <mergeCell ref="A6:D6"/>
+    <mergeCell ref="E6:H6"/>
+    <mergeCell ref="I6:L6"/>
+    <mergeCell ref="A17:D17"/>
+    <mergeCell ref="F17:I17"/>
+    <mergeCell ref="A68:D68"/>
+    <mergeCell ref="A75:D75"/>
+    <mergeCell ref="E75:H75"/>
     <mergeCell ref="A82:D82"/>
     <mergeCell ref="E82:H82"/>
     <mergeCell ref="A25:D25"/>
@@ -7365,16 +7387,6 @@
     <mergeCell ref="E60:H60"/>
     <mergeCell ref="A63:H63"/>
     <mergeCell ref="E68:H68"/>
-    <mergeCell ref="A17:D17"/>
-    <mergeCell ref="F17:I17"/>
-    <mergeCell ref="A68:D68"/>
-    <mergeCell ref="A75:D75"/>
-    <mergeCell ref="E75:H75"/>
-    <mergeCell ref="A1:L1"/>
-    <mergeCell ref="A3:L3"/>
-    <mergeCell ref="A6:D6"/>
-    <mergeCell ref="E6:H6"/>
-    <mergeCell ref="I6:L6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>